<commit_message>
re arranged the scheduler a bit
</commit_message>
<xml_diff>
--- a/Documentation/Obtayn-gantt-chart.xlsx
+++ b/Documentation/Obtayn-gantt-chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study Material\BLUEpineapple\Final project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study Material\BLUEpineapple\Final project\obtayn\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B08A591-E5F2-4E3E-BF16-A4B591324055}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA44F3F2-DBFE-4453-8A46-48F543683FBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="171">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -778,7 +778,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -879,6 +879,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2DCDB"/>
+        <bgColor rgb="FFDEE6EF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FFE6E0EC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1020,7 +1032,7 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1310,16 +1322,22 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="164" fontId="23" fillId="18" borderId="1" xfId="3" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="23" fillId="19" borderId="1" xfId="3" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Date" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1437,6 +1455,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFEBF1DE"/>
+      <color rgb="FFF2DCDB"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1801,8 +1823,8 @@
   <dimension ref="A1:BL146"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
+      <pane ySplit="6" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E83" sqref="E83:F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1849,118 +1871,118 @@
       <c r="B3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="101"/>
-      <c r="E3" s="102">
+      <c r="D3" s="103"/>
+      <c r="E3" s="104">
         <f>DATE(2021,3,31)</f>
         <v>44286</v>
       </c>
-      <c r="F3" s="102"/>
+      <c r="F3" s="104"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="101"/>
+      <c r="D4" s="103"/>
       <c r="E4" s="13">
         <v>1</v>
       </c>
-      <c r="I4" s="103">
+      <c r="I4" s="101">
         <f>I5</f>
         <v>44284</v>
       </c>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="103"/>
-      <c r="O4" s="103"/>
-      <c r="P4" s="103">
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="101"/>
+      <c r="O4" s="101"/>
+      <c r="P4" s="101">
         <f>P5</f>
         <v>44291</v>
       </c>
-      <c r="Q4" s="103"/>
-      <c r="R4" s="103"/>
-      <c r="S4" s="103"/>
-      <c r="T4" s="103"/>
-      <c r="U4" s="103"/>
-      <c r="V4" s="103"/>
-      <c r="W4" s="103">
+      <c r="Q4" s="101"/>
+      <c r="R4" s="101"/>
+      <c r="S4" s="101"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="101"/>
+      <c r="V4" s="101"/>
+      <c r="W4" s="101">
         <f>W5</f>
         <v>44298</v>
       </c>
-      <c r="X4" s="103"/>
-      <c r="Y4" s="103"/>
-      <c r="Z4" s="103"/>
-      <c r="AA4" s="103"/>
-      <c r="AB4" s="103"/>
-      <c r="AC4" s="103"/>
-      <c r="AD4" s="103">
+      <c r="X4" s="101"/>
+      <c r="Y4" s="101"/>
+      <c r="Z4" s="101"/>
+      <c r="AA4" s="101"/>
+      <c r="AB4" s="101"/>
+      <c r="AC4" s="101"/>
+      <c r="AD4" s="101">
         <f>AD5</f>
         <v>44305</v>
       </c>
-      <c r="AE4" s="103"/>
-      <c r="AF4" s="103"/>
-      <c r="AG4" s="103"/>
-      <c r="AH4" s="103"/>
-      <c r="AI4" s="103"/>
-      <c r="AJ4" s="103"/>
-      <c r="AK4" s="103">
+      <c r="AE4" s="101"/>
+      <c r="AF4" s="101"/>
+      <c r="AG4" s="101"/>
+      <c r="AH4" s="101"/>
+      <c r="AI4" s="101"/>
+      <c r="AJ4" s="101"/>
+      <c r="AK4" s="101">
         <f>AK5</f>
         <v>44312</v>
       </c>
-      <c r="AL4" s="103"/>
-      <c r="AM4" s="103"/>
-      <c r="AN4" s="103"/>
-      <c r="AO4" s="103"/>
-      <c r="AP4" s="103"/>
-      <c r="AQ4" s="103"/>
-      <c r="AR4" s="103">
+      <c r="AL4" s="101"/>
+      <c r="AM4" s="101"/>
+      <c r="AN4" s="101"/>
+      <c r="AO4" s="101"/>
+      <c r="AP4" s="101"/>
+      <c r="AQ4" s="101"/>
+      <c r="AR4" s="101">
         <f>AR5</f>
         <v>44319</v>
       </c>
-      <c r="AS4" s="103"/>
-      <c r="AT4" s="103"/>
-      <c r="AU4" s="103"/>
-      <c r="AV4" s="103"/>
-      <c r="AW4" s="103"/>
-      <c r="AX4" s="103"/>
-      <c r="AY4" s="103">
+      <c r="AS4" s="101"/>
+      <c r="AT4" s="101"/>
+      <c r="AU4" s="101"/>
+      <c r="AV4" s="101"/>
+      <c r="AW4" s="101"/>
+      <c r="AX4" s="101"/>
+      <c r="AY4" s="101">
         <f>AY5</f>
         <v>44326</v>
       </c>
-      <c r="AZ4" s="103"/>
-      <c r="BA4" s="103"/>
-      <c r="BB4" s="103"/>
-      <c r="BC4" s="103"/>
-      <c r="BD4" s="103"/>
-      <c r="BE4" s="103"/>
-      <c r="BF4" s="103">
+      <c r="AZ4" s="101"/>
+      <c r="BA4" s="101"/>
+      <c r="BB4" s="101"/>
+      <c r="BC4" s="101"/>
+      <c r="BD4" s="101"/>
+      <c r="BE4" s="101"/>
+      <c r="BF4" s="101">
         <f>BF5</f>
         <v>44333</v>
       </c>
-      <c r="BG4" s="103"/>
-      <c r="BH4" s="103"/>
-      <c r="BI4" s="103"/>
-      <c r="BJ4" s="103"/>
-      <c r="BK4" s="103"/>
-      <c r="BL4" s="103"/>
+      <c r="BG4" s="101"/>
+      <c r="BH4" s="101"/>
+      <c r="BI4" s="101"/>
+      <c r="BJ4" s="101"/>
+      <c r="BK4" s="101"/>
+      <c r="BL4" s="101"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="104"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
       <c r="I5" s="14">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44284</v>
@@ -4059,7 +4081,9 @@
         <v>44</v>
       </c>
       <c r="C28" s="90"/>
-      <c r="D28" s="92"/>
+      <c r="D28" s="92">
+        <v>1</v>
+      </c>
       <c r="E28" s="93">
         <f>DATE(2021,4,7)</f>
         <v>44293</v>
@@ -4671,12 +4695,12 @@
       <c r="C36" s="61"/>
       <c r="D36" s="62"/>
       <c r="E36" s="63">
-        <f>DATE(2021,4,6)</f>
-        <v>44292</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="F36" s="63">
-        <f>DATE(2021,4,6)</f>
-        <v>44292</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
@@ -4743,7 +4767,9 @@
         <v>53</v>
       </c>
       <c r="C37" s="61"/>
-      <c r="D37" s="62"/>
+      <c r="D37" s="62">
+        <v>1</v>
+      </c>
       <c r="E37" s="63">
         <f>DATE(2021,4,5)</f>
         <v>44291</v>
@@ -4817,7 +4843,9 @@
         <v>54</v>
       </c>
       <c r="C38" s="61"/>
-      <c r="D38" s="62"/>
+      <c r="D38" s="62">
+        <v>1</v>
+      </c>
       <c r="E38" s="63">
         <f>DATE(2021,4,5)</f>
         <v>44291</v>
@@ -5641,7 +5669,9 @@
         <v>66</v>
       </c>
       <c r="C49" s="43"/>
-      <c r="D49" s="44"/>
+      <c r="D49" s="44">
+        <v>1</v>
+      </c>
       <c r="E49" s="45">
         <f t="shared" si="9"/>
         <v>44294</v>
@@ -5715,7 +5745,9 @@
         <v>67</v>
       </c>
       <c r="C50" s="43"/>
-      <c r="D50" s="44"/>
+      <c r="D50" s="44">
+        <v>0.5</v>
+      </c>
       <c r="E50" s="45">
         <f>DATE(2021,4,7)</f>
         <v>44293</v>
@@ -5860,7 +5892,7 @@
       </c>
       <c r="C52" s="90"/>
       <c r="D52" s="92">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E52" s="89">
         <f>DATE(2021,4,8)</f>
@@ -6159,12 +6191,12 @@
       <c r="C56" s="61"/>
       <c r="D56" s="62"/>
       <c r="E56" s="63">
-        <f t="shared" si="10"/>
-        <v>44295</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="F56" s="63">
-        <f t="shared" si="10"/>
-        <v>44295</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="G56" s="27"/>
       <c r="H56" s="27"/>
@@ -6307,7 +6339,9 @@
         <v>75</v>
       </c>
       <c r="C58" s="61"/>
-      <c r="D58" s="62"/>
+      <c r="D58" s="62">
+        <v>1</v>
+      </c>
       <c r="E58" s="63">
         <f t="shared" ref="E58:F64" si="11">DATE(2021,4,12)</f>
         <v>44298</v>
@@ -6381,7 +6415,9 @@
         <v>76</v>
       </c>
       <c r="C59" s="61"/>
-      <c r="D59" s="62"/>
+      <c r="D59" s="62">
+        <v>1</v>
+      </c>
       <c r="E59" s="63">
         <f t="shared" si="11"/>
         <v>44298</v>
@@ -6455,7 +6491,9 @@
         <v>77</v>
       </c>
       <c r="C60" s="61"/>
-      <c r="D60" s="62"/>
+      <c r="D60" s="62">
+        <v>1</v>
+      </c>
       <c r="E60" s="63">
         <f t="shared" si="11"/>
         <v>44298</v>
@@ -6603,7 +6641,9 @@
         <v>79</v>
       </c>
       <c r="C62" s="61"/>
-      <c r="D62" s="62"/>
+      <c r="D62" s="62">
+        <v>0.5</v>
+      </c>
       <c r="E62" s="63">
         <f t="shared" si="11"/>
         <v>44298</v>
@@ -6751,7 +6791,9 @@
         <v>81</v>
       </c>
       <c r="C64" s="61"/>
-      <c r="D64" s="62"/>
+      <c r="D64" s="62">
+        <v>0.8</v>
+      </c>
       <c r="E64" s="63">
         <f t="shared" si="11"/>
         <v>44298</v>
@@ -7201,12 +7243,12 @@
       <c r="C70" s="30"/>
       <c r="D70" s="31"/>
       <c r="E70" s="32">
-        <f t="shared" si="12"/>
-        <v>44293</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="F70" s="32">
-        <f t="shared" si="12"/>
-        <v>44293</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="G70" s="27"/>
       <c r="H70" s="27"/>
@@ -7273,7 +7315,9 @@
         <v>88</v>
       </c>
       <c r="C71" s="30"/>
-      <c r="D71" s="31"/>
+      <c r="D71" s="31">
+        <v>1</v>
+      </c>
       <c r="E71" s="32">
         <f t="shared" si="12"/>
         <v>44293</v>
@@ -7347,7 +7391,9 @@
         <v>89</v>
       </c>
       <c r="C72" s="30"/>
-      <c r="D72" s="31"/>
+      <c r="D72" s="31">
+        <v>0.6</v>
+      </c>
       <c r="E72" s="32">
         <f>DATE(2021,4,8)</f>
         <v>44294</v>
@@ -7495,7 +7541,9 @@
         <v>90</v>
       </c>
       <c r="C74" s="30"/>
-      <c r="D74" s="31"/>
+      <c r="D74" s="31">
+        <v>1</v>
+      </c>
       <c r="E74" s="32">
         <f>DATE(2021,4,7)</f>
         <v>44293</v>
@@ -7641,12 +7689,12 @@
       <c r="C76" s="43"/>
       <c r="D76" s="44"/>
       <c r="E76" s="45">
-        <f>DATE(2021,4,8)</f>
-        <v>44294</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="F76" s="45">
-        <f>DATE(2021,4,8)</f>
-        <v>44294</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="G76" s="27"/>
       <c r="H76" s="27"/>
@@ -7715,12 +7763,12 @@
       <c r="C77" s="43"/>
       <c r="D77" s="44"/>
       <c r="E77" s="45">
-        <f>DATE(2021,4,9)</f>
-        <v>44295</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="F77" s="45">
-        <f>DATE(2021,4,9)</f>
-        <v>44295</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="G77" s="27"/>
       <c r="H77" s="27"/>
@@ -7789,12 +7837,12 @@
       <c r="C78" s="43"/>
       <c r="D78" s="44"/>
       <c r="E78" s="45">
-        <f t="shared" ref="E78:F80" si="13">DATE(2021,4,8)</f>
-        <v>44294</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="F78" s="45">
-        <f t="shared" si="13"/>
-        <v>44294</v>
+        <f>DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="G78" s="27"/>
       <c r="H78" s="27"/>
@@ -7863,12 +7911,12 @@
       <c r="C79" s="43"/>
       <c r="D79" s="44"/>
       <c r="E79" s="45">
-        <f t="shared" si="13"/>
-        <v>44294</v>
+        <f>DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="F79" s="45">
-        <f t="shared" si="13"/>
-        <v>44294</v>
+        <f>DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="G79" s="27"/>
       <c r="H79" s="27"/>
@@ -7937,12 +7985,12 @@
       <c r="C80" s="43"/>
       <c r="D80" s="44"/>
       <c r="E80" s="45">
-        <f t="shared" si="13"/>
-        <v>44294</v>
+        <f>DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="F80" s="45">
-        <f t="shared" si="13"/>
-        <v>44294</v>
+        <f>DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="G80" s="27"/>
       <c r="H80" s="27"/>
@@ -8011,12 +8059,12 @@
       <c r="C81" s="43"/>
       <c r="D81" s="44"/>
       <c r="E81" s="45">
-        <f>DATE(2021,4,9)</f>
-        <v>44295</v>
+        <f>DATE(2021,4,16)</f>
+        <v>44302</v>
       </c>
       <c r="F81" s="45">
-        <f>DATE(2021,4,9)</f>
-        <v>44295</v>
+        <f>DATE(2021,4,19)</f>
+        <v>44305</v>
       </c>
       <c r="G81" s="27"/>
       <c r="H81" s="27"/>
@@ -8154,13 +8202,13 @@
       </c>
       <c r="C83" s="52"/>
       <c r="D83" s="53"/>
-      <c r="E83" s="54">
-        <f>DATE(2021,4,9)</f>
-        <v>44295</v>
-      </c>
-      <c r="F83" s="54">
-        <f t="shared" ref="F83:F89" si="14">DATE(2021,4,9)</f>
-        <v>44295</v>
+      <c r="E83" s="106">
+        <f>DATE(2021,4,15)</f>
+        <v>44301</v>
+      </c>
+      <c r="F83" s="106">
+        <f>DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="G83" s="27"/>
       <c r="H83" s="27"/>
@@ -8228,13 +8276,13 @@
       </c>
       <c r="C84" s="52"/>
       <c r="D84" s="53"/>
-      <c r="E84" s="54">
-        <f t="shared" ref="E84:E89" si="15">DATE(2021,4,9)</f>
-        <v>44295</v>
-      </c>
-      <c r="F84" s="54">
-        <f t="shared" si="14"/>
-        <v>44295</v>
+      <c r="E84" s="106">
+        <f>DATE(2021,4,15)</f>
+        <v>44301</v>
+      </c>
+      <c r="F84" s="106">
+        <f>DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="G84" s="27"/>
       <c r="H84" s="27"/>
@@ -8303,12 +8351,12 @@
       <c r="C85" s="52"/>
       <c r="D85" s="53"/>
       <c r="E85" s="54">
-        <f t="shared" si="15"/>
-        <v>44295</v>
+        <f>DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F85" s="54">
-        <f t="shared" si="14"/>
-        <v>44295</v>
+        <f>DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="G85" s="27"/>
       <c r="H85" s="27"/>
@@ -8377,12 +8425,12 @@
       <c r="C86" s="52"/>
       <c r="D86" s="53"/>
       <c r="E86" s="54">
-        <f t="shared" si="15"/>
-        <v>44295</v>
+        <f t="shared" ref="E86:F89" si="13">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F86" s="54">
-        <f t="shared" si="14"/>
-        <v>44295</v>
+        <f t="shared" si="13"/>
+        <v>44307</v>
       </c>
       <c r="G86" s="27"/>
       <c r="H86" s="27"/>
@@ -8451,12 +8499,12 @@
       <c r="C87" s="52"/>
       <c r="D87" s="53"/>
       <c r="E87" s="54">
-        <f t="shared" si="15"/>
-        <v>44295</v>
+        <f t="shared" si="13"/>
+        <v>44307</v>
       </c>
       <c r="F87" s="54">
-        <f t="shared" si="14"/>
-        <v>44295</v>
+        <f t="shared" si="13"/>
+        <v>44307</v>
       </c>
       <c r="G87" s="27"/>
       <c r="H87" s="27"/>
@@ -8525,12 +8573,12 @@
       <c r="C88" s="52"/>
       <c r="D88" s="53"/>
       <c r="E88" s="54">
-        <f t="shared" si="15"/>
-        <v>44295</v>
+        <f t="shared" si="13"/>
+        <v>44307</v>
       </c>
       <c r="F88" s="54">
-        <f t="shared" si="14"/>
-        <v>44295</v>
+        <f t="shared" si="13"/>
+        <v>44307</v>
       </c>
       <c r="G88" s="27"/>
       <c r="H88" s="27"/>
@@ -8599,12 +8647,12 @@
       <c r="C89" s="52"/>
       <c r="D89" s="53"/>
       <c r="E89" s="54">
-        <f t="shared" si="15"/>
-        <v>44295</v>
+        <f t="shared" si="13"/>
+        <v>44307</v>
       </c>
       <c r="F89" s="54">
-        <f t="shared" si="14"/>
-        <v>44295</v>
+        <f t="shared" si="13"/>
+        <v>44307</v>
       </c>
       <c r="G89" s="27"/>
       <c r="H89" s="27"/>
@@ -8741,13 +8789,15 @@
         <v>107</v>
       </c>
       <c r="C91" s="61"/>
-      <c r="D91" s="62"/>
+      <c r="D91" s="62">
+        <v>1</v>
+      </c>
       <c r="E91" s="63">
-        <f t="shared" ref="E91:F93" si="16">DATE(2021,4,13)</f>
+        <f t="shared" ref="E91:F93" si="14">DATE(2021,4,13)</f>
         <v>44299</v>
       </c>
       <c r="F91" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44299</v>
       </c>
       <c r="G91" s="27"/>
@@ -8817,11 +8867,11 @@
       <c r="C92" s="61"/>
       <c r="D92" s="62"/>
       <c r="E92" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44299</v>
       </c>
       <c r="F92" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44299</v>
       </c>
       <c r="G92" s="27"/>
@@ -8891,11 +8941,11 @@
       <c r="C93" s="61"/>
       <c r="D93" s="62"/>
       <c r="E93" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44299</v>
       </c>
       <c r="F93" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44299</v>
       </c>
       <c r="G93" s="27"/>
@@ -9181,13 +9231,15 @@
         <v>113</v>
       </c>
       <c r="C97" s="30"/>
-      <c r="D97" s="31"/>
+      <c r="D97" s="31">
+        <v>1</v>
+      </c>
       <c r="E97" s="66">
-        <f t="shared" ref="E97:F99" si="17">DATE(2021,4,14)</f>
+        <f t="shared" ref="E97:F99" si="15">DATE(2021,4,14)</f>
         <v>44300</v>
       </c>
       <c r="F97" s="66">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>44300</v>
       </c>
       <c r="G97" s="27"/>
@@ -9255,13 +9307,15 @@
         <v>114</v>
       </c>
       <c r="C98" s="30"/>
-      <c r="D98" s="31"/>
+      <c r="D98" s="31">
+        <v>1</v>
+      </c>
       <c r="E98" s="66">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>44300</v>
       </c>
       <c r="F98" s="66">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>44300</v>
       </c>
       <c r="G98" s="27"/>
@@ -9329,13 +9383,15 @@
         <v>115</v>
       </c>
       <c r="C99" s="30"/>
-      <c r="D99" s="31"/>
+      <c r="D99" s="31">
+        <v>1</v>
+      </c>
       <c r="E99" s="66">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>44300</v>
       </c>
       <c r="F99" s="66">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>44300</v>
       </c>
       <c r="G99" s="27"/>
@@ -9477,7 +9533,9 @@
         <v>86</v>
       </c>
       <c r="C101" s="30"/>
-      <c r="D101" s="31"/>
+      <c r="D101" s="31">
+        <v>1</v>
+      </c>
       <c r="E101" s="66">
         <f>DATE(2021,4,14)</f>
         <v>44300</v>
@@ -9553,11 +9611,11 @@
       <c r="C102" s="30"/>
       <c r="D102" s="31"/>
       <c r="E102" s="66">
-        <f t="shared" ref="E102:F105" si="18">DATE(2021,4,15)</f>
+        <f t="shared" ref="E102:F105" si="16">DATE(2021,4,15)</f>
         <v>44301</v>
       </c>
       <c r="F102" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>44301</v>
       </c>
       <c r="G102" s="27"/>
@@ -9625,13 +9683,15 @@
         <v>118</v>
       </c>
       <c r="C103" s="30"/>
-      <c r="D103" s="31"/>
+      <c r="D103" s="31">
+        <v>1</v>
+      </c>
       <c r="E103" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>44301</v>
       </c>
       <c r="F103" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>44301</v>
       </c>
       <c r="G103" s="27"/>
@@ -9701,11 +9761,11 @@
       <c r="C104" s="30"/>
       <c r="D104" s="31"/>
       <c r="E104" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>44301</v>
       </c>
       <c r="F104" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>44301</v>
       </c>
       <c r="G104" s="27"/>
@@ -9775,11 +9835,11 @@
       <c r="C105" s="30"/>
       <c r="D105" s="31"/>
       <c r="E105" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>44301</v>
       </c>
       <c r="F105" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>44301</v>
       </c>
       <c r="G105" s="27"/>
@@ -9919,12 +9979,12 @@
       <c r="C107" s="43"/>
       <c r="D107" s="44"/>
       <c r="E107" s="45">
-        <f t="shared" ref="E107:F110" si="19">DATE(2021,4,16)</f>
-        <v>44302</v>
+        <f>DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F107" s="45">
-        <f t="shared" si="19"/>
-        <v>44302</v>
+        <f t="shared" ref="F107:F110" si="17">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="G107" s="27"/>
       <c r="H107" s="27"/>
@@ -9993,12 +10053,12 @@
       <c r="C108" s="43"/>
       <c r="D108" s="44"/>
       <c r="E108" s="45">
-        <f t="shared" si="19"/>
-        <v>44302</v>
+        <f t="shared" ref="E108:E110" si="18">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F108" s="45">
-        <f t="shared" si="19"/>
-        <v>44302</v>
+        <f t="shared" si="17"/>
+        <v>44307</v>
       </c>
       <c r="G108" s="27"/>
       <c r="H108" s="27"/>
@@ -10067,12 +10127,12 @@
       <c r="C109" s="43"/>
       <c r="D109" s="44"/>
       <c r="E109" s="45">
-        <f t="shared" si="19"/>
-        <v>44302</v>
+        <f t="shared" si="18"/>
+        <v>44307</v>
       </c>
       <c r="F109" s="45">
-        <f t="shared" si="19"/>
-        <v>44302</v>
+        <f t="shared" si="17"/>
+        <v>44307</v>
       </c>
       <c r="G109" s="27"/>
       <c r="H109" s="27"/>
@@ -10141,12 +10201,12 @@
       <c r="C110" s="43"/>
       <c r="D110" s="44"/>
       <c r="E110" s="45">
-        <f t="shared" si="19"/>
-        <v>44302</v>
+        <f t="shared" si="18"/>
+        <v>44307</v>
       </c>
       <c r="F110" s="45">
-        <f t="shared" si="19"/>
-        <v>44302</v>
+        <f t="shared" si="17"/>
+        <v>44307</v>
       </c>
       <c r="G110" s="27"/>
       <c r="H110" s="27"/>
@@ -10285,12 +10345,12 @@
       <c r="C112" s="52"/>
       <c r="D112" s="53"/>
       <c r="E112" s="54">
-        <f>DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f>DATE(2021,4,16)</f>
+        <v>44302</v>
       </c>
       <c r="F112" s="54">
-        <f t="shared" ref="F112:F113" si="20">DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f t="shared" ref="F112:F116" si="19">DATE(2021,4,16)</f>
+        <v>44302</v>
       </c>
       <c r="G112" s="27"/>
       <c r="H112" s="27"/>
@@ -10359,12 +10419,12 @@
       <c r="C113" s="52"/>
       <c r="D113" s="53"/>
       <c r="E113" s="54">
-        <f>DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f t="shared" ref="E113:E116" si="20">DATE(2021,4,16)</f>
+        <v>44302</v>
       </c>
       <c r="F113" s="54">
-        <f t="shared" si="20"/>
-        <v>44298</v>
+        <f t="shared" si="19"/>
+        <v>44302</v>
       </c>
       <c r="G113" s="27"/>
       <c r="H113" s="27"/>
@@ -10433,12 +10493,12 @@
       <c r="C114" s="52"/>
       <c r="D114" s="53"/>
       <c r="E114" s="54">
-        <f>DATE(2021,4,13)</f>
-        <v>44299</v>
+        <f t="shared" si="20"/>
+        <v>44302</v>
       </c>
       <c r="F114" s="54">
-        <f>DATE(2021,4,13)</f>
-        <v>44299</v>
+        <f t="shared" si="19"/>
+        <v>44302</v>
       </c>
       <c r="G114" s="27"/>
       <c r="H114" s="27"/>
@@ -10507,12 +10567,12 @@
       <c r="C115" s="52"/>
       <c r="D115" s="53"/>
       <c r="E115" s="54">
-        <f t="shared" ref="E115:F116" si="21">DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f t="shared" si="20"/>
+        <v>44302</v>
       </c>
       <c r="F115" s="54">
-        <f t="shared" si="21"/>
-        <v>44298</v>
+        <f t="shared" si="19"/>
+        <v>44302</v>
       </c>
       <c r="G115" s="27"/>
       <c r="H115" s="27"/>
@@ -10581,12 +10641,12 @@
       <c r="C116" s="52"/>
       <c r="D116" s="53"/>
       <c r="E116" s="54">
-        <f t="shared" si="21"/>
-        <v>44298</v>
+        <f t="shared" si="20"/>
+        <v>44302</v>
       </c>
       <c r="F116" s="54">
-        <f t="shared" si="21"/>
-        <v>44298</v>
+        <f t="shared" si="19"/>
+        <v>44302</v>
       </c>
       <c r="G116" s="27"/>
       <c r="H116" s="27"/>
@@ -10725,11 +10785,11 @@
       <c r="C118" s="61"/>
       <c r="D118" s="62"/>
       <c r="E118" s="63">
-        <f t="shared" ref="E118:F120" si="22">DATE(2021,4,16)</f>
+        <f t="shared" ref="E118:F120" si="21">DATE(2021,4,16)</f>
         <v>44302</v>
       </c>
       <c r="F118" s="63">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>44302</v>
       </c>
       <c r="G118" s="27"/>
@@ -10799,11 +10859,11 @@
       <c r="C119" s="61"/>
       <c r="D119" s="62"/>
       <c r="E119" s="63">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>44302</v>
       </c>
       <c r="F119" s="63">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>44302</v>
       </c>
       <c r="G119" s="27"/>
@@ -10873,11 +10933,11 @@
       <c r="C120" s="61"/>
       <c r="D120" s="62"/>
       <c r="E120" s="63">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>44302</v>
       </c>
       <c r="F120" s="63">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>44302</v>
       </c>
       <c r="G120" s="27"/>
@@ -10947,11 +11007,11 @@
       <c r="C121" s="61"/>
       <c r="D121" s="62"/>
       <c r="E121" s="63">
-        <f t="shared" ref="E121:F124" si="23">DATE(2021,4,19)</f>
+        <f t="shared" ref="E121:F124" si="22">DATE(2021,4,19)</f>
         <v>44305</v>
       </c>
       <c r="F121" s="63">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>44305</v>
       </c>
       <c r="G121" s="27"/>
@@ -11021,11 +11081,11 @@
       <c r="C122" s="61"/>
       <c r="D122" s="62"/>
       <c r="E122" s="63">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>44305</v>
       </c>
       <c r="F122" s="63">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>44305</v>
       </c>
       <c r="G122" s="27"/>
@@ -11095,11 +11155,11 @@
       <c r="C123" s="67"/>
       <c r="D123" s="62"/>
       <c r="E123" s="63">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>44305</v>
       </c>
       <c r="F123" s="63">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>44305</v>
       </c>
       <c r="G123" s="27"/>
@@ -11169,11 +11229,11 @@
       <c r="C124" s="61"/>
       <c r="D124" s="62"/>
       <c r="E124" s="63">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>44305</v>
       </c>
       <c r="F124" s="63">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>44305</v>
       </c>
       <c r="G124" s="27"/>
@@ -11387,12 +11447,12 @@
       <c r="C127" s="30"/>
       <c r="D127" s="31"/>
       <c r="E127" s="32">
-        <f>DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f>DATE(2021,4,19)</f>
+        <v>44305</v>
       </c>
       <c r="F127" s="32">
-        <f>DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f>DATE(2021,4,19)</f>
+        <v>44305</v>
       </c>
       <c r="G127" s="27"/>
       <c r="H127" s="27"/>
@@ -11461,12 +11521,12 @@
       <c r="C128" s="30"/>
       <c r="D128" s="31"/>
       <c r="E128" s="32">
-        <f>DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f>DATE(2021,4,19)</f>
+        <v>44305</v>
       </c>
       <c r="F128" s="32">
-        <f>DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f>DATE(2021,4,19)</f>
+        <v>44305</v>
       </c>
       <c r="G128" s="27"/>
       <c r="H128" s="27"/>
@@ -11535,12 +11595,12 @@
       <c r="C129" s="30"/>
       <c r="D129" s="31"/>
       <c r="E129" s="32">
-        <f>DATE(2021,4,13)</f>
-        <v>44299</v>
+        <f t="shared" ref="E129:F131" si="23">DATE(2021,4,19)</f>
+        <v>44305</v>
       </c>
       <c r="F129" s="32">
-        <f>DATE(2021,4,13)</f>
-        <v>44299</v>
+        <f t="shared" si="23"/>
+        <v>44305</v>
       </c>
       <c r="G129" s="27"/>
       <c r="H129" s="27"/>
@@ -11609,12 +11669,12 @@
       <c r="C130" s="30"/>
       <c r="D130" s="31"/>
       <c r="E130" s="32">
-        <f t="shared" ref="E130:F131" si="24">DATE(2021,4,13)</f>
-        <v>44299</v>
+        <f t="shared" si="23"/>
+        <v>44305</v>
       </c>
       <c r="F130" s="32">
-        <f t="shared" si="24"/>
-        <v>44299</v>
+        <f t="shared" si="23"/>
+        <v>44305</v>
       </c>
       <c r="G130" s="27"/>
       <c r="H130" s="27"/>
@@ -11683,12 +11743,12 @@
       <c r="C131" s="30"/>
       <c r="D131" s="31"/>
       <c r="E131" s="32">
-        <f t="shared" si="24"/>
-        <v>44299</v>
+        <f t="shared" si="23"/>
+        <v>44305</v>
       </c>
       <c r="F131" s="32">
-        <f t="shared" si="24"/>
-        <v>44299</v>
+        <f t="shared" si="23"/>
+        <v>44305</v>
       </c>
       <c r="G131" s="27"/>
       <c r="H131" s="27"/>
@@ -11757,12 +11817,12 @@
       <c r="C132" s="30"/>
       <c r="D132" s="31"/>
       <c r="E132" s="32">
-        <f>DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f>DATE(2021,4,20)</f>
+        <v>44306</v>
       </c>
       <c r="F132" s="32">
-        <f>DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f t="shared" ref="F132:F133" si="24">DATE(2021,4,20)</f>
+        <v>44306</v>
       </c>
       <c r="G132" s="27"/>
       <c r="H132" s="27"/>
@@ -11831,12 +11891,12 @@
       <c r="C133" s="30"/>
       <c r="D133" s="31"/>
       <c r="E133" s="32">
-        <f>DATE(2021,4,15)</f>
-        <v>44301</v>
+        <f t="shared" ref="E133:F133" si="25">DATE(2021,4,20)</f>
+        <v>44306</v>
       </c>
       <c r="F133" s="32">
-        <f>DATE(2021,4,15)</f>
-        <v>44301</v>
+        <f t="shared" si="24"/>
+        <v>44306</v>
       </c>
       <c r="G133" s="27"/>
       <c r="H133" s="27"/>
@@ -11974,13 +12034,13 @@
       </c>
       <c r="C135" s="43"/>
       <c r="D135" s="44"/>
-      <c r="E135" s="45">
-        <f>DATE(2021,4,15)</f>
-        <v>44301</v>
-      </c>
-      <c r="F135" s="45">
-        <f>DATE(2021,4,15)</f>
-        <v>44301</v>
+      <c r="E135" s="105">
+        <f t="shared" ref="E135:F137" si="26">DATE(2021,4,20)</f>
+        <v>44306</v>
+      </c>
+      <c r="F135" s="105">
+        <f t="shared" si="26"/>
+        <v>44306</v>
       </c>
       <c r="G135" s="27"/>
       <c r="H135" s="27"/>
@@ -12048,13 +12108,13 @@
       </c>
       <c r="C136" s="43"/>
       <c r="D136" s="44"/>
-      <c r="E136" s="45">
-        <f t="shared" ref="E136:F137" si="25">DATE(2021,4,15)</f>
-        <v>44301</v>
-      </c>
-      <c r="F136" s="45">
-        <f t="shared" si="25"/>
-        <v>44301</v>
+      <c r="E136" s="105">
+        <f t="shared" si="26"/>
+        <v>44306</v>
+      </c>
+      <c r="F136" s="105">
+        <f t="shared" si="26"/>
+        <v>44306</v>
       </c>
       <c r="G136" s="27"/>
       <c r="H136" s="27"/>
@@ -12122,13 +12182,13 @@
       </c>
       <c r="C137" s="43"/>
       <c r="D137" s="44"/>
-      <c r="E137" s="45">
-        <f t="shared" si="25"/>
-        <v>44301</v>
-      </c>
-      <c r="F137" s="45">
-        <f t="shared" si="25"/>
-        <v>44301</v>
+      <c r="E137" s="105">
+        <f t="shared" si="26"/>
+        <v>44306</v>
+      </c>
+      <c r="F137" s="105">
+        <f t="shared" si="26"/>
+        <v>44306</v>
       </c>
       <c r="G137" s="27"/>
       <c r="H137" s="27"/>
@@ -12197,12 +12257,12 @@
       <c r="C138" s="43"/>
       <c r="D138" s="44"/>
       <c r="E138" s="45">
-        <f>DATE(2021,4,16)</f>
-        <v>44302</v>
+        <f>DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F138" s="45">
-        <f>DATE(2021,4,16)</f>
-        <v>44302</v>
+        <f t="shared" ref="F138:F140" si="27">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="G138" s="27"/>
       <c r="H138" s="27"/>
@@ -12271,12 +12331,12 @@
       <c r="C139" s="43"/>
       <c r="D139" s="44"/>
       <c r="E139" s="45">
-        <f>DATE(2021,4,16)</f>
-        <v>44302</v>
+        <f t="shared" ref="E139:F140" si="28">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F139" s="45">
-        <f t="shared" ref="F139:F142" si="26">DATE(2021,4,16)</f>
-        <v>44302</v>
+        <f t="shared" si="27"/>
+        <v>44307</v>
       </c>
       <c r="G139" s="27"/>
       <c r="H139" s="27"/>
@@ -12345,12 +12405,12 @@
       <c r="C140" s="43"/>
       <c r="D140" s="44"/>
       <c r="E140" s="45">
-        <f t="shared" ref="E140:E141" si="27">DATE(2021,4,16)</f>
-        <v>44302</v>
+        <f t="shared" si="28"/>
+        <v>44307</v>
       </c>
       <c r="F140" s="45">
-        <f t="shared" si="26"/>
-        <v>44302</v>
+        <f t="shared" si="27"/>
+        <v>44307</v>
       </c>
       <c r="G140" s="27"/>
       <c r="H140" s="27"/>
@@ -12419,12 +12479,12 @@
       <c r="C141" s="43"/>
       <c r="D141" s="44"/>
       <c r="E141" s="45">
-        <f t="shared" si="27"/>
-        <v>44302</v>
+        <f>DATE(2021,4,22)</f>
+        <v>44308</v>
       </c>
       <c r="F141" s="45">
-        <f t="shared" si="26"/>
-        <v>44302</v>
+        <f t="shared" ref="F141:F142" si="29">DATE(2021,4,22)</f>
+        <v>44308</v>
       </c>
       <c r="G141" s="27"/>
       <c r="H141" s="27"/>
@@ -12493,12 +12553,12 @@
       <c r="C142" s="43"/>
       <c r="D142" s="44"/>
       <c r="E142" s="45">
-        <f>DATE(2021,4,19)</f>
-        <v>44305</v>
+        <f t="shared" ref="E142:F142" si="30">DATE(2021,4,22)</f>
+        <v>44308</v>
       </c>
       <c r="F142" s="45">
-        <f t="shared" si="26"/>
-        <v>44302</v>
+        <f t="shared" si="29"/>
+        <v>44308</v>
       </c>
       <c r="G142" s="27"/>
       <c r="H142" s="27"/>
@@ -12708,6 +12768,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="W4:AC4"/>
@@ -12715,11 +12780,6 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D38 D61:D64 D71:D74 D81 D84:D89 D103:D105 D124:D125 D143">
     <cfRule type="dataBar" priority="2">

</xml_diff>

<commit_message>
minor changes, gantt chart update
</commit_message>
<xml_diff>
--- a/Documentation/Obtayn-gantt-chart.xlsx
+++ b/Documentation/Obtayn-gantt-chart.xlsx
@@ -1030,7 +1030,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1184,7 +1184,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1208,11 +1208,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="24" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1236,7 +1236,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1272,7 +1272,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1288,7 +1288,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="24" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1312,7 +1312,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1332,7 +1332,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1356,7 +1356,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1588,9 +1588,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1904040</xdr:colOff>
+      <xdr:colOff>1903680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1606,7 +1606,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="95400"/>
-          <a:ext cx="1904040" cy="427680"/>
+          <a:ext cx="1903680" cy="427320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1629,12 +1629,12 @@
   <dimension ref="A1:BL146"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D119" activeCellId="0" sqref="D119"/>
+      <selection pane="bottomLeft" activeCell="B120" activeCellId="0" sqref="B120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.58"/>
@@ -7502,7 +7502,9 @@
         <v>92</v>
       </c>
       <c r="C76" s="47"/>
-      <c r="D76" s="48"/>
+      <c r="D76" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="E76" s="49" t="n">
         <f aca="false">DATE(2021,4,12)</f>
         <v>44298</v>
@@ -7576,7 +7578,9 @@
         <v>93</v>
       </c>
       <c r="C77" s="47"/>
-      <c r="D77" s="48"/>
+      <c r="D77" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="E77" s="49" t="n">
         <f aca="false">DATE(2021,4,12)</f>
         <v>44298</v>
@@ -7650,7 +7654,9 @@
         <v>94</v>
       </c>
       <c r="C78" s="47"/>
-      <c r="D78" s="48"/>
+      <c r="D78" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="E78" s="49" t="n">
         <f aca="false">DATE(2021,4,12)</f>
         <v>44298</v>
@@ -8016,7 +8022,9 @@
         <v>99</v>
       </c>
       <c r="C83" s="77"/>
-      <c r="D83" s="78"/>
+      <c r="D83" s="78" t="n">
+        <v>1</v>
+      </c>
       <c r="E83" s="79" t="n">
         <f aca="false">DATE(2021,4,15)</f>
         <v>44301</v>
@@ -8090,7 +8098,9 @@
         <v>100</v>
       </c>
       <c r="C84" s="77"/>
-      <c r="D84" s="78"/>
+      <c r="D84" s="78" t="n">
+        <v>1</v>
+      </c>
       <c r="E84" s="79" t="n">
         <f aca="false">DATE(2021,4,15)</f>
         <v>44301</v>
@@ -8238,7 +8248,9 @@
         <v>102</v>
       </c>
       <c r="C86" s="77"/>
-      <c r="D86" s="78"/>
+      <c r="D86" s="78" t="n">
+        <v>1</v>
+      </c>
       <c r="E86" s="79" t="n">
         <f aca="false">DATE(2021,4,21)</f>
         <v>44307</v>
@@ -8386,7 +8398,9 @@
         <v>104</v>
       </c>
       <c r="C88" s="77"/>
-      <c r="D88" s="78"/>
+      <c r="D88" s="78" t="n">
+        <v>1</v>
+      </c>
       <c r="E88" s="79" t="n">
         <f aca="false">DATE(2021,4,21)</f>
         <v>44307</v>
@@ -9804,7 +9818,9 @@
         <v>99</v>
       </c>
       <c r="C107" s="47"/>
-      <c r="D107" s="48"/>
+      <c r="D107" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="E107" s="49" t="n">
         <f aca="false">DATE(2021,4,21)</f>
         <v>44307</v>
@@ -9878,7 +9894,9 @@
         <v>121</v>
       </c>
       <c r="C108" s="47"/>
-      <c r="D108" s="48"/>
+      <c r="D108" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="E108" s="49" t="n">
         <f aca="false">DATE(2021,4,21)</f>
         <v>44307</v>
@@ -9952,7 +9970,9 @@
         <v>102</v>
       </c>
       <c r="C109" s="47"/>
-      <c r="D109" s="48"/>
+      <c r="D109" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="E109" s="49" t="n">
         <f aca="false">DATE(2021,4,21)</f>
         <v>44307</v>
@@ -10026,7 +10046,9 @@
         <v>104</v>
       </c>
       <c r="C110" s="47"/>
-      <c r="D110" s="48"/>
+      <c r="D110" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="E110" s="49" t="n">
         <f aca="false">DATE(2021,4,21)</f>
         <v>44307</v>
@@ -10170,7 +10192,9 @@
         <v>123</v>
       </c>
       <c r="C112" s="77"/>
-      <c r="D112" s="78"/>
+      <c r="D112" s="78" t="n">
+        <v>1</v>
+      </c>
       <c r="E112" s="79" t="n">
         <f aca="false">DATE(2021,4,16)</f>
         <v>44302</v>
@@ -10244,7 +10268,9 @@
         <v>124</v>
       </c>
       <c r="C113" s="77"/>
-      <c r="D113" s="78"/>
+      <c r="D113" s="78" t="n">
+        <v>1</v>
+      </c>
       <c r="E113" s="79" t="n">
         <f aca="false">DATE(2021,4,16)</f>
         <v>44302</v>
@@ -10318,7 +10344,9 @@
         <v>125</v>
       </c>
       <c r="C114" s="77"/>
-      <c r="D114" s="78"/>
+      <c r="D114" s="78" t="n">
+        <v>1</v>
+      </c>
       <c r="E114" s="79" t="n">
         <f aca="false">DATE(2021,4,16)</f>
         <v>44302</v>
@@ -12617,7 +12645,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1E3A29CB-A3A0-414B-AA80-47A22E2DEE3F}</x14:id>
+          <x14:id>{8D42991C-D645-48E7-A776-C05AEDEF4BD0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12644,7 +12672,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4A6D3DF0-2441-4CF0-B945-53CCC3D7681C}</x14:id>
+          <x14:id>{DFD93713-8851-40AB-B8BB-6A2ADACFAEFF}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12658,7 +12686,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A44A48ED-A171-4282-8250-FA526D30B77B}</x14:id>
+          <x14:id>{21C0784E-30B3-4999-BF75-A01E135D336B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12672,7 +12700,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4B6E9593-1B6C-4988-9F78-7D2AE4758BD9}</x14:id>
+          <x14:id>{B1D23618-C639-4FD9-BAA1-ED92BBDBE36D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12686,7 +12714,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3700DCB4-C083-4C9C-8F6D-94D2282AC520}</x14:id>
+          <x14:id>{15592367-4D25-48EE-B553-C57B588D7191}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12700,7 +12728,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ABBE991E-807A-4914-8393-FE6DE2A7CD9F}</x14:id>
+          <x14:id>{E01D9BC0-2B38-4093-8C41-80FFE6932554}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12714,7 +12742,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{543A7AAF-9DE4-43B9-A83D-F06E804DEECC}</x14:id>
+          <x14:id>{A2C0B4A2-FF66-4E20-80F0-2BB824BB6E20}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12728,7 +12756,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{63D6A198-D015-4BD5-B1A5-F3FA50F19495}</x14:id>
+          <x14:id>{3A412A91-4B81-4E50-A8DB-BC997326621A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12742,7 +12770,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1E4A9916-4F12-432A-9116-71545FB3D284}</x14:id>
+          <x14:id>{C2DF9CA3-6014-42EB-9555-A744CE4773CA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12756,7 +12784,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{71872257-5790-42E7-A696-5CD58461523A}</x14:id>
+          <x14:id>{AF60A951-66B4-4962-95E5-D6337E7860F7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12770,7 +12798,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{52BFE0C4-91E5-405B-8F70-C0C8B6D52647}</x14:id>
+          <x14:id>{D68F7780-6F59-4C8A-A48A-73A78B7E8F49}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12784,7 +12812,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{25DE9868-2974-47E0-B6A3-CC3AA093E448}</x14:id>
+          <x14:id>{435AD490-3680-4C8D-8F45-D19C7AB988DA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12798,7 +12826,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{56F6802F-CE29-44C6-B463-4FA03CD06BD9}</x14:id>
+          <x14:id>{E2577128-187F-4885-B172-6F5D41B9256E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12812,7 +12840,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B1AEA79A-F5A8-4AE6-A316-44B9BE152AB4}</x14:id>
+          <x14:id>{5CA4A411-8BF0-4EC0-AA7A-4189C286316D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12826,7 +12854,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F2F8ADDC-CE80-4CF2-ADA3-AEE9B2FCA59F}</x14:id>
+          <x14:id>{6A38A5D5-9ADC-481E-819A-90FC64685F63}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12840,7 +12868,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A74B6B1A-7EB4-45D1-B23C-F32AAA25EA6B}</x14:id>
+          <x14:id>{90B03EA0-541D-4260-9A73-B5F04F926D49}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12854,7 +12882,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{11F6A9E0-9F25-409C-A56F-96167DAEB319}</x14:id>
+          <x14:id>{ABF75091-F0BB-4BD2-8977-65FB5A7E725C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12868,7 +12896,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D6EFF06B-2A40-4CC9-9128-F07035D491DC}</x14:id>
+          <x14:id>{58425357-D7F4-4719-8C50-B3EBD43E8450}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12882,7 +12910,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{65EC955A-3B7F-41D0-989C-411FBAC0687A}</x14:id>
+          <x14:id>{5F2E50C5-8099-44BD-9945-19D6AFCF2B41}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12904,7 +12932,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1E3A29CB-A3A0-414B-AA80-47A22E2DEE3F}">
+          <x14:cfRule type="dataBar" id="{8D42991C-D645-48E7-A776-C05AEDEF4BD0}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12919,7 +12947,7 @@
           <xm:sqref>D7:D38 D61:D64 D71:D74 D81 D84:D89 D103:D105 D124:D125 D143</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4A6D3DF0-2441-4CF0-B945-53CCC3D7681C}">
+          <x14:cfRule type="dataBar" id="{DFD93713-8851-40AB-B8BB-6A2ADACFAEFF}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12934,7 +12962,7 @@
           <xm:sqref>D75:D80</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A44A48ED-A171-4282-8250-FA526D30B77B}">
+          <x14:cfRule type="dataBar" id="{21C0784E-30B3-4999-BF75-A01E135D336B}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12949,7 +12977,7 @@
           <xm:sqref>D111:D112</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4B6E9593-1B6C-4988-9F78-7D2AE4758BD9}">
+          <x14:cfRule type="dataBar" id="{B1D23618-C639-4FD9-BAA1-ED92BBDBE36D}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12964,7 +12992,7 @@
           <xm:sqref>D134:D142</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3700DCB4-C083-4C9C-8F6D-94D2282AC520}">
+          <x14:cfRule type="dataBar" id="{15592367-4D25-48EE-B553-C57B588D7191}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12979,7 +13007,7 @@
           <xm:sqref>D39:D44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ABBE991E-807A-4914-8393-FE6DE2A7CD9F}">
+          <x14:cfRule type="dataBar" id="{E01D9BC0-2B38-4093-8C41-80FFE6932554}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12994,7 +13022,7 @@
           <xm:sqref>D45:D50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{543A7AAF-9DE4-43B9-A83D-F06E804DEECC}">
+          <x14:cfRule type="dataBar" id="{A2C0B4A2-FF66-4E20-80F0-2BB824BB6E20}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13009,7 +13037,7 @@
           <xm:sqref>D51:D52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{63D6A198-D015-4BD5-B1A5-F3FA50F19495}">
+          <x14:cfRule type="dataBar" id="{3A412A91-4B81-4E50-A8DB-BC997326621A}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13024,7 +13052,7 @@
           <xm:sqref>D53:D60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1E4A9916-4F12-432A-9116-71545FB3D284}">
+          <x14:cfRule type="dataBar" id="{C2DF9CA3-6014-42EB-9555-A744CE4773CA}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13039,7 +13067,7 @@
           <xm:sqref>D65:D70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{71872257-5790-42E7-A696-5CD58461523A}">
+          <x14:cfRule type="dataBar" id="{AF60A951-66B4-4962-95E5-D6337E7860F7}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13054,7 +13082,7 @@
           <xm:sqref>D82:D83</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{52BFE0C4-91E5-405B-8F70-C0C8B6D52647}">
+          <x14:cfRule type="dataBar" id="{D68F7780-6F59-4C8A-A48A-73A78B7E8F49}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13069,7 +13097,7 @@
           <xm:sqref>D113:D116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{25DE9868-2974-47E0-B6A3-CC3AA093E448}">
+          <x14:cfRule type="dataBar" id="{435AD490-3680-4C8D-8F45-D19C7AB988DA}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13084,7 +13112,7 @@
           <xm:sqref>D90:D95</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{56F6802F-CE29-44C6-B463-4FA03CD06BD9}">
+          <x14:cfRule type="dataBar" id="{E2577128-187F-4885-B172-6F5D41B9256E}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13099,7 +13127,7 @@
           <xm:sqref>D102</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B1AEA79A-F5A8-4AE6-A316-44B9BE152AB4}">
+          <x14:cfRule type="dataBar" id="{5CA4A411-8BF0-4EC0-AA7A-4189C286316D}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13114,7 +13142,7 @@
           <xm:sqref>D96:D101</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F2F8ADDC-CE80-4CF2-ADA3-AEE9B2FCA59F}">
+          <x14:cfRule type="dataBar" id="{6A38A5D5-9ADC-481E-819A-90FC64685F63}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13129,7 +13157,7 @@
           <xm:sqref>D106:D110</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A74B6B1A-7EB4-45D1-B23C-F32AAA25EA6B}">
+          <x14:cfRule type="dataBar" id="{90B03EA0-541D-4260-9A73-B5F04F926D49}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13144,7 +13172,7 @@
           <xm:sqref>D126:D131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{11F6A9E0-9F25-409C-A56F-96167DAEB319}">
+          <x14:cfRule type="dataBar" id="{ABF75091-F0BB-4BD2-8977-65FB5A7E725C}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13159,7 +13187,7 @@
           <xm:sqref>D117:D123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D6EFF06B-2A40-4CC9-9128-F07035D491DC}">
+          <x14:cfRule type="dataBar" id="{58425357-D7F4-4719-8C50-B3EBD43E8450}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13174,7 +13202,7 @@
           <xm:sqref>D133</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{65EC955A-3B7F-41D0-989C-411FBAC0687A}">
+          <x14:cfRule type="dataBar" id="{5F2E50C5-8099-44BD-9945-19D6AFCF2B41}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13205,7 +13233,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="93" width="87.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="6" width="9.13"/>

</xml_diff>

<commit_message>
changed Feed avatar, added req component buttons
</commit_message>
<xml_diff>
--- a/Documentation/Obtayn-gantt-chart.xlsx
+++ b/Documentation/Obtayn-gantt-chart.xlsx
@@ -1030,7 +1030,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1184,7 +1184,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1208,11 +1208,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="24" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1236,7 +1236,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1272,7 +1272,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1288,7 +1288,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="24" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1312,7 +1312,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1332,7 +1332,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1356,7 +1356,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1588,9 +1588,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1903680</xdr:colOff>
+      <xdr:colOff>1903320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>522720</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1606,7 +1606,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="95400"/>
-          <a:ext cx="1903680" cy="427320"/>
+          <a:ext cx="1903320" cy="426960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1629,12 +1629,12 @@
   <dimension ref="A1:BL146"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B120" activeCellId="0" sqref="B120"/>
+      <selection pane="bottomLeft" activeCell="L125" activeCellId="0" sqref="L125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.58"/>
@@ -10714,7 +10714,9 @@
         <v>130</v>
       </c>
       <c r="C119" s="66"/>
-      <c r="D119" s="67"/>
+      <c r="D119" s="67" t="n">
+        <v>1</v>
+      </c>
       <c r="E119" s="68" t="n">
         <f aca="false">DATE(2021,4,16)</f>
         <v>44302</v>
@@ -10788,7 +10790,9 @@
         <v>131</v>
       </c>
       <c r="C120" s="66"/>
-      <c r="D120" s="67"/>
+      <c r="D120" s="67" t="n">
+        <v>1</v>
+      </c>
       <c r="E120" s="68" t="n">
         <f aca="false">DATE(2021,4,16)</f>
         <v>44302</v>
@@ -10862,7 +10866,9 @@
         <v>132</v>
       </c>
       <c r="C121" s="66"/>
-      <c r="D121" s="67"/>
+      <c r="D121" s="67" t="n">
+        <v>1</v>
+      </c>
       <c r="E121" s="68" t="n">
         <f aca="false">DATE(2021,4,19)</f>
         <v>44305</v>
@@ -10936,7 +10942,9 @@
         <v>133</v>
       </c>
       <c r="C122" s="66"/>
-      <c r="D122" s="67"/>
+      <c r="D122" s="67" t="n">
+        <v>1</v>
+      </c>
       <c r="E122" s="68" t="n">
         <f aca="false">DATE(2021,4,19)</f>
         <v>44305</v>
@@ -11004,13 +11012,15 @@
       <c r="BK122" s="25"/>
       <c r="BL122" s="25"/>
     </row>
-    <row r="123" s="32" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="123" s="32" customFormat="true" ht="57.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
       <c r="B123" s="65" t="s">
         <v>134</v>
       </c>
       <c r="C123" s="81"/>
-      <c r="D123" s="67"/>
+      <c r="D123" s="67" t="n">
+        <v>1</v>
+      </c>
       <c r="E123" s="68" t="n">
         <f aca="false">DATE(2021,4,19)</f>
         <v>44305</v>
@@ -11084,7 +11094,9 @@
         <v>135</v>
       </c>
       <c r="C124" s="66"/>
-      <c r="D124" s="67"/>
+      <c r="D124" s="67" t="n">
+        <v>1</v>
+      </c>
       <c r="E124" s="68" t="n">
         <f aca="false">DATE(2021,4,19)</f>
         <v>44305</v>
@@ -11152,13 +11164,15 @@
       <c r="BK124" s="25"/>
       <c r="BL124" s="25"/>
     </row>
-    <row r="125" s="32" customFormat="true" ht="57.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="125" s="32" customFormat="true" ht="96" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="1"/>
       <c r="B125" s="65" t="s">
         <v>136</v>
       </c>
       <c r="C125" s="66"/>
-      <c r="D125" s="67"/>
+      <c r="D125" s="67" t="n">
+        <v>1</v>
+      </c>
       <c r="E125" s="68" t="n">
         <f aca="false">DATE(2021,4,20)</f>
         <v>44306</v>
@@ -12645,7 +12659,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8D42991C-D645-48E7-A776-C05AEDEF4BD0}</x14:id>
+          <x14:id>{7797717E-2A97-4152-951E-63FF88D6D74B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12672,7 +12686,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{DFD93713-8851-40AB-B8BB-6A2ADACFAEFF}</x14:id>
+          <x14:id>{2C316CFB-CED1-42F0-A657-76909045C2CC}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12686,7 +12700,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{21C0784E-30B3-4999-BF75-A01E135D336B}</x14:id>
+          <x14:id>{1043AD58-D0A1-4067-ACC0-1B6B2E6380DE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12700,7 +12714,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B1D23618-C639-4FD9-BAA1-ED92BBDBE36D}</x14:id>
+          <x14:id>{768A9717-CBD0-4E37-B3B2-4359C0A99BE5}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12714,7 +12728,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{15592367-4D25-48EE-B553-C57B588D7191}</x14:id>
+          <x14:id>{B46F28DA-64F1-4B2D-AB1D-D5E674A2364C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12728,7 +12742,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E01D9BC0-2B38-4093-8C41-80FFE6932554}</x14:id>
+          <x14:id>{3247F9DA-6B54-488A-8A56-F827EEB2A01F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12742,7 +12756,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A2C0B4A2-FF66-4E20-80F0-2BB824BB6E20}</x14:id>
+          <x14:id>{1E2B7594-D079-4236-8FC0-9912B4B32BF3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12756,7 +12770,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3A412A91-4B81-4E50-A8DB-BC997326621A}</x14:id>
+          <x14:id>{5380EA1B-7BF6-4DCB-9641-2361A7B0E18F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12770,7 +12784,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C2DF9CA3-6014-42EB-9555-A744CE4773CA}</x14:id>
+          <x14:id>{4F73E35C-D293-42BB-88B1-E652B0FAFE49}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12784,7 +12798,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{AF60A951-66B4-4962-95E5-D6337E7860F7}</x14:id>
+          <x14:id>{3733A1B1-46F3-4848-BCC9-F9C048E2A4E5}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12798,7 +12812,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D68F7780-6F59-4C8A-A48A-73A78B7E8F49}</x14:id>
+          <x14:id>{648BAD85-A18B-456F-9A7A-C73491D15062}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12812,7 +12826,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{435AD490-3680-4C8D-8F45-D19C7AB988DA}</x14:id>
+          <x14:id>{38C762CC-9C60-4A25-A8A0-E3F03DD0E3A8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12826,7 +12840,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E2577128-187F-4885-B172-6F5D41B9256E}</x14:id>
+          <x14:id>{191C5526-B428-4D48-A048-A4248C83AE74}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12840,7 +12854,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5CA4A411-8BF0-4EC0-AA7A-4189C286316D}</x14:id>
+          <x14:id>{201037ED-F28F-4ECF-92A7-54AB88396950}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12854,7 +12868,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6A38A5D5-9ADC-481E-819A-90FC64685F63}</x14:id>
+          <x14:id>{5A282831-6D83-422E-9E92-A6E96F1980DD}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12868,7 +12882,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{90B03EA0-541D-4260-9A73-B5F04F926D49}</x14:id>
+          <x14:id>{8F37671B-A0EF-404B-9E46-9ADBA385BADE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12882,7 +12896,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ABF75091-F0BB-4BD2-8977-65FB5A7E725C}</x14:id>
+          <x14:id>{A588F9DA-DD1B-4820-89C9-A8CAA1F96AE4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12896,7 +12910,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{58425357-D7F4-4719-8C50-B3EBD43E8450}</x14:id>
+          <x14:id>{14B511BC-EE53-4260-8D9F-D450911AC93F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12910,7 +12924,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5F2E50C5-8099-44BD-9945-19D6AFCF2B41}</x14:id>
+          <x14:id>{CAC7A453-9114-4781-9C87-40654984E2D8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12932,7 +12946,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8D42991C-D645-48E7-A776-C05AEDEF4BD0}">
+          <x14:cfRule type="dataBar" id="{7797717E-2A97-4152-951E-63FF88D6D74B}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12947,7 +12961,7 @@
           <xm:sqref>D7:D38 D61:D64 D71:D74 D81 D84:D89 D103:D105 D124:D125 D143</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DFD93713-8851-40AB-B8BB-6A2ADACFAEFF}">
+          <x14:cfRule type="dataBar" id="{2C316CFB-CED1-42F0-A657-76909045C2CC}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12962,7 +12976,7 @@
           <xm:sqref>D75:D80</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{21C0784E-30B3-4999-BF75-A01E135D336B}">
+          <x14:cfRule type="dataBar" id="{1043AD58-D0A1-4067-ACC0-1B6B2E6380DE}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12977,7 +12991,7 @@
           <xm:sqref>D111:D112</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B1D23618-C639-4FD9-BAA1-ED92BBDBE36D}">
+          <x14:cfRule type="dataBar" id="{768A9717-CBD0-4E37-B3B2-4359C0A99BE5}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -12992,7 +13006,7 @@
           <xm:sqref>D134:D142</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{15592367-4D25-48EE-B553-C57B588D7191}">
+          <x14:cfRule type="dataBar" id="{B46F28DA-64F1-4B2D-AB1D-D5E674A2364C}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13007,7 +13021,7 @@
           <xm:sqref>D39:D44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E01D9BC0-2B38-4093-8C41-80FFE6932554}">
+          <x14:cfRule type="dataBar" id="{3247F9DA-6B54-488A-8A56-F827EEB2A01F}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13022,7 +13036,7 @@
           <xm:sqref>D45:D50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A2C0B4A2-FF66-4E20-80F0-2BB824BB6E20}">
+          <x14:cfRule type="dataBar" id="{1E2B7594-D079-4236-8FC0-9912B4B32BF3}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13037,7 +13051,7 @@
           <xm:sqref>D51:D52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3A412A91-4B81-4E50-A8DB-BC997326621A}">
+          <x14:cfRule type="dataBar" id="{5380EA1B-7BF6-4DCB-9641-2361A7B0E18F}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13052,7 +13066,7 @@
           <xm:sqref>D53:D60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C2DF9CA3-6014-42EB-9555-A744CE4773CA}">
+          <x14:cfRule type="dataBar" id="{4F73E35C-D293-42BB-88B1-E652B0FAFE49}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13067,7 +13081,7 @@
           <xm:sqref>D65:D70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{AF60A951-66B4-4962-95E5-D6337E7860F7}">
+          <x14:cfRule type="dataBar" id="{3733A1B1-46F3-4848-BCC9-F9C048E2A4E5}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13082,7 +13096,7 @@
           <xm:sqref>D82:D83</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D68F7780-6F59-4C8A-A48A-73A78B7E8F49}">
+          <x14:cfRule type="dataBar" id="{648BAD85-A18B-456F-9A7A-C73491D15062}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13097,7 +13111,7 @@
           <xm:sqref>D113:D116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{435AD490-3680-4C8D-8F45-D19C7AB988DA}">
+          <x14:cfRule type="dataBar" id="{38C762CC-9C60-4A25-A8A0-E3F03DD0E3A8}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13112,7 +13126,7 @@
           <xm:sqref>D90:D95</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E2577128-187F-4885-B172-6F5D41B9256E}">
+          <x14:cfRule type="dataBar" id="{191C5526-B428-4D48-A048-A4248C83AE74}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13127,7 +13141,7 @@
           <xm:sqref>D102</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5CA4A411-8BF0-4EC0-AA7A-4189C286316D}">
+          <x14:cfRule type="dataBar" id="{201037ED-F28F-4ECF-92A7-54AB88396950}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13142,7 +13156,7 @@
           <xm:sqref>D96:D101</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6A38A5D5-9ADC-481E-819A-90FC64685F63}">
+          <x14:cfRule type="dataBar" id="{5A282831-6D83-422E-9E92-A6E96F1980DD}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13157,7 +13171,7 @@
           <xm:sqref>D106:D110</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{90B03EA0-541D-4260-9A73-B5F04F926D49}">
+          <x14:cfRule type="dataBar" id="{8F37671B-A0EF-404B-9E46-9ADBA385BADE}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13172,7 +13186,7 @@
           <xm:sqref>D126:D131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ABF75091-F0BB-4BD2-8977-65FB5A7E725C}">
+          <x14:cfRule type="dataBar" id="{A588F9DA-DD1B-4820-89C9-A8CAA1F96AE4}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13187,7 +13201,7 @@
           <xm:sqref>D117:D123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{58425357-D7F4-4719-8C50-B3EBD43E8450}">
+          <x14:cfRule type="dataBar" id="{14B511BC-EE53-4260-8D9F-D450911AC93F}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13202,7 +13216,7 @@
           <xm:sqref>D133</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5F2E50C5-8099-44BD-9945-19D6AFCF2B41}">
+          <x14:cfRule type="dataBar" id="{CAC7A453-9114-4781-9C87-40654984E2D8}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
added request deleted notification
</commit_message>
<xml_diff>
--- a/Documentation/Obtayn-gantt-chart.xlsx
+++ b/Documentation/Obtayn-gantt-chart.xlsx
@@ -1622,9 +1622,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1902600</xdr:colOff>
+      <xdr:colOff>1902240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>521640</xdr:rowOff>
+      <xdr:rowOff>521280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1640,7 +1640,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="95400"/>
-          <a:ext cx="1902600" cy="426240"/>
+          <a:ext cx="1902240" cy="425880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1663,12 +1663,12 @@
   <dimension ref="A1:BL146"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B133" activeCellId="0" sqref="B133"/>
+      <selection pane="bottomLeft" activeCell="E85" activeCellId="0" sqref="E85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="35.58"/>
@@ -8210,7 +8210,9 @@
         <v>101</v>
       </c>
       <c r="C85" s="77"/>
-      <c r="D85" s="78"/>
+      <c r="D85" s="78" t="n">
+        <v>1</v>
+      </c>
       <c r="E85" s="79" t="n">
         <f aca="false">DATE(2021,4,21)</f>
         <v>44307</v>
@@ -12710,7 +12712,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5F811F99-7539-43D5-A99D-377F4D1840C8}</x14:id>
+          <x14:id>{B3669140-B196-4E9C-BDAD-AD6E42CBB44E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12737,7 +12739,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{47568D90-94B5-49F5-83DD-C31FB08DF847}</x14:id>
+          <x14:id>{C2CB3C29-373E-41ED-9E53-D0E9291D538D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12751,7 +12753,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{70B3AFA9-B8AA-4598-8473-80629CFAD274}</x14:id>
+          <x14:id>{F55427F2-ADA4-4053-BD20-BC87DAE4C0E9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12765,7 +12767,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2D5424A5-7CE2-4970-B6F8-75E2746D2527}</x14:id>
+          <x14:id>{3989764E-F095-45A5-9BCB-84F63D668964}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12779,7 +12781,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{83E54036-476C-47BD-AE9E-F5EEA1EBF1BE}</x14:id>
+          <x14:id>{E62DF740-30B0-4D42-9B5A-95C7AE651613}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12793,7 +12795,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6833D88B-CE58-423C-8F6F-C036FD28CF16}</x14:id>
+          <x14:id>{AAFEC3C4-2157-4C36-85E7-C9D1AB9F9487}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12807,7 +12809,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4FCF14D3-6066-4337-9148-5CBDD9D97737}</x14:id>
+          <x14:id>{3CCAABB9-BE51-41BD-A38E-92B7CF006560}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12821,7 +12823,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7A3BCBB7-6551-46C2-9611-26939F5FF02D}</x14:id>
+          <x14:id>{89E5A2E2-30D6-4530-BD85-9BCABEE52AE6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12835,7 +12837,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3AB2A3C6-E21A-4FE5-BC8B-9F25C96D2D71}</x14:id>
+          <x14:id>{54E28360-96EE-4590-AD67-FFC87BDFE86D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12849,7 +12851,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5B65866B-9A81-4DE0-89EA-F27365ADD456}</x14:id>
+          <x14:id>{654748D6-D2F5-47CC-A450-DEE05C92C7B6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12863,7 +12865,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9020698F-D55A-4128-8170-9BE512E418AF}</x14:id>
+          <x14:id>{75B9AC4A-C313-4B66-8829-9DE39DBD11C4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12877,7 +12879,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{DADC10BE-BCA9-4687-B044-3042E53415E2}</x14:id>
+          <x14:id>{7F217241-83E3-4299-B254-88D5B6E78389}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12891,7 +12893,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{454F8872-D0E9-4CAA-9249-5DE754BE2819}</x14:id>
+          <x14:id>{CF2D83F6-BA8E-47E3-BCE4-2EEB30E6E945}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12905,7 +12907,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{62747F00-A1B9-4DA0-B723-705618A4FAB2}</x14:id>
+          <x14:id>{99A34868-2D4B-42C6-99C0-92E186CA3AF9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12919,7 +12921,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8FEFC9BB-4E79-4E68-A8D8-53C013AF3350}</x14:id>
+          <x14:id>{BAEDA295-B5CE-4E25-81AA-72406049E5F8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12933,7 +12935,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{505413A3-60D1-4214-BD7B-52B2403DCF93}</x14:id>
+          <x14:id>{E732D960-8A19-4AB8-B9A8-15D83ED7CA42}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12947,7 +12949,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8FD0EDC0-845B-4011-ACD3-7262A339ED62}</x14:id>
+          <x14:id>{209E7AE6-538E-4339-B715-9360DB9DB810}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12961,7 +12963,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F48C184A-78CE-4551-9E35-C9B767F56040}</x14:id>
+          <x14:id>{C1CF6C97-5AE0-42D0-BE41-2A3E23A88CA0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12975,7 +12977,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{403CE37D-7779-452E-B2DD-5A7978777391}</x14:id>
+          <x14:id>{58B91061-78FB-461A-ACD3-951AB82639F7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -12997,7 +12999,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5F811F99-7539-43D5-A99D-377F4D1840C8}">
+          <x14:cfRule type="dataBar" id="{B3669140-B196-4E9C-BDAD-AD6E42CBB44E}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13012,7 +13014,7 @@
           <xm:sqref>D7:D38 D61:D64 D71:D74 D81 D84:D89 D103:D105 D124:D125 D143</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{47568D90-94B5-49F5-83DD-C31FB08DF847}">
+          <x14:cfRule type="dataBar" id="{C2CB3C29-373E-41ED-9E53-D0E9291D538D}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13027,7 +13029,7 @@
           <xm:sqref>D75:D80</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{70B3AFA9-B8AA-4598-8473-80629CFAD274}">
+          <x14:cfRule type="dataBar" id="{F55427F2-ADA4-4053-BD20-BC87DAE4C0E9}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13042,7 +13044,7 @@
           <xm:sqref>D111:D112</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2D5424A5-7CE2-4970-B6F8-75E2746D2527}">
+          <x14:cfRule type="dataBar" id="{3989764E-F095-45A5-9BCB-84F63D668964}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13057,7 +13059,7 @@
           <xm:sqref>D134:D142</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{83E54036-476C-47BD-AE9E-F5EEA1EBF1BE}">
+          <x14:cfRule type="dataBar" id="{E62DF740-30B0-4D42-9B5A-95C7AE651613}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13072,7 +13074,7 @@
           <xm:sqref>D39:D44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6833D88B-CE58-423C-8F6F-C036FD28CF16}">
+          <x14:cfRule type="dataBar" id="{AAFEC3C4-2157-4C36-85E7-C9D1AB9F9487}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13087,7 +13089,7 @@
           <xm:sqref>D45:D50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4FCF14D3-6066-4337-9148-5CBDD9D97737}">
+          <x14:cfRule type="dataBar" id="{3CCAABB9-BE51-41BD-A38E-92B7CF006560}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13102,7 +13104,7 @@
           <xm:sqref>D51:D52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7A3BCBB7-6551-46C2-9611-26939F5FF02D}">
+          <x14:cfRule type="dataBar" id="{89E5A2E2-30D6-4530-BD85-9BCABEE52AE6}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13117,7 +13119,7 @@
           <xm:sqref>D53:D60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3AB2A3C6-E21A-4FE5-BC8B-9F25C96D2D71}">
+          <x14:cfRule type="dataBar" id="{54E28360-96EE-4590-AD67-FFC87BDFE86D}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13132,7 +13134,7 @@
           <xm:sqref>D65:D70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5B65866B-9A81-4DE0-89EA-F27365ADD456}">
+          <x14:cfRule type="dataBar" id="{654748D6-D2F5-47CC-A450-DEE05C92C7B6}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13147,7 +13149,7 @@
           <xm:sqref>D82:D83</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9020698F-D55A-4128-8170-9BE512E418AF}">
+          <x14:cfRule type="dataBar" id="{75B9AC4A-C313-4B66-8829-9DE39DBD11C4}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13162,7 +13164,7 @@
           <xm:sqref>D113:D116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DADC10BE-BCA9-4687-B044-3042E53415E2}">
+          <x14:cfRule type="dataBar" id="{7F217241-83E3-4299-B254-88D5B6E78389}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13177,7 +13179,7 @@
           <xm:sqref>D90:D95</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{454F8872-D0E9-4CAA-9249-5DE754BE2819}">
+          <x14:cfRule type="dataBar" id="{CF2D83F6-BA8E-47E3-BCE4-2EEB30E6E945}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13192,7 +13194,7 @@
           <xm:sqref>D102</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{62747F00-A1B9-4DA0-B723-705618A4FAB2}">
+          <x14:cfRule type="dataBar" id="{99A34868-2D4B-42C6-99C0-92E186CA3AF9}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13207,7 +13209,7 @@
           <xm:sqref>D96:D101</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8FEFC9BB-4E79-4E68-A8D8-53C013AF3350}">
+          <x14:cfRule type="dataBar" id="{BAEDA295-B5CE-4E25-81AA-72406049E5F8}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13222,7 +13224,7 @@
           <xm:sqref>D106:D110</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{505413A3-60D1-4214-BD7B-52B2403DCF93}">
+          <x14:cfRule type="dataBar" id="{E732D960-8A19-4AB8-B9A8-15D83ED7CA42}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13237,7 +13239,7 @@
           <xm:sqref>D126:D131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8FD0EDC0-845B-4011-ACD3-7262A339ED62}">
+          <x14:cfRule type="dataBar" id="{209E7AE6-538E-4339-B715-9360DB9DB810}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13252,7 +13254,7 @@
           <xm:sqref>D117:D123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F48C184A-78CE-4551-9E35-C9B767F56040}">
+          <x14:cfRule type="dataBar" id="{C1CF6C97-5AE0-42D0-BE41-2A3E23A88CA0}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -13267,7 +13269,7 @@
           <xm:sqref>D133</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{403CE37D-7779-452E-B2DD-5A7978777391}">
+          <x14:cfRule type="dataBar" id="{58B91061-78FB-461A-ACD3-951AB82639F7}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
changed My Requests layout
</commit_message>
<xml_diff>
--- a/Documentation/Obtayn-gantt-chart.xlsx
+++ b/Documentation/Obtayn-gantt-chart.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="200">
   <si>
     <t xml:space="preserve">Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -592,6 +592,9 @@
   </si>
   <si>
     <t xml:space="preserve">Create a back button which redirects Users to a list of chats.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hai</t>
   </si>
   <si>
     <t xml:space="preserve">Write function to handle “Network Error” exception.</t>
@@ -1719,9 +1722,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1901160</xdr:colOff>
+      <xdr:colOff>1900800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>520200</xdr:rowOff>
+      <xdr:rowOff>519840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1737,7 +1740,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="95400"/>
-          <a:ext cx="1901160" cy="424800"/>
+          <a:ext cx="1900800" cy="424440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1760,12 +1763,12 @@
   <dimension ref="A1:BL180"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="X164" activeCellId="0" sqref="X164"/>
+      <selection pane="bottomLeft" activeCell="D129" activeCellId="0" sqref="D129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="35.58"/>
@@ -5228,7 +5231,9 @@
         <v>61</v>
       </c>
       <c r="C44" s="65"/>
-      <c r="D44" s="66"/>
+      <c r="D44" s="66" t="n">
+        <v>1</v>
+      </c>
       <c r="E44" s="67" t="s">
         <v>62</v>
       </c>
@@ -11517,7 +11522,9 @@
         <v>49</v>
       </c>
       <c r="C128" s="76"/>
-      <c r="D128" s="36"/>
+      <c r="D128" s="36" t="n">
+        <v>1</v>
+      </c>
       <c r="E128" s="92" t="n">
         <f aca="false">DATE(2021,4,27)</f>
         <v>44313</v>
@@ -11591,7 +11598,9 @@
         <v>142</v>
       </c>
       <c r="C129" s="76"/>
-      <c r="D129" s="36"/>
+      <c r="D129" s="36" t="n">
+        <v>1</v>
+      </c>
       <c r="E129" s="92" t="n">
         <f aca="false">DATE(2021,4,27)</f>
         <v>44313</v>
@@ -14247,7 +14256,9 @@
       <c r="U164" s="26"/>
       <c r="V164" s="26"/>
       <c r="W164" s="26"/>
-      <c r="X164" s="26"/>
+      <c r="X164" s="26" t="s">
+        <v>175</v>
+      </c>
       <c r="Y164" s="26"/>
       <c r="Z164" s="26"/>
       <c r="AA164" s="26"/>
@@ -14292,7 +14303,7 @@
     <row r="165" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="1"/>
       <c r="B165" s="79" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C165" s="80"/>
       <c r="D165" s="48"/>
@@ -14366,7 +14377,7 @@
     <row r="166" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="1"/>
       <c r="B166" s="79" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C166" s="80"/>
       <c r="D166" s="48"/>
@@ -14440,7 +14451,7 @@
     <row r="167" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="1"/>
       <c r="B167" s="79" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C167" s="80"/>
       <c r="D167" s="48"/>
@@ -14514,7 +14525,7 @@
     <row r="168" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="1"/>
       <c r="B168" s="79" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C168" s="80"/>
       <c r="D168" s="48" t="n">
@@ -14590,7 +14601,7 @@
     <row r="169" s="33" customFormat="true" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="1"/>
       <c r="B169" s="79" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C169" s="80"/>
       <c r="D169" s="48"/>
@@ -14730,10 +14741,10 @@
     <row r="171" s="33" customFormat="true" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="1"/>
       <c r="B171" s="90" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C171" s="91" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D171" s="61"/>
       <c r="E171" s="62"/>
@@ -15064,7 +15075,7 @@
     <row r="176" s="33" customFormat="true" ht="54.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="1"/>
       <c r="B176" s="94" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C176" s="95"/>
       <c r="D176" s="96"/>
@@ -15131,7 +15142,7 @@
     </row>
     <row r="177" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B177" s="99"/>
       <c r="E177" s="3"/>
@@ -15230,7 +15241,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F4D24858-94C7-45FA-BB20-4177C8F49437}</x14:id>
+          <x14:id>{C080A050-F829-47B0-952B-2270E4E4ABED}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15257,7 +15268,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B6B56117-3AB2-4A64-AF5A-E0E814A8D290}</x14:id>
+          <x14:id>{EF786A24-7DA2-46C3-9071-A940585C6A9C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15271,7 +15282,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{506D65BC-E49F-448C-9679-C4E0E013B2F4}</x14:id>
+          <x14:id>{AEB056F3-608D-4768-8C7E-A4D75F602EE5}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15285,7 +15296,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3564F7B7-4C84-4112-9772-83E42EF97084}</x14:id>
+          <x14:id>{5F892128-009E-4649-B29D-9082F6ED9E73}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15299,7 +15310,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{39975D2D-64C6-4F76-B73E-22C3F62CB0D9}</x14:id>
+          <x14:id>{9F91BB67-A57C-4AD8-9CD8-D4EB903ACD4E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15313,7 +15324,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{58BFCA9C-3A1D-41E4-BA8F-6E1FCAC13AE0}</x14:id>
+          <x14:id>{40E98492-B0B0-42B4-868A-C578EC6C3BC0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15327,7 +15338,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C2A726C8-AEF7-4AFB-B43A-3FA6CD44DBE7}</x14:id>
+          <x14:id>{1B72A765-1F96-4064-B7CE-5D42C1BF4FE9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15341,7 +15352,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FC8EF268-874D-43E3-A437-678F85DEA9B6}</x14:id>
+          <x14:id>{E65F409D-4A64-42C9-BA60-5C801FEC4B5F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15355,7 +15366,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6BDAF12F-90C2-4A29-A53C-1690F0D09E8A}</x14:id>
+          <x14:id>{477F571A-D913-4B51-AC90-10C6961C95AA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15369,7 +15380,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9796F53C-E7DF-49E5-9552-8D56674D92A6}</x14:id>
+          <x14:id>{ED1E6BC1-CEB0-42F0-A2E7-59997F609DE1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15383,7 +15394,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8EB45483-683C-45A1-9A60-726BB054EF2F}</x14:id>
+          <x14:id>{266BEF85-50B0-4F4D-B9B5-FB6A97D47357}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15397,7 +15408,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3629FB3F-9C72-4EB2-B625-436F2EB88A8D}</x14:id>
+          <x14:id>{B6CEFD25-B337-4B98-AD60-E4CA77149B2F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15411,7 +15422,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{29289CDB-87C8-4848-906D-3C1477796DC2}</x14:id>
+          <x14:id>{4C99CC22-6E53-48FE-BE47-5690CE6722E1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15425,7 +15436,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C4CCD07B-A32C-49B1-8E5C-AC2EE9747C52}</x14:id>
+          <x14:id>{DE7738E3-722E-4AEC-8483-63D762D1ACED}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15439,7 +15450,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6330188B-593A-4A11-96BE-E6DDE28F7483}</x14:id>
+          <x14:id>{5B20BB4D-8E48-43A4-81C1-F6A1739A6D8A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15453,7 +15464,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{79B71F00-9A11-49C4-8EC8-E14090A131A6}</x14:id>
+          <x14:id>{32F056F3-8B26-4E8E-8930-577E8B916D88}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15467,7 +15478,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5F499CC8-2A71-42AB-B249-D389B1302847}</x14:id>
+          <x14:id>{F45A331E-CA85-46C8-BDA5-5FAF24D24274}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15481,7 +15492,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3ACED8AC-527A-419B-BAC1-631FA27B158A}</x14:id>
+          <x14:id>{50E0D46D-765B-4300-939D-31DD9061717F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15495,7 +15506,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{304BB86E-E15C-44A1-BC8F-93826EEE9BEF}</x14:id>
+          <x14:id>{C7C54C10-60E9-46B4-B0BB-165133AD3799}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15509,7 +15520,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7D2C9EEF-CBFB-4510-806C-195741916D00}</x14:id>
+          <x14:id>{F067EF1C-8E12-46BE-B371-B3B6B683C311}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15523,7 +15534,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7069EE30-CDEF-4866-B1F1-6B3E7CBBF772}</x14:id>
+          <x14:id>{B0A4E8CB-E0A6-4D25-B2BB-1851AEABC545}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15545,7 +15556,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F4D24858-94C7-45FA-BB20-4177C8F49437}">
+          <x14:cfRule type="dataBar" id="{C080A050-F829-47B0-952B-2270E4E4ABED}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15560,7 +15571,7 @@
           <xm:sqref>D7:D44 D71:D81 D88:D91 D98 D101:D107 D125:D129 D146:D149</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B6B56117-3AB2-4A64-AF5A-E0E814A8D290}">
+          <x14:cfRule type="dataBar" id="{EF786A24-7DA2-46C3-9071-A940585C6A9C}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15575,7 +15586,7 @@
           <xm:sqref>D92:D97</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{506D65BC-E49F-448C-9679-C4E0E013B2F4}">
+          <x14:cfRule type="dataBar" id="{AEB056F3-608D-4768-8C7E-A4D75F602EE5}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15590,7 +15601,7 @@
           <xm:sqref>D135:D136</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3564F7B7-4C84-4112-9772-83E42EF97084}">
+          <x14:cfRule type="dataBar" id="{5F892128-009E-4649-B29D-9082F6ED9E73}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15605,7 +15616,7 @@
           <xm:sqref>D158:D170</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{39975D2D-64C6-4F76-B73E-22C3F62CB0D9}">
+          <x14:cfRule type="dataBar" id="{9F91BB67-A57C-4AD8-9CD8-D4EB903ACD4E}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15620,7 +15631,7 @@
           <xm:sqref>D45:D52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{58BFCA9C-3A1D-41E4-BA8F-6E1FCAC13AE0}">
+          <x14:cfRule type="dataBar" id="{40E98492-B0B0-42B4-868A-C578EC6C3BC0}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15635,7 +15646,7 @@
           <xm:sqref>D53:D59</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C2A726C8-AEF7-4AFB-B43A-3FA6CD44DBE7}">
+          <x14:cfRule type="dataBar" id="{1B72A765-1F96-4064-B7CE-5D42C1BF4FE9}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15650,7 +15661,7 @@
           <xm:sqref>D60:D62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FC8EF268-874D-43E3-A437-678F85DEA9B6}">
+          <x14:cfRule type="dataBar" id="{E65F409D-4A64-42C9-BA60-5C801FEC4B5F}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15665,7 +15676,7 @@
           <xm:sqref>D63:D70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6BDAF12F-90C2-4A29-A53C-1690F0D09E8A}">
+          <x14:cfRule type="dataBar" id="{477F571A-D913-4B51-AC90-10C6961C95AA}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15680,7 +15691,7 @@
           <xm:sqref>D82:D87</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9796F53C-E7DF-49E5-9552-8D56674D92A6}">
+          <x14:cfRule type="dataBar" id="{ED1E6BC1-CEB0-42F0-A2E7-59997F609DE1}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15695,7 +15706,7 @@
           <xm:sqref>D99:D100</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8EB45483-683C-45A1-9A60-726BB054EF2F}">
+          <x14:cfRule type="dataBar" id="{266BEF85-50B0-4F4D-B9B5-FB6A97D47357}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15710,7 +15721,7 @@
           <xm:sqref>D137:D138</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3629FB3F-9C72-4EB2-B625-436F2EB88A8D}">
+          <x14:cfRule type="dataBar" id="{B6CEFD25-B337-4B98-AD60-E4CA77149B2F}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15725,7 +15736,7 @@
           <xm:sqref>D108:D117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{29289CDB-87C8-4848-906D-3C1477796DC2}">
+          <x14:cfRule type="dataBar" id="{4C99CC22-6E53-48FE-BE47-5690CE6722E1}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15740,7 +15751,7 @@
           <xm:sqref>D124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C4CCD07B-A32C-49B1-8E5C-AC2EE9747C52}">
+          <x14:cfRule type="dataBar" id="{DE7738E3-722E-4AEC-8483-63D762D1ACED}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15755,7 +15766,7 @@
           <xm:sqref>D118:D123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6330188B-593A-4A11-96BE-E6DDE28F7483}">
+          <x14:cfRule type="dataBar" id="{5B20BB4D-8E48-43A4-81C1-F6A1739A6D8A}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15770,7 +15781,7 @@
           <xm:sqref>D130:D134</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{79B71F00-9A11-49C4-8EC8-E14090A131A6}">
+          <x14:cfRule type="dataBar" id="{32F056F3-8B26-4E8E-8930-577E8B916D88}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15785,7 +15796,7 @@
           <xm:sqref>D150:D155</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5F499CC8-2A71-42AB-B249-D389B1302847}">
+          <x14:cfRule type="dataBar" id="{F45A331E-CA85-46C8-BDA5-5FAF24D24274}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15800,7 +15811,7 @@
           <xm:sqref>D139:D145</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3ACED8AC-527A-419B-BAC1-631FA27B158A}">
+          <x14:cfRule type="dataBar" id="{50E0D46D-765B-4300-939D-31DD9061717F}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15815,7 +15826,7 @@
           <xm:sqref>D157</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{304BB86E-E15C-44A1-BC8F-93826EEE9BEF}">
+          <x14:cfRule type="dataBar" id="{C7C54C10-60E9-46B4-B0BB-165133AD3799}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15830,7 +15841,7 @@
           <xm:sqref>D156</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7D2C9EEF-CBFB-4510-806C-195741916D00}">
+          <x14:cfRule type="dataBar" id="{F067EF1C-8E12-46BE-B371-B3B6B683C311}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15845,7 +15856,7 @@
           <xm:sqref>D176</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7069EE30-CDEF-4866-B1F1-6B3E7CBBF772}">
+          <x14:cfRule type="dataBar" id="{B0A4E8CB-E0A6-4D25-B2BB-1851AEABC545}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15876,7 +15887,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="105" width="87.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="7" width="9.13"/>
@@ -15885,79 +15896,79 @@
     <row r="1" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" s="107" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="106" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B2" s="106"/>
     </row>
     <row r="3" s="109" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="108" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B3" s="108"/>
     </row>
     <row r="4" s="111" customFormat="true" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="110" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="74.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="112" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="110" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" s="105" customFormat="true" ht="204.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="113" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" s="111" customFormat="true" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="110" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="112" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" s="105" customFormat="true" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="114" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" s="111" customFormat="true" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="110" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="112" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" s="105" customFormat="true" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="114" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" s="111" customFormat="true" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="110" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="112" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="112" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Dismiss All button
</commit_message>
<xml_diff>
--- a/Documentation/Obtayn-gantt-chart.xlsx
+++ b/Documentation/Obtayn-gantt-chart.xlsx
@@ -1722,9 +1722,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1900800</xdr:colOff>
+      <xdr:colOff>1900440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>519840</xdr:rowOff>
+      <xdr:rowOff>519480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1740,7 +1740,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="95400"/>
-          <a:ext cx="1900800" cy="424440"/>
+          <a:ext cx="1900440" cy="424080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1763,12 +1763,12 @@
   <dimension ref="A1:BL180"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D129" activeCellId="0" sqref="D129"/>
+      <selection pane="bottomLeft" activeCell="D116" activeCellId="0" sqref="D116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="35.58"/>
@@ -5758,7 +5758,9 @@
         <v>70</v>
       </c>
       <c r="C51" s="35"/>
-      <c r="D51" s="36"/>
+      <c r="D51" s="36" t="n">
+        <v>1</v>
+      </c>
       <c r="E51" s="69" t="n">
         <f aca="false">DATE(2021,4,29)</f>
         <v>44315</v>
@@ -5832,7 +5834,9 @@
         <v>71</v>
       </c>
       <c r="C52" s="35"/>
-      <c r="D52" s="36"/>
+      <c r="D52" s="36" t="n">
+        <v>1</v>
+      </c>
       <c r="E52" s="69" t="n">
         <f aca="false">DATE(2021,4,26)</f>
         <v>44312</v>
@@ -10620,7 +10624,9 @@
         <v>132</v>
       </c>
       <c r="C116" s="72"/>
-      <c r="D116" s="66"/>
+      <c r="D116" s="66" t="n">
+        <v>1</v>
+      </c>
       <c r="E116" s="67" t="n">
         <f aca="false">DATE(2021,4,27)</f>
         <v>44313</v>
@@ -15241,7 +15247,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C080A050-F829-47B0-952B-2270E4E4ABED}</x14:id>
+          <x14:id>{6F4E1070-46A0-434B-9442-E0F7779B1E2C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15268,7 +15274,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{EF786A24-7DA2-46C3-9071-A940585C6A9C}</x14:id>
+          <x14:id>{B5182A24-F1E4-441E-8F3B-BEFADF855772}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15282,7 +15288,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{AEB056F3-608D-4768-8C7E-A4D75F602EE5}</x14:id>
+          <x14:id>{CAC4D5B2-BD12-45AF-977E-5E8059CC2280}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15296,7 +15302,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5F892128-009E-4649-B29D-9082F6ED9E73}</x14:id>
+          <x14:id>{AE208D84-3557-4BCA-9C17-F4D83B61BA4E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15310,7 +15316,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9F91BB67-A57C-4AD8-9CD8-D4EB903ACD4E}</x14:id>
+          <x14:id>{44DD904D-9E38-486D-B8EC-C19B70F2EE17}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15324,7 +15330,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{40E98492-B0B0-42B4-868A-C578EC6C3BC0}</x14:id>
+          <x14:id>{674E5E4D-94CF-4742-9CF1-E116E416D71F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15338,7 +15344,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1B72A765-1F96-4064-B7CE-5D42C1BF4FE9}</x14:id>
+          <x14:id>{5EF02217-6B93-4AA0-98AC-98DDA9E4BC82}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15352,7 +15358,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E65F409D-4A64-42C9-BA60-5C801FEC4B5F}</x14:id>
+          <x14:id>{7DBB1733-0074-4356-9480-1DB041706A7B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15366,7 +15372,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{477F571A-D913-4B51-AC90-10C6961C95AA}</x14:id>
+          <x14:id>{8BD0F448-3835-4C55-AAB8-2D8F5A63B17E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15380,7 +15386,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ED1E6BC1-CEB0-42F0-A2E7-59997F609DE1}</x14:id>
+          <x14:id>{1CCC7EA1-F02D-4AD1-A5A0-F879CC8BB773}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15394,7 +15400,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{266BEF85-50B0-4F4D-B9B5-FB6A97D47357}</x14:id>
+          <x14:id>{B940D933-51CA-403B-82C3-95F8B36A2250}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15408,7 +15414,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B6CEFD25-B337-4B98-AD60-E4CA77149B2F}</x14:id>
+          <x14:id>{7D30D387-48FC-4DCF-8B31-607AD1C67090}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15422,7 +15428,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4C99CC22-6E53-48FE-BE47-5690CE6722E1}</x14:id>
+          <x14:id>{E2FA16F7-375B-4615-9CE9-963F59D9C0CF}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15436,7 +15442,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{DE7738E3-722E-4AEC-8483-63D762D1ACED}</x14:id>
+          <x14:id>{AE6E8BE9-5ACC-40AC-B73A-D7A98C6C47C0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15450,7 +15456,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5B20BB4D-8E48-43A4-81C1-F6A1739A6D8A}</x14:id>
+          <x14:id>{F5CEBBA7-D4A3-4A78-B3F2-8391456640C0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15464,7 +15470,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{32F056F3-8B26-4E8E-8930-577E8B916D88}</x14:id>
+          <x14:id>{E042E570-7B1E-41A2-93D6-DD2A3039AB68}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15478,7 +15484,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F45A331E-CA85-46C8-BDA5-5FAF24D24274}</x14:id>
+          <x14:id>{47CB6FC0-B263-47BD-A711-25BFD1A477E9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15492,7 +15498,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{50E0D46D-765B-4300-939D-31DD9061717F}</x14:id>
+          <x14:id>{2BF0D138-C833-48A3-A2BC-40EF12F079F2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15506,7 +15512,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C7C54C10-60E9-46B4-B0BB-165133AD3799}</x14:id>
+          <x14:id>{8FE0C4D0-5BCA-41E8-8886-1A6486489075}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15520,7 +15526,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F067EF1C-8E12-46BE-B371-B3B6B683C311}</x14:id>
+          <x14:id>{77D63316-20D2-4C21-8CFF-B72B6EAF1690}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15534,7 +15540,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B0A4E8CB-E0A6-4D25-B2BB-1851AEABC545}</x14:id>
+          <x14:id>{8197C44A-E0BC-426B-85CA-D0F4EC7D8070}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15556,7 +15562,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C080A050-F829-47B0-952B-2270E4E4ABED}">
+          <x14:cfRule type="dataBar" id="{6F4E1070-46A0-434B-9442-E0F7779B1E2C}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15571,7 +15577,7 @@
           <xm:sqref>D7:D44 D71:D81 D88:D91 D98 D101:D107 D125:D129 D146:D149</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{EF786A24-7DA2-46C3-9071-A940585C6A9C}">
+          <x14:cfRule type="dataBar" id="{B5182A24-F1E4-441E-8F3B-BEFADF855772}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15586,7 +15592,7 @@
           <xm:sqref>D92:D97</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{AEB056F3-608D-4768-8C7E-A4D75F602EE5}">
+          <x14:cfRule type="dataBar" id="{CAC4D5B2-BD12-45AF-977E-5E8059CC2280}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15601,7 +15607,7 @@
           <xm:sqref>D135:D136</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5F892128-009E-4649-B29D-9082F6ED9E73}">
+          <x14:cfRule type="dataBar" id="{AE208D84-3557-4BCA-9C17-F4D83B61BA4E}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15616,7 +15622,7 @@
           <xm:sqref>D158:D170</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9F91BB67-A57C-4AD8-9CD8-D4EB903ACD4E}">
+          <x14:cfRule type="dataBar" id="{44DD904D-9E38-486D-B8EC-C19B70F2EE17}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15631,7 +15637,7 @@
           <xm:sqref>D45:D52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{40E98492-B0B0-42B4-868A-C578EC6C3BC0}">
+          <x14:cfRule type="dataBar" id="{674E5E4D-94CF-4742-9CF1-E116E416D71F}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15646,7 +15652,7 @@
           <xm:sqref>D53:D59</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1B72A765-1F96-4064-B7CE-5D42C1BF4FE9}">
+          <x14:cfRule type="dataBar" id="{5EF02217-6B93-4AA0-98AC-98DDA9E4BC82}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15661,7 +15667,7 @@
           <xm:sqref>D60:D62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E65F409D-4A64-42C9-BA60-5C801FEC4B5F}">
+          <x14:cfRule type="dataBar" id="{7DBB1733-0074-4356-9480-1DB041706A7B}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15676,7 +15682,7 @@
           <xm:sqref>D63:D70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{477F571A-D913-4B51-AC90-10C6961C95AA}">
+          <x14:cfRule type="dataBar" id="{8BD0F448-3835-4C55-AAB8-2D8F5A63B17E}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15691,7 +15697,7 @@
           <xm:sqref>D82:D87</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ED1E6BC1-CEB0-42F0-A2E7-59997F609DE1}">
+          <x14:cfRule type="dataBar" id="{1CCC7EA1-F02D-4AD1-A5A0-F879CC8BB773}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15706,7 +15712,7 @@
           <xm:sqref>D99:D100</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{266BEF85-50B0-4F4D-B9B5-FB6A97D47357}">
+          <x14:cfRule type="dataBar" id="{B940D933-51CA-403B-82C3-95F8B36A2250}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15721,7 +15727,7 @@
           <xm:sqref>D137:D138</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B6CEFD25-B337-4B98-AD60-E4CA77149B2F}">
+          <x14:cfRule type="dataBar" id="{7D30D387-48FC-4DCF-8B31-607AD1C67090}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15736,7 +15742,7 @@
           <xm:sqref>D108:D117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4C99CC22-6E53-48FE-BE47-5690CE6722E1}">
+          <x14:cfRule type="dataBar" id="{E2FA16F7-375B-4615-9CE9-963F59D9C0CF}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15751,7 +15757,7 @@
           <xm:sqref>D124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DE7738E3-722E-4AEC-8483-63D762D1ACED}">
+          <x14:cfRule type="dataBar" id="{AE6E8BE9-5ACC-40AC-B73A-D7A98C6C47C0}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15766,7 +15772,7 @@
           <xm:sqref>D118:D123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5B20BB4D-8E48-43A4-81C1-F6A1739A6D8A}">
+          <x14:cfRule type="dataBar" id="{F5CEBBA7-D4A3-4A78-B3F2-8391456640C0}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15781,7 +15787,7 @@
           <xm:sqref>D130:D134</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{32F056F3-8B26-4E8E-8930-577E8B916D88}">
+          <x14:cfRule type="dataBar" id="{E042E570-7B1E-41A2-93D6-DD2A3039AB68}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15796,7 +15802,7 @@
           <xm:sqref>D150:D155</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F45A331E-CA85-46C8-BDA5-5FAF24D24274}">
+          <x14:cfRule type="dataBar" id="{47CB6FC0-B263-47BD-A711-25BFD1A477E9}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15811,7 +15817,7 @@
           <xm:sqref>D139:D145</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{50E0D46D-765B-4300-939D-31DD9061717F}">
+          <x14:cfRule type="dataBar" id="{2BF0D138-C833-48A3-A2BC-40EF12F079F2}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15826,7 +15832,7 @@
           <xm:sqref>D157</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C7C54C10-60E9-46B4-B0BB-165133AD3799}">
+          <x14:cfRule type="dataBar" id="{8FE0C4D0-5BCA-41E8-8886-1A6486489075}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15841,7 +15847,7 @@
           <xm:sqref>D156</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F067EF1C-8E12-46BE-B371-B3B6B683C311}">
+          <x14:cfRule type="dataBar" id="{77D63316-20D2-4C21-8CFF-B72B6EAF1690}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15856,7 +15862,7 @@
           <xm:sqref>D176</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B0A4E8CB-E0A6-4D25-B2BB-1851AEABC545}">
+          <x14:cfRule type="dataBar" id="{8197C44A-E0BC-426B-85CA-D0F4EC7D8070}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
made navbar responsive, fixed Post issue
</commit_message>
<xml_diff>
--- a/Documentation/Obtayn-gantt-chart.xlsx
+++ b/Documentation/Obtayn-gantt-chart.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="199">
   <si>
     <t xml:space="preserve">Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -270,9 +270,6 @@
     <t xml:space="preserve">Write a function to show relevant requests as search results.</t>
   </si>
   <si>
-    <t xml:space="preserve">Write a function to handle “Network Error” exception.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Write a function to handle “No match found” exception.</t>
   </si>
   <si>
@@ -353,9 +350,6 @@
     <t xml:space="preserve">Add Search bar in Feed</t>
   </si>
   <si>
-    <t xml:space="preserve">Show action button on hover of Post</t>
-  </si>
-  <si>
     <t xml:space="preserve">Change Accept Request icon</t>
   </si>
   <si>
@@ -389,6 +383,9 @@
     <t xml:space="preserve">Write a function to show the new Request on top of the Feed.</t>
   </si>
   <si>
+    <t xml:space="preserve">Write a function to handle “Network Error” exception.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Write a function to close the Create Post modal when the “Add Request” button is clicked.</t>
   </si>
   <si>
@@ -468,6 +465,9 @@
   </si>
   <si>
     <t xml:space="preserve">Show Notifications from My Requests page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide “Dismiss All” button when notifications are empty.</t>
   </si>
   <si>
     <t xml:space="preserve">Write new Post</t>
@@ -592,9 +592,6 @@
   </si>
   <si>
     <t xml:space="preserve">Create a back button which redirects Users to a list of chats.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hai</t>
   </si>
   <si>
     <t xml:space="preserve">Write function to handle “Network Error” exception.</t>
@@ -1722,9 +1719,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1900440</xdr:colOff>
+      <xdr:colOff>1900080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>519480</xdr:rowOff>
+      <xdr:rowOff>519120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1740,7 +1737,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="95400"/>
-          <a:ext cx="1900440" cy="424080"/>
+          <a:ext cx="1900080" cy="423720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1760,15 +1757,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:BL180"/>
+  <dimension ref="A1:BL1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D116" activeCellId="0" sqref="D116"/>
+      <selection pane="bottomLeft" activeCell="B78" activeCellId="0" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="35.58"/>
@@ -5608,14 +5605,16 @@
         <v>68</v>
       </c>
       <c r="C49" s="35"/>
-      <c r="D49" s="36"/>
+      <c r="D49" s="36" t="n">
+        <v>1</v>
+      </c>
       <c r="E49" s="37" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
+        <f aca="false">DATE(2021,4,22)</f>
+        <v>44308</v>
       </c>
       <c r="F49" s="37" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
+        <f aca="false">DATE(2021,4,22)</f>
+        <v>44308</v>
       </c>
       <c r="G49" s="32"/>
       <c r="H49" s="32"/>
@@ -5685,13 +5684,13 @@
       <c r="D50" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="E50" s="37" t="n">
-        <f aca="false">DATE(2021,4,22)</f>
-        <v>44308</v>
-      </c>
-      <c r="F50" s="37" t="n">
-        <f aca="false">DATE(2021,4,22)</f>
-        <v>44308</v>
+      <c r="E50" s="69" t="n">
+        <f aca="false">DATE(2021,4,29)</f>
+        <v>44315</v>
+      </c>
+      <c r="F50" s="69" t="n">
+        <f aca="false">DATE(2021,4,29)</f>
+        <v>44315</v>
       </c>
       <c r="G50" s="32"/>
       <c r="H50" s="32"/>
@@ -5762,12 +5761,12 @@
         <v>1</v>
       </c>
       <c r="E51" s="69" t="n">
-        <f aca="false">DATE(2021,4,29)</f>
-        <v>44315</v>
+        <f aca="false">DATE(2021,4,26)</f>
+        <v>44312</v>
       </c>
       <c r="F51" s="69" t="n">
-        <f aca="false">DATE(2021,4,29)</f>
-        <v>44315</v>
+        <f aca="false">DATE(2021,4,26)</f>
+        <v>44312</v>
       </c>
       <c r="G51" s="32"/>
       <c r="H51" s="32"/>
@@ -5830,21 +5829,15 @@
     </row>
     <row r="52" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="35"/>
-      <c r="D52" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" s="69" t="n">
-        <f aca="false">DATE(2021,4,26)</f>
-        <v>44312</v>
-      </c>
-      <c r="F52" s="69" t="n">
-        <f aca="false">DATE(2021,4,26)</f>
-        <v>44312</v>
-      </c>
+      <c r="C52" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="43"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="45"/>
       <c r="G52" s="32"/>
       <c r="H52" s="32"/>
       <c r="I52" s="26"/>
@@ -5906,15 +5899,21 @@
     </row>
     <row r="53" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1"/>
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C53" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="D53" s="43"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="45"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="49" t="n">
+        <f aca="false">DATE(2021,4,7)</f>
+        <v>44293</v>
+      </c>
+      <c r="F53" s="49" t="n">
+        <f aca="false">DATE(2021,4,7)</f>
+        <v>44293</v>
+      </c>
       <c r="G53" s="32"/>
       <c r="H53" s="32"/>
       <c r="I53" s="26"/>
@@ -5984,12 +5983,12 @@
         <v>1</v>
       </c>
       <c r="E54" s="49" t="n">
-        <f aca="false">DATE(2021,4,7)</f>
-        <v>44293</v>
+        <f aca="false">DATE(2021,4,8)</f>
+        <v>44294</v>
       </c>
       <c r="F54" s="49" t="n">
-        <f aca="false">DATE(2021,4,7)</f>
-        <v>44293</v>
+        <f aca="false">DATE(2021,4,8)</f>
+        <v>44294</v>
       </c>
       <c r="G54" s="32"/>
       <c r="H54" s="32"/>
@@ -6212,12 +6211,12 @@
         <v>1</v>
       </c>
       <c r="E57" s="49" t="n">
-        <f aca="false">DATE(2021,4,8)</f>
-        <v>44294</v>
+        <f aca="false">DATE(2021,4,7)</f>
+        <v>44293</v>
       </c>
       <c r="F57" s="49" t="n">
-        <f aca="false">DATE(2021,4,8)</f>
-        <v>44294</v>
+        <f aca="false">DATE(2021,4,7)</f>
+        <v>44293</v>
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="32"/>
@@ -6288,12 +6287,12 @@
         <v>1</v>
       </c>
       <c r="E58" s="49" t="n">
-        <f aca="false">DATE(2021,4,7)</f>
-        <v>44293</v>
+        <f aca="false">DATE(2021,4,30)</f>
+        <v>44316</v>
       </c>
       <c r="F58" s="49" t="n">
-        <f aca="false">DATE(2021,4,7)</f>
-        <v>44293</v>
+        <f aca="false">DATE(2021,4,30)</f>
+        <v>44316</v>
       </c>
       <c r="G58" s="32"/>
       <c r="H58" s="32"/>
@@ -6356,19 +6355,15 @@
     </row>
     <row r="59" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1"/>
-      <c r="B59" s="46" t="s">
+      <c r="B59" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="47"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="49" t="n">
-        <f aca="false">DATE(2021,4,30)</f>
-        <v>44316</v>
-      </c>
-      <c r="F59" s="49" t="n">
-        <f aca="false">DATE(2021,4,30)</f>
-        <v>44316</v>
-      </c>
+      <c r="C59" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D59" s="52"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="54"/>
       <c r="G59" s="32"/>
       <c r="H59" s="32"/>
       <c r="I59" s="26"/>
@@ -6428,17 +6423,23 @@
       <c r="BK59" s="26"/>
       <c r="BL59" s="26"/>
     </row>
-    <row r="60" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" s="33" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1"/>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="C60" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="D60" s="52"/>
-      <c r="E60" s="53"/>
-      <c r="F60" s="54"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="58" t="n">
+        <f aca="false">DATE(2021,4,8)</f>
+        <v>44294</v>
+      </c>
+      <c r="F60" s="58" t="n">
+        <f aca="false">DATE(2021,4,8)</f>
+        <v>44294</v>
+      </c>
       <c r="G60" s="32"/>
       <c r="H60" s="32"/>
       <c r="I60" s="26"/>
@@ -6498,23 +6499,13 @@
       <c r="BK60" s="26"/>
       <c r="BL60" s="26"/>
     </row>
-    <row r="61" s="33" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" s="33" customFormat="true" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1"/>
-      <c r="B61" s="70" t="s">
-        <v>80</v>
-      </c>
+      <c r="B61" s="70"/>
       <c r="C61" s="56"/>
-      <c r="D61" s="57" t="n">
-        <v>1</v>
-      </c>
-      <c r="E61" s="58" t="n">
-        <f aca="false">DATE(2021,4,8)</f>
-        <v>44294</v>
-      </c>
-      <c r="F61" s="58" t="n">
-        <f aca="false">DATE(2021,4,8)</f>
-        <v>44294</v>
-      </c>
+      <c r="D61" s="57"/>
+      <c r="E61" s="58"/>
+      <c r="F61" s="58"/>
       <c r="G61" s="32"/>
       <c r="H61" s="32"/>
       <c r="I61" s="26"/>
@@ -6574,13 +6565,17 @@
       <c r="BK61" s="26"/>
       <c r="BL61" s="26"/>
     </row>
-    <row r="62" s="33" customFormat="true" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1"/>
-      <c r="B62" s="70"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="58"/>
-      <c r="F62" s="58"/>
+      <c r="B62" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="D62" s="61"/>
+      <c r="E62" s="62"/>
+      <c r="F62" s="63"/>
       <c r="G62" s="32"/>
       <c r="H62" s="32"/>
       <c r="I62" s="26"/>
@@ -6642,15 +6637,21 @@
     </row>
     <row r="63" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1"/>
-      <c r="B63" s="59" t="s">
+      <c r="B63" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="C63" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="D63" s="61"/>
-      <c r="E63" s="62"/>
-      <c r="F63" s="63"/>
+      <c r="C63" s="65"/>
+      <c r="D63" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" s="67" t="n">
+        <f aca="false">DATE(2021,4,9)</f>
+        <v>44295</v>
+      </c>
+      <c r="F63" s="67" t="n">
+        <f aca="false">DATE(2021,4,9)</f>
+        <v>44295</v>
+      </c>
       <c r="G63" s="32"/>
       <c r="H63" s="32"/>
       <c r="I63" s="26"/>
@@ -6796,12 +6797,12 @@
         <v>1</v>
       </c>
       <c r="E65" s="67" t="n">
-        <f aca="false">DATE(2021,4,9)</f>
-        <v>44295</v>
+        <f aca="false">DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="F65" s="67" t="n">
-        <f aca="false">DATE(2021,4,9)</f>
-        <v>44295</v>
+        <f aca="false">DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="G65" s="32"/>
       <c r="H65" s="32"/>
@@ -6864,20 +6865,20 @@
     </row>
     <row r="66" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1"/>
-      <c r="B66" s="64" t="s">
+      <c r="B66" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="C66" s="65"/>
+      <c r="C66" s="72"/>
       <c r="D66" s="66" t="n">
         <v>1</v>
       </c>
       <c r="E66" s="67" t="n">
-        <f aca="false">DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f aca="false">DATE(2021,4,9)</f>
+        <v>44295</v>
       </c>
       <c r="F66" s="67" t="n">
-        <f aca="false">DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f aca="false">DATE(2021,4,9)</f>
+        <v>44295</v>
       </c>
       <c r="G66" s="32"/>
       <c r="H66" s="32"/>
@@ -6948,12 +6949,12 @@
         <v>1</v>
       </c>
       <c r="E67" s="67" t="n">
-        <f aca="false">DATE(2021,4,9)</f>
-        <v>44295</v>
+        <f aca="false">DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="F67" s="67" t="n">
-        <f aca="false">DATE(2021,4,9)</f>
-        <v>44295</v>
+        <f aca="false">DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="G67" s="32"/>
       <c r="H67" s="32"/>
@@ -7090,7 +7091,7 @@
       <c r="BK68" s="26"/>
       <c r="BL68" s="26"/>
     </row>
-    <row r="69" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" s="33" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1"/>
       <c r="B69" s="71" t="s">
         <v>87</v>
@@ -7166,7 +7167,7 @@
       <c r="BK69" s="26"/>
       <c r="BL69" s="26"/>
     </row>
-    <row r="70" s="33" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" s="33" customFormat="true" ht="41.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1"/>
       <c r="B70" s="71" t="s">
         <v>88</v>
@@ -7242,7 +7243,7 @@
       <c r="BK70" s="26"/>
       <c r="BL70" s="26"/>
     </row>
-    <row r="71" s="33" customFormat="true" ht="41.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" s="33" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1"/>
       <c r="B71" s="71" t="s">
         <v>89</v>
@@ -7318,7 +7319,7 @@
       <c r="BK71" s="26"/>
       <c r="BL71" s="26"/>
     </row>
-    <row r="72" s="33" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" s="33" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1"/>
       <c r="B72" s="71" t="s">
         <v>90</v>
@@ -7394,7 +7395,7 @@
       <c r="BK72" s="26"/>
       <c r="BL72" s="26"/>
     </row>
-    <row r="73" s="33" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" s="33" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1"/>
       <c r="B73" s="71" t="s">
         <v>91</v>
@@ -7480,12 +7481,12 @@
         <v>1</v>
       </c>
       <c r="E74" s="67" t="n">
-        <f aca="false">DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f aca="false">DATE(2021,4,26)</f>
+        <v>44312</v>
       </c>
       <c r="F74" s="67" t="n">
-        <f aca="false">DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f aca="false">DATE(2021,4,26)</f>
+        <v>44312</v>
       </c>
       <c r="G74" s="32"/>
       <c r="H74" s="32"/>
@@ -7556,12 +7557,12 @@
         <v>1</v>
       </c>
       <c r="E75" s="67" t="n">
-        <f aca="false">DATE(2021,4,26)</f>
-        <v>44312</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="F75" s="67" t="n">
-        <f aca="false">DATE(2021,4,26)</f>
-        <v>44312</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="G75" s="32"/>
       <c r="H75" s="32"/>
@@ -7632,12 +7633,12 @@
         <v>1</v>
       </c>
       <c r="E76" s="67" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
+        <f aca="false">DATE(2021,4,26)</f>
+        <v>44312</v>
       </c>
       <c r="F76" s="67" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
+        <f aca="false">DATE(2021,4,27)</f>
+        <v>44313</v>
       </c>
       <c r="G76" s="32"/>
       <c r="H76" s="32"/>
@@ -7706,12 +7707,12 @@
       <c r="C77" s="72"/>
       <c r="D77" s="66"/>
       <c r="E77" s="67" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
+        <f aca="false">DATE(2021,4,30)</f>
+        <v>44316</v>
       </c>
       <c r="F77" s="67" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
+        <f aca="false">DATE(2021,4,30)</f>
+        <v>44316</v>
       </c>
       <c r="G77" s="32"/>
       <c r="H77" s="32"/>
@@ -7778,14 +7779,16 @@
         <v>96</v>
       </c>
       <c r="C78" s="72"/>
-      <c r="D78" s="66"/>
+      <c r="D78" s="66" t="n">
+        <v>1</v>
+      </c>
       <c r="E78" s="67" t="n">
-        <f aca="false">DATE(2021,4,26)</f>
-        <v>44312</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="F78" s="67" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="G78" s="32"/>
       <c r="H78" s="32"/>
@@ -7848,19 +7851,11 @@
     </row>
     <row r="79" s="33" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1"/>
-      <c r="B79" s="71" t="s">
-        <v>97</v>
-      </c>
+      <c r="B79" s="71"/>
       <c r="C79" s="72"/>
       <c r="D79" s="66"/>
-      <c r="E79" s="67" t="n">
-        <f aca="false">DATE(2021,4,28)</f>
-        <v>44314</v>
-      </c>
-      <c r="F79" s="67" t="n">
-        <f aca="false">DATE(2021,4,28)</f>
-        <v>44314</v>
-      </c>
+      <c r="E79" s="67"/>
+      <c r="F79" s="67"/>
       <c r="G79" s="32"/>
       <c r="H79" s="32"/>
       <c r="I79" s="26"/>
@@ -7920,23 +7915,17 @@
       <c r="BK79" s="26"/>
       <c r="BL79" s="26"/>
     </row>
-    <row r="80" s="33" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1"/>
-      <c r="B80" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="C80" s="72"/>
-      <c r="D80" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="E80" s="67" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
-      </c>
-      <c r="F80" s="67" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
-      </c>
+      <c r="B80" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="D80" s="29"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="31"/>
       <c r="G80" s="32"/>
       <c r="H80" s="32"/>
       <c r="I80" s="26"/>
@@ -7996,13 +7985,23 @@
       <c r="BK80" s="26"/>
       <c r="BL80" s="26"/>
     </row>
-    <row r="81" s="33" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1"/>
-      <c r="B81" s="71"/>
-      <c r="C81" s="72"/>
-      <c r="D81" s="66"/>
-      <c r="E81" s="67"/>
-      <c r="F81" s="67"/>
+      <c r="B81" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="C81" s="76"/>
+      <c r="D81" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E81" s="37" t="n">
+        <f aca="false">DATE(2021,4,7)</f>
+        <v>44293</v>
+      </c>
+      <c r="F81" s="37" t="n">
+        <f aca="false">DATE(2021,4,7)</f>
+        <v>44293</v>
+      </c>
       <c r="G81" s="32"/>
       <c r="H81" s="32"/>
       <c r="I81" s="26"/>
@@ -8062,17 +8061,23 @@
       <c r="BK81" s="26"/>
       <c r="BL81" s="26"/>
     </row>
-    <row r="82" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" s="33" customFormat="true" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1"/>
-      <c r="B82" s="73" t="s">
+      <c r="B82" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="C82" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="D82" s="29"/>
-      <c r="E82" s="30"/>
-      <c r="F82" s="31"/>
+      <c r="C82" s="76"/>
+      <c r="D82" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E82" s="37" t="n">
+        <f aca="false">DATE(2021,4,7)</f>
+        <v>44293</v>
+      </c>
+      <c r="F82" s="37" t="n">
+        <f aca="false">DATE(2021,4,7)</f>
+        <v>44293</v>
+      </c>
       <c r="G82" s="32"/>
       <c r="H82" s="32"/>
       <c r="I82" s="26"/>
@@ -8132,7 +8137,7 @@
       <c r="BK82" s="26"/>
       <c r="BL82" s="26"/>
     </row>
-    <row r="83" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" s="33" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1"/>
       <c r="B83" s="75" t="s">
         <v>100</v>
@@ -8142,12 +8147,12 @@
         <v>1</v>
       </c>
       <c r="E83" s="37" t="n">
-        <f aca="false">DATE(2021,4,7)</f>
-        <v>44293</v>
+        <f aca="false">DATE(2021,4,8)</f>
+        <v>44294</v>
       </c>
       <c r="F83" s="37" t="n">
-        <f aca="false">DATE(2021,4,7)</f>
-        <v>44293</v>
+        <f aca="false">DATE(2021,4,8)</f>
+        <v>44294</v>
       </c>
       <c r="G83" s="32"/>
       <c r="H83" s="32"/>
@@ -8208,7 +8213,7 @@
       <c r="BK83" s="26"/>
       <c r="BL83" s="26"/>
     </row>
-    <row r="84" s="33" customFormat="true" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" s="33" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1"/>
       <c r="B84" s="75" t="s">
         <v>101</v>
@@ -8284,7 +8289,7 @@
       <c r="BK84" s="26"/>
       <c r="BL84" s="26"/>
     </row>
-    <row r="85" s="33" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" s="33" customFormat="true" ht="42.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1"/>
       <c r="B85" s="75" t="s">
         <v>102</v>
@@ -8294,12 +8299,12 @@
         <v>1</v>
       </c>
       <c r="E85" s="37" t="n">
-        <f aca="false">DATE(2021,4,8)</f>
-        <v>44294</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F85" s="37" t="n">
-        <f aca="false">DATE(2021,4,8)</f>
-        <v>44294</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="G85" s="32"/>
       <c r="H85" s="32"/>
@@ -8360,7 +8365,7 @@
       <c r="BK85" s="26"/>
       <c r="BL85" s="26"/>
     </row>
-    <row r="86" s="33" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" s="33" customFormat="true" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1"/>
       <c r="B86" s="75" t="s">
         <v>103</v>
@@ -8436,7 +8441,7 @@
       <c r="BK86" s="26"/>
       <c r="BL86" s="26"/>
     </row>
-    <row r="87" s="33" customFormat="true" ht="42.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" s="33" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1"/>
       <c r="B87" s="75" t="s">
         <v>104</v>
@@ -8446,12 +8451,12 @@
         <v>1</v>
       </c>
       <c r="E87" s="37" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
+        <f aca="false">DATE(2021,4,8)</f>
+        <v>44294</v>
       </c>
       <c r="F87" s="37" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
+        <f aca="false">DATE(2021,4,8)</f>
+        <v>44294</v>
       </c>
       <c r="G87" s="32"/>
       <c r="H87" s="32"/>
@@ -8512,22 +8517,20 @@
       <c r="BK87" s="26"/>
       <c r="BL87" s="26"/>
     </row>
-    <row r="88" s="33" customFormat="true" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1"/>
       <c r="B88" s="75" t="s">
         <v>105</v>
       </c>
       <c r="C88" s="76"/>
-      <c r="D88" s="36" t="n">
-        <v>1</v>
-      </c>
+      <c r="D88" s="36"/>
       <c r="E88" s="37" t="n">
-        <f aca="false">DATE(2021,4,7)</f>
-        <v>44293</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="F88" s="37" t="n">
-        <f aca="false">DATE(2021,4,7)</f>
-        <v>44293</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="G88" s="32"/>
       <c r="H88" s="32"/>
@@ -8588,7 +8591,7 @@
       <c r="BK88" s="26"/>
       <c r="BL88" s="26"/>
     </row>
-    <row r="89" s="33" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" s="33" customFormat="true" ht="42.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1"/>
       <c r="B89" s="75" t="s">
         <v>106</v>
@@ -8598,12 +8601,12 @@
         <v>1</v>
       </c>
       <c r="E89" s="37" t="n">
-        <f aca="false">DATE(2021,4,8)</f>
-        <v>44294</v>
+        <f aca="false">DATE(2021,4,7)</f>
+        <v>44293</v>
       </c>
       <c r="F89" s="37" t="n">
-        <f aca="false">DATE(2021,4,8)</f>
-        <v>44294</v>
+        <f aca="false">DATE(2021,4,7)</f>
+        <v>44293</v>
       </c>
       <c r="G89" s="32"/>
       <c r="H89" s="32"/>
@@ -8664,21 +8667,17 @@
       <c r="BK89" s="26"/>
       <c r="BL89" s="26"/>
     </row>
-    <row r="90" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1"/>
-      <c r="B90" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="C90" s="76"/>
-      <c r="D90" s="36"/>
-      <c r="E90" s="37" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
-      </c>
-      <c r="F90" s="37" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
-      </c>
+      <c r="B90" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="C90" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90" s="43"/>
+      <c r="E90" s="44"/>
+      <c r="F90" s="45"/>
       <c r="G90" s="32"/>
       <c r="H90" s="32"/>
       <c r="I90" s="26"/>
@@ -8738,22 +8737,22 @@
       <c r="BK90" s="26"/>
       <c r="BL90" s="26"/>
     </row>
-    <row r="91" s="33" customFormat="true" ht="42.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" s="33" customFormat="true" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1"/>
-      <c r="B91" s="75" t="s">
-        <v>107</v>
-      </c>
-      <c r="C91" s="76"/>
-      <c r="D91" s="36" t="n">
+      <c r="B91" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="C91" s="80"/>
+      <c r="D91" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="E91" s="37" t="n">
-        <f aca="false">DATE(2021,4,7)</f>
-        <v>44293</v>
-      </c>
-      <c r="F91" s="37" t="n">
-        <f aca="false">DATE(2021,4,7)</f>
-        <v>44293</v>
+      <c r="E91" s="49" t="n">
+        <f aca="false">DATE(2021,4,12)</f>
+        <v>44298</v>
+      </c>
+      <c r="F91" s="49" t="n">
+        <f aca="false">DATE(2021,4,12)</f>
+        <v>44298</v>
       </c>
       <c r="G91" s="32"/>
       <c r="H91" s="32"/>
@@ -8814,17 +8813,23 @@
       <c r="BK91" s="26"/>
       <c r="BL91" s="26"/>
     </row>
-    <row r="92" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="92" s="33" customFormat="true" ht="39.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1"/>
-      <c r="B92" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="C92" s="78" t="s">
-        <v>29</v>
-      </c>
-      <c r="D92" s="43"/>
-      <c r="E92" s="44"/>
-      <c r="F92" s="45"/>
+      <c r="B92" s="79" t="s">
+        <v>109</v>
+      </c>
+      <c r="C92" s="80"/>
+      <c r="D92" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E92" s="49" t="n">
+        <f aca="false">DATE(2021,4,12)</f>
+        <v>44298</v>
+      </c>
+      <c r="F92" s="49" t="n">
+        <f aca="false">DATE(2021,4,12)</f>
+        <v>44298</v>
+      </c>
       <c r="G92" s="32"/>
       <c r="H92" s="32"/>
       <c r="I92" s="26"/>
@@ -8884,10 +8889,10 @@
       <c r="BK92" s="26"/>
       <c r="BL92" s="26"/>
     </row>
-    <row r="93" s="33" customFormat="true" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="93" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1"/>
       <c r="B93" s="79" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C93" s="80"/>
       <c r="D93" s="48" t="n">
@@ -8960,22 +8965,22 @@
       <c r="BK93" s="26"/>
       <c r="BL93" s="26"/>
     </row>
-    <row r="94" s="33" customFormat="true" ht="39.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="94" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1"/>
       <c r="B94" s="79" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C94" s="80"/>
       <c r="D94" s="48" t="n">
         <v>1</v>
       </c>
       <c r="E94" s="49" t="n">
-        <f aca="false">DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f aca="false">DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="F94" s="49" t="n">
-        <f aca="false">DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f aca="false">DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="G94" s="32"/>
       <c r="H94" s="32"/>
@@ -9039,19 +9044,19 @@
     <row r="95" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1"/>
       <c r="B95" s="79" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C95" s="80"/>
       <c r="D95" s="48" t="n">
         <v>1</v>
       </c>
       <c r="E95" s="49" t="n">
-        <f aca="false">DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F95" s="49" t="n">
-        <f aca="false">DATE(2021,4,12)</f>
-        <v>44298</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="G95" s="32"/>
       <c r="H95" s="32"/>
@@ -9115,19 +9120,19 @@
     <row r="96" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="1"/>
       <c r="B96" s="79" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C96" s="80"/>
       <c r="D96" s="48" t="n">
         <v>1</v>
       </c>
       <c r="E96" s="49" t="n">
-        <f aca="false">DATE(2021,4,15)</f>
-        <v>44301</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F96" s="49" t="n">
-        <f aca="false">DATE(2021,4,15)</f>
-        <v>44301</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="G96" s="32"/>
       <c r="H96" s="32"/>
@@ -9190,21 +9195,15 @@
     </row>
     <row r="97" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1"/>
-      <c r="B97" s="79" t="s">
-        <v>113</v>
-      </c>
-      <c r="C97" s="80"/>
-      <c r="D97" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="E97" s="49" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
-      </c>
-      <c r="F97" s="49" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
-      </c>
+      <c r="B97" s="81" t="s">
+        <v>114</v>
+      </c>
+      <c r="C97" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="D97" s="83"/>
+      <c r="E97" s="84"/>
+      <c r="F97" s="85"/>
       <c r="G97" s="32"/>
       <c r="H97" s="32"/>
       <c r="I97" s="26"/>
@@ -9264,22 +9263,22 @@
       <c r="BK97" s="26"/>
       <c r="BL97" s="26"/>
     </row>
-    <row r="98" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1"/>
-      <c r="B98" s="79" t="s">
-        <v>114</v>
-      </c>
-      <c r="C98" s="80"/>
-      <c r="D98" s="48" t="n">
+      <c r="B98" s="86" t="s">
+        <v>115</v>
+      </c>
+      <c r="C98" s="87"/>
+      <c r="D98" s="88" t="n">
         <v>1</v>
       </c>
-      <c r="E98" s="49" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
-      </c>
-      <c r="F98" s="49" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
+      <c r="E98" s="89" t="n">
+        <f aca="false">DATE(2021,4,15)</f>
+        <v>44301</v>
+      </c>
+      <c r="F98" s="89" t="n">
+        <f aca="false">DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="G98" s="32"/>
       <c r="H98" s="32"/>
@@ -9340,17 +9339,23 @@
       <c r="BK98" s="26"/>
       <c r="BL98" s="26"/>
     </row>
-    <row r="99" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" s="33" customFormat="true" ht="47.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1"/>
-      <c r="B99" s="81" t="s">
-        <v>115</v>
-      </c>
-      <c r="C99" s="82" t="s">
-        <v>29</v>
-      </c>
-      <c r="D99" s="83"/>
-      <c r="E99" s="84"/>
-      <c r="F99" s="85"/>
+      <c r="B99" s="86" t="s">
+        <v>116</v>
+      </c>
+      <c r="C99" s="87"/>
+      <c r="D99" s="88" t="n">
+        <v>1</v>
+      </c>
+      <c r="E99" s="89" t="n">
+        <f aca="false">DATE(2021,4,15)</f>
+        <v>44301</v>
+      </c>
+      <c r="F99" s="89" t="n">
+        <f aca="false">DATE(2021,4,15)</f>
+        <v>44301</v>
+      </c>
       <c r="G99" s="32"/>
       <c r="H99" s="32"/>
       <c r="I99" s="26"/>
@@ -9410,22 +9415,22 @@
       <c r="BK99" s="26"/>
       <c r="BL99" s="26"/>
     </row>
-    <row r="100" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" s="33" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1"/>
       <c r="B100" s="86" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C100" s="87"/>
       <c r="D100" s="88" t="n">
         <v>1</v>
       </c>
       <c r="E100" s="89" t="n">
-        <f aca="false">DATE(2021,4,15)</f>
-        <v>44301</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F100" s="89" t="n">
-        <f aca="false">DATE(2021,4,15)</f>
-        <v>44301</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="G100" s="32"/>
       <c r="H100" s="32"/>
@@ -9486,22 +9491,22 @@
       <c r="BK100" s="26"/>
       <c r="BL100" s="26"/>
     </row>
-    <row r="101" s="33" customFormat="true" ht="47.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1"/>
       <c r="B101" s="86" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C101" s="87"/>
       <c r="D101" s="88" t="n">
         <v>1</v>
       </c>
       <c r="E101" s="89" t="n">
-        <f aca="false">DATE(2021,4,15)</f>
-        <v>44301</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F101" s="89" t="n">
-        <f aca="false">DATE(2021,4,15)</f>
-        <v>44301</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="G101" s="32"/>
       <c r="H101" s="32"/>
@@ -9562,10 +9567,10 @@
       <c r="BK101" s="26"/>
       <c r="BL101" s="26"/>
     </row>
-    <row r="102" s="33" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" s="33" customFormat="true" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1"/>
       <c r="B102" s="86" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C102" s="87"/>
       <c r="D102" s="88" t="n">
@@ -9638,10 +9643,10 @@
       <c r="BK102" s="26"/>
       <c r="BL102" s="26"/>
     </row>
-    <row r="103" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" s="33" customFormat="true" ht="48.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1"/>
       <c r="B103" s="86" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C103" s="87"/>
       <c r="D103" s="88" t="n">
@@ -9714,22 +9719,22 @@
       <c r="BK103" s="26"/>
       <c r="BL103" s="26"/>
     </row>
-    <row r="104" s="33" customFormat="true" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" s="33" customFormat="true" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1"/>
       <c r="B104" s="86" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C104" s="87"/>
       <c r="D104" s="88" t="n">
         <v>1</v>
       </c>
       <c r="E104" s="89" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="F104" s="89" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="G104" s="32"/>
       <c r="H104" s="32"/>
@@ -9790,22 +9795,22 @@
       <c r="BK104" s="26"/>
       <c r="BL104" s="26"/>
     </row>
-    <row r="105" s="33" customFormat="true" ht="48.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="105" s="33" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1"/>
       <c r="B105" s="86" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C105" s="87"/>
       <c r="D105" s="88" t="n">
         <v>1</v>
       </c>
       <c r="E105" s="89" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="F105" s="89" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="G105" s="32"/>
       <c r="H105" s="32"/>
@@ -9866,23 +9871,17 @@
       <c r="BK105" s="26"/>
       <c r="BL105" s="26"/>
     </row>
-    <row r="106" s="33" customFormat="true" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="106" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1"/>
-      <c r="B106" s="86" t="s">
-        <v>122</v>
-      </c>
-      <c r="C106" s="87"/>
-      <c r="D106" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="E106" s="89" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
-      </c>
-      <c r="F106" s="89" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
-      </c>
+      <c r="B106" s="90" t="s">
+        <v>123</v>
+      </c>
+      <c r="C106" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="D106" s="61"/>
+      <c r="E106" s="62"/>
+      <c r="F106" s="63"/>
       <c r="G106" s="32"/>
       <c r="H106" s="32"/>
       <c r="I106" s="26"/>
@@ -9942,22 +9941,22 @@
       <c r="BK106" s="26"/>
       <c r="BL106" s="26"/>
     </row>
-    <row r="107" s="33" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1"/>
-      <c r="B107" s="86" t="s">
-        <v>123</v>
-      </c>
-      <c r="C107" s="87"/>
-      <c r="D107" s="88" t="n">
+      <c r="B107" s="71" t="s">
+        <v>124</v>
+      </c>
+      <c r="C107" s="72"/>
+      <c r="D107" s="66" t="n">
         <v>1</v>
       </c>
-      <c r="E107" s="89" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
-      </c>
-      <c r="F107" s="89" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
+      <c r="E107" s="67" t="n">
+        <f aca="false">DATE(2021,4,13)</f>
+        <v>44299</v>
+      </c>
+      <c r="F107" s="67" t="n">
+        <f aca="false">DATE(2021,4,13)</f>
+        <v>44299</v>
       </c>
       <c r="G107" s="32"/>
       <c r="H107" s="32"/>
@@ -10018,17 +10017,23 @@
       <c r="BK107" s="26"/>
       <c r="BL107" s="26"/>
     </row>
-    <row r="108" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="108" s="33" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1"/>
-      <c r="B108" s="90" t="s">
-        <v>124</v>
-      </c>
-      <c r="C108" s="91" t="s">
-        <v>51</v>
-      </c>
-      <c r="D108" s="61"/>
-      <c r="E108" s="62"/>
-      <c r="F108" s="63"/>
+      <c r="B108" s="71" t="s">
+        <v>125</v>
+      </c>
+      <c r="C108" s="72"/>
+      <c r="D108" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="E108" s="67" t="n">
+        <f aca="false">DATE(2021,4,13)</f>
+        <v>44299</v>
+      </c>
+      <c r="F108" s="67" t="n">
+        <f aca="false">DATE(2021,4,13)</f>
+        <v>44299</v>
+      </c>
       <c r="G108" s="32"/>
       <c r="H108" s="32"/>
       <c r="I108" s="26"/>
@@ -10088,10 +10093,10 @@
       <c r="BK108" s="26"/>
       <c r="BL108" s="26"/>
     </row>
-    <row r="109" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="109" s="33" customFormat="true" ht="42.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1"/>
       <c r="B109" s="71" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C109" s="72"/>
       <c r="D109" s="66" t="n">
@@ -10164,22 +10169,22 @@
       <c r="BK109" s="26"/>
       <c r="BL109" s="26"/>
     </row>
-    <row r="110" s="33" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="110" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1"/>
       <c r="B110" s="71" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C110" s="72"/>
       <c r="D110" s="66" t="n">
         <v>1</v>
       </c>
       <c r="E110" s="67" t="n">
-        <f aca="false">DATE(2021,4,13)</f>
-        <v>44299</v>
+        <f aca="false">DATE(2021,4,14)</f>
+        <v>44300</v>
       </c>
       <c r="F110" s="67" t="n">
-        <f aca="false">DATE(2021,4,13)</f>
-        <v>44299</v>
+        <f aca="false">DATE(2021,4,14)</f>
+        <v>44300</v>
       </c>
       <c r="G110" s="32"/>
       <c r="H110" s="32"/>
@@ -10240,22 +10245,22 @@
       <c r="BK110" s="26"/>
       <c r="BL110" s="26"/>
     </row>
-    <row r="111" s="33" customFormat="true" ht="42.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="111" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1"/>
       <c r="B111" s="71" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C111" s="72"/>
       <c r="D111" s="66" t="n">
         <v>1</v>
       </c>
       <c r="E111" s="67" t="n">
-        <f aca="false">DATE(2021,4,13)</f>
-        <v>44299</v>
+        <f aca="false">DATE(2021,4,14)</f>
+        <v>44300</v>
       </c>
       <c r="F111" s="67" t="n">
-        <f aca="false">DATE(2021,4,13)</f>
-        <v>44299</v>
+        <f aca="false">DATE(2021,4,14)</f>
+        <v>44300</v>
       </c>
       <c r="G111" s="32"/>
       <c r="H111" s="32"/>
@@ -10316,22 +10321,22 @@
       <c r="BK111" s="26"/>
       <c r="BL111" s="26"/>
     </row>
-    <row r="112" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="112" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1"/>
       <c r="B112" s="71" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C112" s="72"/>
       <c r="D112" s="66" t="n">
         <v>1</v>
       </c>
       <c r="E112" s="67" t="n">
-        <f aca="false">DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="F112" s="67" t="n">
-        <f aca="false">DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="G112" s="32"/>
       <c r="H112" s="32"/>
@@ -10395,19 +10400,19 @@
     <row r="113" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1"/>
       <c r="B113" s="71" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C113" s="72"/>
       <c r="D113" s="66" t="n">
         <v>1</v>
       </c>
       <c r="E113" s="67" t="n">
-        <f aca="false">DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f aca="false">DATE(2021,4,29)</f>
+        <v>44315</v>
       </c>
       <c r="F113" s="67" t="n">
-        <f aca="false">DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f aca="false">DATE(2021,4,29)</f>
+        <v>44315</v>
       </c>
       <c r="G113" s="32"/>
       <c r="H113" s="32"/>
@@ -10471,19 +10476,19 @@
     <row r="114" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1"/>
       <c r="B114" s="71" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C114" s="72"/>
       <c r="D114" s="66" t="n">
         <v>1</v>
       </c>
       <c r="E114" s="67" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
+        <f aca="false">DATE(2021,4,27)</f>
+        <v>44313</v>
       </c>
       <c r="F114" s="67" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
+        <f aca="false">DATE(2021,4,27)</f>
+        <v>44313</v>
       </c>
       <c r="G114" s="32"/>
       <c r="H114" s="32"/>
@@ -10547,17 +10552,19 @@
     <row r="115" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="1"/>
       <c r="B115" s="71" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C115" s="72"/>
-      <c r="D115" s="66"/>
+      <c r="D115" s="66" t="n">
+        <v>1</v>
+      </c>
       <c r="E115" s="67" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
+        <f aca="false">DATE(2021,4,25)</f>
+        <v>44311</v>
       </c>
       <c r="F115" s="67" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
+        <f aca="false">DATE(2021,4,25)</f>
+        <v>44311</v>
       </c>
       <c r="G115" s="32"/>
       <c r="H115" s="32"/>
@@ -10621,19 +10628,17 @@
     <row r="116" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="1"/>
       <c r="B116" s="71" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C116" s="72"/>
-      <c r="D116" s="66" t="n">
-        <v>1</v>
-      </c>
+      <c r="D116" s="66"/>
       <c r="E116" s="67" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
+        <f aca="false">DATE(2021,4,30)</f>
+        <v>44316</v>
       </c>
       <c r="F116" s="67" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
+        <f aca="false">DATE(2021,4,30)</f>
+        <v>44316</v>
       </c>
       <c r="G116" s="32"/>
       <c r="H116" s="32"/>
@@ -10694,23 +10699,17 @@
       <c r="BK116" s="26"/>
       <c r="BL116" s="26"/>
     </row>
-    <row r="117" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="117" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1"/>
-      <c r="B117" s="71" t="s">
-        <v>133</v>
-      </c>
-      <c r="C117" s="72"/>
-      <c r="D117" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="E117" s="67" t="n">
-        <f aca="false">DATE(2021,4,25)</f>
-        <v>44311</v>
-      </c>
-      <c r="F117" s="67" t="n">
-        <f aca="false">DATE(2021,4,25)</f>
-        <v>44311</v>
-      </c>
+      <c r="B117" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C117" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D117" s="29"/>
+      <c r="E117" s="30"/>
+      <c r="F117" s="31"/>
       <c r="G117" s="32"/>
       <c r="H117" s="32"/>
       <c r="I117" s="26"/>
@@ -10772,15 +10771,21 @@
     </row>
     <row r="118" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="1"/>
-      <c r="B118" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="C118" s="74" t="s">
-        <v>51</v>
-      </c>
-      <c r="D118" s="29"/>
-      <c r="E118" s="30"/>
-      <c r="F118" s="31"/>
+      <c r="B118" s="75" t="s">
+        <v>135</v>
+      </c>
+      <c r="C118" s="76"/>
+      <c r="D118" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" s="92" t="n">
+        <f aca="false">DATE(2021,4,14)</f>
+        <v>44300</v>
+      </c>
+      <c r="F118" s="92" t="n">
+        <f aca="false">DATE(2021,4,14)</f>
+        <v>44300</v>
+      </c>
       <c r="G118" s="32"/>
       <c r="H118" s="32"/>
       <c r="I118" s="26"/>
@@ -10840,10 +10845,10 @@
       <c r="BK118" s="26"/>
       <c r="BL118" s="26"/>
     </row>
-    <row r="119" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="119" s="33" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="1"/>
       <c r="B119" s="75" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C119" s="76"/>
       <c r="D119" s="36" t="n">
@@ -10916,10 +10921,10 @@
       <c r="BK119" s="26"/>
       <c r="BL119" s="26"/>
     </row>
-    <row r="120" s="33" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="120" s="33" customFormat="true" ht="38.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="1"/>
       <c r="B120" s="75" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C120" s="76"/>
       <c r="D120" s="36" t="n">
@@ -10992,22 +10997,22 @@
       <c r="BK120" s="26"/>
       <c r="BL120" s="26"/>
     </row>
-    <row r="121" s="33" customFormat="true" ht="38.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="121" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="1"/>
       <c r="B121" s="75" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C121" s="76"/>
       <c r="D121" s="36" t="n">
         <v>1</v>
       </c>
       <c r="E121" s="92" t="n">
-        <f aca="false">DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f aca="false">DATE(2021,4,22)</f>
+        <v>44308</v>
       </c>
       <c r="F121" s="92" t="n">
-        <f aca="false">DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f aca="false">DATE(2021,4,22)</f>
+        <v>44308</v>
       </c>
       <c r="G121" s="32"/>
       <c r="H121" s="32"/>
@@ -11068,22 +11073,22 @@
       <c r="BK121" s="26"/>
       <c r="BL121" s="26"/>
     </row>
-    <row r="122" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="122" s="33" customFormat="true" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="1"/>
       <c r="B122" s="75" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="C122" s="76"/>
       <c r="D122" s="36" t="n">
         <v>1</v>
       </c>
       <c r="E122" s="92" t="n">
-        <f aca="false">DATE(2021,4,22)</f>
-        <v>44308</v>
+        <f aca="false">DATE(2021,4,14)</f>
+        <v>44300</v>
       </c>
       <c r="F122" s="92" t="n">
-        <f aca="false">DATE(2021,4,22)</f>
-        <v>44308</v>
+        <f aca="false">DATE(2021,4,14)</f>
+        <v>44300</v>
       </c>
       <c r="G122" s="32"/>
       <c r="H122" s="32"/>
@@ -11144,22 +11149,22 @@
       <c r="BK122" s="26"/>
       <c r="BL122" s="26"/>
     </row>
-    <row r="123" s="33" customFormat="true" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="123" s="33" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
       <c r="B123" s="75" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="C123" s="76"/>
       <c r="D123" s="36" t="n">
         <v>1</v>
       </c>
       <c r="E123" s="92" t="n">
-        <f aca="false">DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f aca="false">DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="F123" s="92" t="n">
-        <f aca="false">DATE(2021,4,14)</f>
-        <v>44300</v>
+        <f aca="false">DATE(2021,4,15)</f>
+        <v>44301</v>
       </c>
       <c r="G123" s="32"/>
       <c r="H123" s="32"/>
@@ -11220,10 +11225,10 @@
       <c r="BK123" s="26"/>
       <c r="BL123" s="26"/>
     </row>
-    <row r="124" s="33" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="124" s="33" customFormat="true" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="1"/>
       <c r="B124" s="75" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C124" s="76"/>
       <c r="D124" s="36" t="n">
@@ -11296,10 +11301,10 @@
       <c r="BK124" s="26"/>
       <c r="BL124" s="26"/>
     </row>
-    <row r="125" s="33" customFormat="true" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="125" s="33" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="1"/>
       <c r="B125" s="75" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C125" s="76"/>
       <c r="D125" s="36" t="n">
@@ -11372,22 +11377,20 @@
       <c r="BK125" s="26"/>
       <c r="BL125" s="26"/>
     </row>
-    <row r="126" s="33" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="126" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="1"/>
       <c r="B126" s="75" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C126" s="76"/>
-      <c r="D126" s="36" t="n">
-        <v>1</v>
-      </c>
+      <c r="D126" s="36"/>
       <c r="E126" s="92" t="n">
-        <f aca="false">DATE(2021,4,15)</f>
-        <v>44301</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="F126" s="92" t="n">
-        <f aca="false">DATE(2021,4,15)</f>
-        <v>44301</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="G126" s="32"/>
       <c r="H126" s="32"/>
@@ -11451,17 +11454,19 @@
     <row r="127" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="1"/>
       <c r="B127" s="75" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C127" s="76"/>
-      <c r="D127" s="36"/>
+      <c r="D127" s="36" t="n">
+        <v>1</v>
+      </c>
       <c r="E127" s="92" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
+        <f aca="false">DATE(2021,4,27)</f>
+        <v>44313</v>
       </c>
       <c r="F127" s="92" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
+        <f aca="false">DATE(2021,4,27)</f>
+        <v>44313</v>
       </c>
       <c r="G127" s="32"/>
       <c r="H127" s="32"/>
@@ -11525,7 +11530,7 @@
     <row r="128" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="1"/>
       <c r="B128" s="75" t="s">
-        <v>49</v>
+        <v>142</v>
       </c>
       <c r="C128" s="76"/>
       <c r="D128" s="36" t="n">
@@ -11600,21 +11605,15 @@
     </row>
     <row r="129" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="1"/>
-      <c r="B129" s="75" t="s">
-        <v>142</v>
-      </c>
-      <c r="C129" s="76"/>
-      <c r="D129" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="E129" s="92" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
-      </c>
-      <c r="F129" s="92" t="n">
-        <f aca="false">DATE(2021,4,27)</f>
-        <v>44313</v>
-      </c>
+      <c r="B129" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="C129" s="78" t="s">
+        <v>51</v>
+      </c>
+      <c r="D129" s="43"/>
+      <c r="E129" s="44"/>
+      <c r="F129" s="45"/>
       <c r="G129" s="32"/>
       <c r="H129" s="32"/>
       <c r="I129" s="26"/>
@@ -11676,15 +11675,21 @@
     </row>
     <row r="130" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="1"/>
-      <c r="B130" s="77" t="s">
-        <v>143</v>
-      </c>
-      <c r="C130" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="D130" s="43"/>
-      <c r="E130" s="44"/>
-      <c r="F130" s="45"/>
+      <c r="B130" s="79" t="s">
+        <v>115</v>
+      </c>
+      <c r="C130" s="80"/>
+      <c r="D130" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E130" s="49" t="n">
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
+      </c>
+      <c r="F130" s="49" t="n">
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
+      </c>
       <c r="G130" s="32"/>
       <c r="H130" s="32"/>
       <c r="I130" s="26"/>
@@ -11747,7 +11752,7 @@
     <row r="131" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="1"/>
       <c r="B131" s="79" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="C131" s="80"/>
       <c r="D131" s="48" t="n">
@@ -11823,7 +11828,7 @@
     <row r="132" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="1"/>
       <c r="B132" s="79" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="C132" s="80"/>
       <c r="D132" s="48" t="n">
@@ -11972,23 +11977,17 @@
       <c r="BK133" s="26"/>
       <c r="BL133" s="26"/>
     </row>
-    <row r="134" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="134" s="33" customFormat="true" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="1"/>
-      <c r="B134" s="79" t="s">
-        <v>120</v>
-      </c>
-      <c r="C134" s="80"/>
-      <c r="D134" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="E134" s="49" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
-      </c>
-      <c r="F134" s="49" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
-      </c>
+      <c r="B134" s="81" t="s">
+        <v>145</v>
+      </c>
+      <c r="C134" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="D134" s="83"/>
+      <c r="E134" s="84"/>
+      <c r="F134" s="85"/>
       <c r="G134" s="32"/>
       <c r="H134" s="32"/>
       <c r="I134" s="26"/>
@@ -12048,17 +12047,23 @@
       <c r="BK134" s="26"/>
       <c r="BL134" s="26"/>
     </row>
-    <row r="135" s="33" customFormat="true" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="135" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="1"/>
-      <c r="B135" s="81" t="s">
-        <v>145</v>
-      </c>
-      <c r="C135" s="82" t="s">
-        <v>29</v>
-      </c>
-      <c r="D135" s="83"/>
-      <c r="E135" s="84"/>
-      <c r="F135" s="85"/>
+      <c r="B135" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="C135" s="87"/>
+      <c r="D135" s="88" t="n">
+        <v>1</v>
+      </c>
+      <c r="E135" s="89" t="n">
+        <f aca="false">DATE(2021,4,16)</f>
+        <v>44302</v>
+      </c>
+      <c r="F135" s="89" t="n">
+        <f aca="false">DATE(2021,4,16)</f>
+        <v>44302</v>
+      </c>
       <c r="G135" s="32"/>
       <c r="H135" s="32"/>
       <c r="I135" s="26"/>
@@ -12118,10 +12123,10 @@
       <c r="BK135" s="26"/>
       <c r="BL135" s="26"/>
     </row>
-    <row r="136" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="136" s="33" customFormat="true" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="1"/>
       <c r="B136" s="86" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C136" s="87"/>
       <c r="D136" s="88" t="n">
@@ -12194,10 +12199,10 @@
       <c r="BK136" s="26"/>
       <c r="BL136" s="26"/>
     </row>
-    <row r="137" s="33" customFormat="true" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="137" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="1"/>
       <c r="B137" s="86" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C137" s="87"/>
       <c r="D137" s="88" t="n">
@@ -12270,23 +12275,17 @@
       <c r="BK137" s="26"/>
       <c r="BL137" s="26"/>
     </row>
-    <row r="138" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="138" s="33" customFormat="true" ht="45.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="1"/>
-      <c r="B138" s="86" t="s">
-        <v>148</v>
-      </c>
-      <c r="C138" s="87"/>
-      <c r="D138" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="E138" s="89" t="n">
-        <f aca="false">DATE(2021,4,16)</f>
-        <v>44302</v>
-      </c>
-      <c r="F138" s="89" t="n">
-        <f aca="false">DATE(2021,4,16)</f>
-        <v>44302</v>
-      </c>
+      <c r="B138" s="90" t="s">
+        <v>149</v>
+      </c>
+      <c r="C138" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="D138" s="61"/>
+      <c r="E138" s="62"/>
+      <c r="F138" s="63"/>
       <c r="G138" s="32"/>
       <c r="H138" s="32"/>
       <c r="I138" s="26"/>
@@ -12346,17 +12345,23 @@
       <c r="BK138" s="26"/>
       <c r="BL138" s="26"/>
     </row>
-    <row r="139" s="33" customFormat="true" ht="45.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="139" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="1"/>
-      <c r="B139" s="90" t="s">
-        <v>149</v>
-      </c>
-      <c r="C139" s="91" t="s">
-        <v>51</v>
-      </c>
-      <c r="D139" s="61"/>
-      <c r="E139" s="62"/>
-      <c r="F139" s="63"/>
+      <c r="B139" s="71" t="s">
+        <v>150</v>
+      </c>
+      <c r="C139" s="72"/>
+      <c r="D139" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="E139" s="67" t="n">
+        <f aca="false">DATE(2021,4,16)</f>
+        <v>44302</v>
+      </c>
+      <c r="F139" s="67" t="n">
+        <f aca="false">DATE(2021,4,16)</f>
+        <v>44302</v>
+      </c>
       <c r="G139" s="32"/>
       <c r="H139" s="32"/>
       <c r="I139" s="26"/>
@@ -12416,10 +12421,10 @@
       <c r="BK139" s="26"/>
       <c r="BL139" s="26"/>
     </row>
-    <row r="140" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="140" s="33" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="1"/>
       <c r="B140" s="71" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C140" s="72"/>
       <c r="D140" s="66" t="n">
@@ -12492,10 +12497,10 @@
       <c r="BK140" s="26"/>
       <c r="BL140" s="26"/>
     </row>
-    <row r="141" s="33" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="141" s="33" customFormat="true" ht="95.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="1"/>
       <c r="B141" s="71" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C141" s="72"/>
       <c r="D141" s="66" t="n">
@@ -12568,22 +12573,22 @@
       <c r="BK141" s="26"/>
       <c r="BL141" s="26"/>
     </row>
-    <row r="142" s="33" customFormat="true" ht="95.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="142" s="33" customFormat="true" ht="59.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="1"/>
       <c r="B142" s="71" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C142" s="72"/>
       <c r="D142" s="66" t="n">
         <v>1</v>
       </c>
       <c r="E142" s="67" t="n">
-        <f aca="false">DATE(2021,4,16)</f>
-        <v>44302</v>
+        <f aca="false">DATE(2021,4,19)</f>
+        <v>44305</v>
       </c>
       <c r="F142" s="67" t="n">
-        <f aca="false">DATE(2021,4,16)</f>
-        <v>44302</v>
+        <f aca="false">DATE(2021,4,19)</f>
+        <v>44305</v>
       </c>
       <c r="G142" s="32"/>
       <c r="H142" s="32"/>
@@ -12644,10 +12649,10 @@
       <c r="BK142" s="26"/>
       <c r="BL142" s="26"/>
     </row>
-    <row r="143" s="33" customFormat="true" ht="59.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="143" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="1"/>
       <c r="B143" s="71" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C143" s="72"/>
       <c r="D143" s="66" t="n">
@@ -12720,10 +12725,10 @@
       <c r="BK143" s="26"/>
       <c r="BL143" s="26"/>
     </row>
-    <row r="144" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="144" s="33" customFormat="true" ht="57.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="1"/>
       <c r="B144" s="71" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C144" s="72"/>
       <c r="D144" s="66" t="n">
@@ -12796,10 +12801,10 @@
       <c r="BK144" s="26"/>
       <c r="BL144" s="26"/>
     </row>
-    <row r="145" s="33" customFormat="true" ht="57.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1"/>
+    <row r="145" s="33" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A145" s="93"/>
       <c r="B145" s="71" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C145" s="72"/>
       <c r="D145" s="66" t="n">
@@ -12872,22 +12877,22 @@
       <c r="BK145" s="26"/>
       <c r="BL145" s="26"/>
     </row>
-    <row r="146" s="33" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="93"/>
+    <row r="146" s="33" customFormat="true" ht="96" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1"/>
       <c r="B146" s="71" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C146" s="72"/>
       <c r="D146" s="66" t="n">
         <v>1</v>
       </c>
       <c r="E146" s="67" t="n">
-        <f aca="false">DATE(2021,4,19)</f>
-        <v>44305</v>
+        <f aca="false">DATE(2021,4,20)</f>
+        <v>44306</v>
       </c>
       <c r="F146" s="67" t="n">
-        <f aca="false">DATE(2021,4,19)</f>
-        <v>44305</v>
+        <f aca="false">DATE(2021,4,20)</f>
+        <v>44306</v>
       </c>
       <c r="G146" s="32"/>
       <c r="H146" s="32"/>
@@ -12948,22 +12953,22 @@
       <c r="BK146" s="26"/>
       <c r="BL146" s="26"/>
     </row>
-    <row r="147" s="33" customFormat="true" ht="96" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="147" s="33" customFormat="true" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="1"/>
       <c r="B147" s="71" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C147" s="72"/>
       <c r="D147" s="66" t="n">
         <v>1</v>
       </c>
       <c r="E147" s="67" t="n">
-        <f aca="false">DATE(2021,4,20)</f>
-        <v>44306</v>
+        <f aca="false">DATE(2021,4,26)</f>
+        <v>44312</v>
       </c>
       <c r="F147" s="67" t="n">
-        <f aca="false">DATE(2021,4,20)</f>
-        <v>44306</v>
+        <f aca="false">DATE(2021,4,26)</f>
+        <v>44312</v>
       </c>
       <c r="G147" s="32"/>
       <c r="H147" s="32"/>
@@ -13027,7 +13032,7 @@
     <row r="148" s="33" customFormat="true" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="1"/>
       <c r="B148" s="71" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C148" s="72"/>
       <c r="D148" s="66" t="n">
@@ -13100,23 +13105,17 @@
       <c r="BK148" s="26"/>
       <c r="BL148" s="26"/>
     </row>
-    <row r="149" s="33" customFormat="true" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="149" s="33" customFormat="true" ht="30.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="1"/>
-      <c r="B149" s="71" t="s">
-        <v>159</v>
-      </c>
-      <c r="C149" s="72"/>
-      <c r="D149" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="E149" s="67" t="n">
-        <f aca="false">DATE(2021,4,26)</f>
-        <v>44312</v>
-      </c>
-      <c r="F149" s="67" t="n">
-        <f aca="false">DATE(2021,4,26)</f>
-        <v>44312</v>
-      </c>
+      <c r="B149" s="73" t="s">
+        <v>160</v>
+      </c>
+      <c r="C149" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="D149" s="29"/>
+      <c r="E149" s="30"/>
+      <c r="F149" s="31"/>
       <c r="G149" s="32"/>
       <c r="H149" s="32"/>
       <c r="I149" s="26"/>
@@ -13176,17 +13175,23 @@
       <c r="BK149" s="26"/>
       <c r="BL149" s="26"/>
     </row>
-    <row r="150" s="33" customFormat="true" ht="30.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="150" s="33" customFormat="true" ht="56.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="1"/>
-      <c r="B150" s="73" t="s">
-        <v>160</v>
-      </c>
-      <c r="C150" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="D150" s="29"/>
-      <c r="E150" s="30"/>
-      <c r="F150" s="31"/>
+      <c r="B150" s="75" t="s">
+        <v>161</v>
+      </c>
+      <c r="C150" s="76"/>
+      <c r="D150" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E150" s="37" t="n">
+        <f aca="false">DATE(2021,4,19)</f>
+        <v>44305</v>
+      </c>
+      <c r="F150" s="37" t="n">
+        <f aca="false">DATE(2021,4,19)</f>
+        <v>44305</v>
+      </c>
       <c r="G150" s="32"/>
       <c r="H150" s="32"/>
       <c r="I150" s="26"/>
@@ -13246,10 +13251,10 @@
       <c r="BK150" s="26"/>
       <c r="BL150" s="26"/>
     </row>
-    <row r="151" s="33" customFormat="true" ht="56.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="151" s="33" customFormat="true" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="1"/>
       <c r="B151" s="75" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C151" s="76"/>
       <c r="D151" s="36" t="n">
@@ -13322,10 +13327,10 @@
       <c r="BK151" s="26"/>
       <c r="BL151" s="26"/>
     </row>
-    <row r="152" s="33" customFormat="true" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="152" s="33" customFormat="true" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="1"/>
       <c r="B152" s="75" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C152" s="76"/>
       <c r="D152" s="36" t="n">
@@ -13398,10 +13403,10 @@
       <c r="BK152" s="26"/>
       <c r="BL152" s="26"/>
     </row>
-    <row r="153" s="33" customFormat="true" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="153" s="33" customFormat="true" ht="48.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="1"/>
       <c r="B153" s="75" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C153" s="76"/>
       <c r="D153" s="36" t="n">
@@ -13474,10 +13479,10 @@
       <c r="BK153" s="26"/>
       <c r="BL153" s="26"/>
     </row>
-    <row r="154" s="33" customFormat="true" ht="48.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="154" s="33" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="1"/>
       <c r="B154" s="75" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C154" s="76"/>
       <c r="D154" s="36" t="n">
@@ -13550,22 +13555,22 @@
       <c r="BK154" s="26"/>
       <c r="BL154" s="26"/>
     </row>
-    <row r="155" s="33" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="155" s="33" customFormat="true" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="1"/>
       <c r="B155" s="75" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C155" s="76"/>
       <c r="D155" s="36" t="n">
         <v>1</v>
       </c>
       <c r="E155" s="37" t="n">
-        <f aca="false">DATE(2021,4,19)</f>
-        <v>44305</v>
+        <f aca="false">DATE(2021,4,20)</f>
+        <v>44306</v>
       </c>
       <c r="F155" s="37" t="n">
-        <f aca="false">DATE(2021,4,19)</f>
-        <v>44305</v>
+        <f aca="false">DATE(2021,4,20)</f>
+        <v>44306</v>
       </c>
       <c r="G155" s="32"/>
       <c r="H155" s="32"/>
@@ -13626,22 +13631,22 @@
       <c r="BK155" s="26"/>
       <c r="BL155" s="26"/>
     </row>
-    <row r="156" s="33" customFormat="true" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="156" s="33" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="1"/>
       <c r="B156" s="75" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C156" s="76"/>
       <c r="D156" s="36" t="n">
         <v>1</v>
       </c>
       <c r="E156" s="37" t="n">
-        <f aca="false">DATE(2021,4,20)</f>
-        <v>44306</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F156" s="37" t="n">
-        <f aca="false">DATE(2021,4,20)</f>
-        <v>44306</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="G156" s="32"/>
       <c r="H156" s="32"/>
@@ -13702,23 +13707,17 @@
       <c r="BK156" s="26"/>
       <c r="BL156" s="26"/>
     </row>
-    <row r="157" s="33" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="157" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="1"/>
-      <c r="B157" s="75" t="s">
-        <v>167</v>
-      </c>
-      <c r="C157" s="76"/>
-      <c r="D157" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="E157" s="37" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
-      </c>
-      <c r="F157" s="37" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
-      </c>
+      <c r="B157" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="C157" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D157" s="43"/>
+      <c r="E157" s="44"/>
+      <c r="F157" s="45"/>
       <c r="G157" s="32"/>
       <c r="H157" s="32"/>
       <c r="I157" s="26"/>
@@ -13778,17 +13777,23 @@
       <c r="BK157" s="26"/>
       <c r="BL157" s="26"/>
     </row>
-    <row r="158" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="158" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="1"/>
-      <c r="B158" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="C158" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="D158" s="43"/>
-      <c r="E158" s="44"/>
-      <c r="F158" s="45"/>
+      <c r="B158" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="C158" s="47"/>
+      <c r="D158" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E158" s="49" t="n">
+        <f aca="false">DATE(2021,4,20)</f>
+        <v>44306</v>
+      </c>
+      <c r="F158" s="49" t="n">
+        <f aca="false">DATE(2021,4,20)</f>
+        <v>44306</v>
+      </c>
       <c r="G158" s="32"/>
       <c r="H158" s="32"/>
       <c r="I158" s="26"/>
@@ -13848,12 +13853,12 @@
       <c r="BK158" s="26"/>
       <c r="BL158" s="26"/>
     </row>
-    <row r="159" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="159" s="33" customFormat="true" ht="50.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="1"/>
-      <c r="B159" s="46" t="s">
-        <v>169</v>
-      </c>
-      <c r="C159" s="47"/>
+      <c r="B159" s="79" t="s">
+        <v>170</v>
+      </c>
+      <c r="C159" s="80"/>
       <c r="D159" s="48" t="n">
         <v>1</v>
       </c>
@@ -13924,10 +13929,10 @@
       <c r="BK159" s="26"/>
       <c r="BL159" s="26"/>
     </row>
-    <row r="160" s="33" customFormat="true" ht="50.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="160" s="33" customFormat="true" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="1"/>
       <c r="B160" s="79" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C160" s="80"/>
       <c r="D160" s="48" t="n">
@@ -14000,22 +14005,22 @@
       <c r="BK160" s="26"/>
       <c r="BL160" s="26"/>
     </row>
-    <row r="161" s="33" customFormat="true" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="161" s="33" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="1"/>
       <c r="B161" s="79" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C161" s="80"/>
       <c r="D161" s="48" t="n">
         <v>1</v>
       </c>
       <c r="E161" s="49" t="n">
-        <f aca="false">DATE(2021,4,20)</f>
-        <v>44306</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="F161" s="49" t="n">
-        <f aca="false">DATE(2021,4,20)</f>
-        <v>44306</v>
+        <f aca="false">DATE(2021,4,21)</f>
+        <v>44307</v>
       </c>
       <c r="G161" s="32"/>
       <c r="H161" s="32"/>
@@ -14076,10 +14081,10 @@
       <c r="BK161" s="26"/>
       <c r="BL161" s="26"/>
     </row>
-    <row r="162" s="33" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="162" s="33" customFormat="true" ht="44.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="1"/>
       <c r="B162" s="79" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C162" s="80"/>
       <c r="D162" s="48" t="n">
@@ -14152,10 +14157,10 @@
       <c r="BK162" s="26"/>
       <c r="BL162" s="26"/>
     </row>
-    <row r="163" s="33" customFormat="true" ht="44.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="163" s="33" customFormat="true" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="1"/>
       <c r="B163" s="79" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C163" s="80"/>
       <c r="D163" s="48" t="n">
@@ -14228,22 +14233,20 @@
       <c r="BK163" s="26"/>
       <c r="BL163" s="26"/>
     </row>
-    <row r="164" s="33" customFormat="true" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="164" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="1"/>
       <c r="B164" s="79" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C164" s="80"/>
-      <c r="D164" s="48" t="n">
-        <v>1</v>
-      </c>
+      <c r="D164" s="48"/>
       <c r="E164" s="49" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="F164" s="49" t="n">
-        <f aca="false">DATE(2021,4,21)</f>
-        <v>44307</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="G164" s="32"/>
       <c r="H164" s="32"/>
@@ -14262,9 +14265,7 @@
       <c r="U164" s="26"/>
       <c r="V164" s="26"/>
       <c r="W164" s="26"/>
-      <c r="X164" s="26" t="s">
-        <v>175</v>
-      </c>
+      <c r="X164" s="26"/>
       <c r="Y164" s="26"/>
       <c r="Z164" s="26"/>
       <c r="AA164" s="26"/>
@@ -14314,12 +14315,12 @@
       <c r="C165" s="80"/>
       <c r="D165" s="48"/>
       <c r="E165" s="49" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
+        <f aca="false">DATE(2021,4,26)</f>
+        <v>44312</v>
       </c>
       <c r="F165" s="49" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
+        <f aca="false">DATE(2021,4,30)</f>
+        <v>44316</v>
       </c>
       <c r="G165" s="32"/>
       <c r="H165" s="32"/>
@@ -14460,14 +14461,16 @@
         <v>178</v>
       </c>
       <c r="C167" s="80"/>
-      <c r="D167" s="48"/>
+      <c r="D167" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="E167" s="49" t="n">
         <f aca="false">DATE(2021,4,26)</f>
         <v>44312</v>
       </c>
       <c r="F167" s="49" t="n">
-        <f aca="false">DATE(2021,4,30)</f>
-        <v>44316</v>
+        <f aca="false">DATE(2021,4,26)</f>
+        <v>44312</v>
       </c>
       <c r="G167" s="32"/>
       <c r="H167" s="32"/>
@@ -14528,7 +14531,7 @@
       <c r="BK167" s="26"/>
       <c r="BL167" s="26"/>
     </row>
-    <row r="168" s="33" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="168" s="33" customFormat="true" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="1"/>
       <c r="B168" s="79" t="s">
         <v>179</v>
@@ -14538,12 +14541,12 @@
         <v>1</v>
       </c>
       <c r="E168" s="49" t="n">
-        <f aca="false">DATE(2021,4,26)</f>
-        <v>44312</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="F168" s="49" t="n">
-        <f aca="false">DATE(2021,4,26)</f>
-        <v>44312</v>
+        <f aca="false">DATE(2021,4,23)</f>
+        <v>44309</v>
       </c>
       <c r="G168" s="32"/>
       <c r="H168" s="32"/>
@@ -14606,19 +14609,11 @@
     </row>
     <row r="169" s="33" customFormat="true" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="1"/>
-      <c r="B169" s="79" t="s">
-        <v>180</v>
-      </c>
+      <c r="B169" s="79"/>
       <c r="C169" s="80"/>
       <c r="D169" s="48"/>
-      <c r="E169" s="49" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
-      </c>
-      <c r="F169" s="49" t="n">
-        <f aca="false">DATE(2021,4,23)</f>
-        <v>44309</v>
-      </c>
+      <c r="E169" s="49"/>
+      <c r="F169" s="49"/>
       <c r="G169" s="32"/>
       <c r="H169" s="32"/>
       <c r="I169" s="26"/>
@@ -14680,11 +14675,15 @@
     </row>
     <row r="170" s="33" customFormat="true" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="1"/>
-      <c r="B170" s="79"/>
-      <c r="C170" s="80"/>
-      <c r="D170" s="48"/>
-      <c r="E170" s="49"/>
-      <c r="F170" s="49"/>
+      <c r="B170" s="90" t="s">
+        <v>180</v>
+      </c>
+      <c r="C170" s="91" t="s">
+        <v>181</v>
+      </c>
+      <c r="D170" s="61"/>
+      <c r="E170" s="62"/>
+      <c r="F170" s="63"/>
       <c r="G170" s="32"/>
       <c r="H170" s="32"/>
       <c r="I170" s="26"/>
@@ -14746,15 +14745,11 @@
     </row>
     <row r="171" s="33" customFormat="true" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="1"/>
-      <c r="B171" s="90" t="s">
-        <v>181</v>
-      </c>
-      <c r="C171" s="91" t="s">
-        <v>182</v>
-      </c>
-      <c r="D171" s="61"/>
-      <c r="E171" s="62"/>
-      <c r="F171" s="63"/>
+      <c r="B171" s="71"/>
+      <c r="C171" s="72"/>
+      <c r="D171" s="66"/>
+      <c r="E171" s="67"/>
+      <c r="F171" s="67"/>
       <c r="G171" s="32"/>
       <c r="H171" s="32"/>
       <c r="I171" s="26"/>
@@ -15012,13 +15007,15 @@
       <c r="BK174" s="26"/>
       <c r="BL174" s="26"/>
     </row>
-    <row r="175" s="33" customFormat="true" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="175" s="33" customFormat="true" ht="54.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="1"/>
-      <c r="B175" s="71"/>
-      <c r="C175" s="72"/>
-      <c r="D175" s="66"/>
-      <c r="E175" s="67"/>
-      <c r="F175" s="67"/>
+      <c r="B175" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="C175" s="95"/>
+      <c r="D175" s="96"/>
+      <c r="E175" s="97"/>
+      <c r="F175" s="98"/>
       <c r="G175" s="32"/>
       <c r="H175" s="32"/>
       <c r="I175" s="26"/>
@@ -15078,151 +15075,84 @@
       <c r="BK175" s="26"/>
       <c r="BL175" s="26"/>
     </row>
-    <row r="176" s="33" customFormat="true" ht="54.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1"/>
-      <c r="B176" s="94" t="s">
+    <row r="176" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A176" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C176" s="95"/>
-      <c r="D176" s="96"/>
-      <c r="E176" s="97"/>
-      <c r="F176" s="98"/>
-      <c r="G176" s="32"/>
-      <c r="H176" s="32"/>
-      <c r="I176" s="26"/>
-      <c r="J176" s="26"/>
-      <c r="K176" s="26"/>
-      <c r="L176" s="26"/>
-      <c r="M176" s="26"/>
-      <c r="N176" s="26"/>
-      <c r="O176" s="26"/>
-      <c r="P176" s="26"/>
-      <c r="Q176" s="26"/>
-      <c r="R176" s="26"/>
-      <c r="S176" s="26"/>
-      <c r="T176" s="26"/>
-      <c r="U176" s="26"/>
-      <c r="V176" s="26"/>
-      <c r="W176" s="26"/>
-      <c r="X176" s="26"/>
-      <c r="Y176" s="26"/>
-      <c r="Z176" s="26"/>
-      <c r="AA176" s="26"/>
-      <c r="AB176" s="26"/>
-      <c r="AC176" s="26"/>
-      <c r="AD176" s="26"/>
-      <c r="AE176" s="26"/>
-      <c r="AF176" s="26"/>
-      <c r="AG176" s="26"/>
-      <c r="AH176" s="26"/>
-      <c r="AI176" s="26"/>
-      <c r="AJ176" s="26"/>
-      <c r="AK176" s="26"/>
-      <c r="AL176" s="26"/>
-      <c r="AM176" s="26"/>
-      <c r="AN176" s="26"/>
-      <c r="AO176" s="26"/>
-      <c r="AP176" s="26"/>
-      <c r="AQ176" s="26"/>
-      <c r="AR176" s="26"/>
-      <c r="AS176" s="26"/>
-      <c r="AT176" s="26"/>
-      <c r="AU176" s="26"/>
-      <c r="AV176" s="26"/>
-      <c r="AW176" s="26"/>
-      <c r="AX176" s="26"/>
-      <c r="AY176" s="26"/>
-      <c r="AZ176" s="26"/>
-      <c r="BA176" s="26"/>
-      <c r="BB176" s="26"/>
-      <c r="BC176" s="26"/>
-      <c r="BD176" s="26"/>
-      <c r="BE176" s="26"/>
-      <c r="BF176" s="26"/>
-      <c r="BG176" s="26"/>
-      <c r="BH176" s="26"/>
-      <c r="BI176" s="26"/>
-      <c r="BJ176" s="26"/>
-      <c r="BK176" s="26"/>
-      <c r="BL176" s="26"/>
-    </row>
-    <row r="177" s="33" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="B177" s="99"/>
-      <c r="E177" s="3"/>
-      <c r="G177" s="100"/>
-      <c r="H177" s="100" t="str">
+      <c r="B176" s="99"/>
+      <c r="E176" s="3"/>
+      <c r="G176" s="100"/>
+      <c r="H176" s="100" t="str">
         <f aca="false">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I177" s="101"/>
-      <c r="J177" s="101"/>
-      <c r="K177" s="101"/>
-      <c r="L177" s="101"/>
-      <c r="M177" s="101"/>
-      <c r="N177" s="101"/>
-      <c r="O177" s="101"/>
-      <c r="P177" s="101"/>
-      <c r="Q177" s="101"/>
-      <c r="R177" s="101"/>
-      <c r="S177" s="101"/>
-      <c r="T177" s="101"/>
-      <c r="U177" s="101"/>
-      <c r="V177" s="101"/>
-      <c r="W177" s="101"/>
-      <c r="X177" s="101"/>
-      <c r="Y177" s="101"/>
-      <c r="Z177" s="101"/>
-      <c r="AA177" s="101"/>
-      <c r="AB177" s="101"/>
-      <c r="AC177" s="101"/>
-      <c r="AD177" s="101"/>
-      <c r="AE177" s="101"/>
-      <c r="AF177" s="101"/>
-      <c r="AG177" s="101"/>
-      <c r="AH177" s="101"/>
-      <c r="AI177" s="101"/>
-      <c r="AJ177" s="101"/>
-      <c r="AK177" s="101"/>
-      <c r="AL177" s="101"/>
-      <c r="AM177" s="101"/>
-      <c r="AN177" s="101"/>
-      <c r="AO177" s="101"/>
-      <c r="AP177" s="101"/>
-      <c r="AQ177" s="101"/>
-      <c r="AR177" s="101"/>
-      <c r="AS177" s="101"/>
-      <c r="AT177" s="101"/>
-      <c r="AU177" s="101"/>
-      <c r="AV177" s="101"/>
-      <c r="AW177" s="101"/>
-      <c r="AX177" s="101"/>
-      <c r="AY177" s="101"/>
-      <c r="AZ177" s="101"/>
-      <c r="BA177" s="101"/>
-      <c r="BB177" s="101"/>
-      <c r="BC177" s="101"/>
-      <c r="BD177" s="101"/>
-      <c r="BE177" s="101"/>
-      <c r="BF177" s="101"/>
-      <c r="BG177" s="101"/>
-      <c r="BH177" s="101"/>
-      <c r="BI177" s="101"/>
-      <c r="BJ177" s="101"/>
-      <c r="BK177" s="101"/>
-      <c r="BL177" s="101"/>
+      <c r="I176" s="101"/>
+      <c r="J176" s="101"/>
+      <c r="K176" s="101"/>
+      <c r="L176" s="101"/>
+      <c r="M176" s="101"/>
+      <c r="N176" s="101"/>
+      <c r="O176" s="101"/>
+      <c r="P176" s="101"/>
+      <c r="Q176" s="101"/>
+      <c r="R176" s="101"/>
+      <c r="S176" s="101"/>
+      <c r="T176" s="101"/>
+      <c r="U176" s="101"/>
+      <c r="V176" s="101"/>
+      <c r="W176" s="101"/>
+      <c r="X176" s="101"/>
+      <c r="Y176" s="101"/>
+      <c r="Z176" s="101"/>
+      <c r="AA176" s="101"/>
+      <c r="AB176" s="101"/>
+      <c r="AC176" s="101"/>
+      <c r="AD176" s="101"/>
+      <c r="AE176" s="101"/>
+      <c r="AF176" s="101"/>
+      <c r="AG176" s="101"/>
+      <c r="AH176" s="101"/>
+      <c r="AI176" s="101"/>
+      <c r="AJ176" s="101"/>
+      <c r="AK176" s="101"/>
+      <c r="AL176" s="101"/>
+      <c r="AM176" s="101"/>
+      <c r="AN176" s="101"/>
+      <c r="AO176" s="101"/>
+      <c r="AP176" s="101"/>
+      <c r="AQ176" s="101"/>
+      <c r="AR176" s="101"/>
+      <c r="AS176" s="101"/>
+      <c r="AT176" s="101"/>
+      <c r="AU176" s="101"/>
+      <c r="AV176" s="101"/>
+      <c r="AW176" s="101"/>
+      <c r="AX176" s="101"/>
+      <c r="AY176" s="101"/>
+      <c r="AZ176" s="101"/>
+      <c r="BA176" s="101"/>
+      <c r="BB176" s="101"/>
+      <c r="BC176" s="101"/>
+      <c r="BD176" s="101"/>
+      <c r="BE176" s="101"/>
+      <c r="BF176" s="101"/>
+      <c r="BG176" s="101"/>
+      <c r="BH176" s="101"/>
+      <c r="BI176" s="101"/>
+      <c r="BJ176" s="101"/>
+      <c r="BK176" s="101"/>
+      <c r="BL176" s="101"/>
+    </row>
+    <row r="177" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C177" s="10"/>
+      <c r="F177" s="102"/>
+      <c r="G177" s="103"/>
     </row>
     <row r="178" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C178" s="10"/>
-      <c r="F178" s="102"/>
-      <c r="G178" s="103"/>
-    </row>
-    <row r="179" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C179" s="104"/>
-    </row>
-    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C178" s="104"/>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="C3:D3"/>
@@ -15238,7 +15168,7 @@
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="B5:G5"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D44 D71:D81 D88:D91 D98 D101:D107 D125:D129 D146:D149">
+  <conditionalFormatting sqref="D7:D44 D70:D79 D86:D89 D96 D99:D105 D124:D128 D145:D148">
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15247,17 +15177,17 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6F4E1070-46A0-434B-9442-E0F7779B1E2C}</x14:id>
+          <x14:id>{3AAB484E-2246-46C7-BAB5-902CFF5230FE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL177">
+  <conditionalFormatting sqref="I5:BL176">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL177">
+  <conditionalFormatting sqref="I7:BL176">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -15265,7 +15195,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D92:D97">
+  <conditionalFormatting sqref="D90:D95">
     <cfRule type="dataBar" priority="6">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15274,12 +15204,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B5182A24-F1E4-441E-8F3B-BEFADF855772}</x14:id>
+          <x14:id>{E9FE152D-BEEA-4F54-AFA1-F9CEBD6055CE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D135:D136">
+  <conditionalFormatting sqref="D134:D135">
     <cfRule type="dataBar" priority="7">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15288,12 +15218,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CAC4D5B2-BD12-45AF-977E-5E8059CC2280}</x14:id>
+          <x14:id>{EDB86696-8D41-4C4E-A626-A3902F37BC71}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D158:D170">
+  <conditionalFormatting sqref="D157:D169">
     <cfRule type="dataBar" priority="8">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15302,12 +15232,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{AE208D84-3557-4BCA-9C17-F4D83B61BA4E}</x14:id>
+          <x14:id>{D42E474A-D3F6-4532-9730-E630FCECF518}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45:D52">
+  <conditionalFormatting sqref="D45:D51">
     <cfRule type="dataBar" priority="9">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15316,12 +15246,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{44DD904D-9E38-486D-B8EC-C19B70F2EE17}</x14:id>
+          <x14:id>{6B6729A7-9A31-451D-A654-A04BB8D8953B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D59">
+  <conditionalFormatting sqref="D52:D58">
     <cfRule type="dataBar" priority="10">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15330,12 +15260,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{674E5E4D-94CF-4742-9CF1-E116E416D71F}</x14:id>
+          <x14:id>{D8DD32ED-2011-42C9-8970-90EB215D25DA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60:D62">
+  <conditionalFormatting sqref="D59:D61">
     <cfRule type="dataBar" priority="11">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15344,12 +15274,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5EF02217-6B93-4AA0-98AC-98DDA9E4BC82}</x14:id>
+          <x14:id>{49B3E9F6-88DA-4350-BE6A-23865CAF4AF7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63:D70">
+  <conditionalFormatting sqref="D62:D69">
     <cfRule type="dataBar" priority="12">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15358,12 +15288,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7DBB1733-0074-4356-9480-1DB041706A7B}</x14:id>
+          <x14:id>{168569D0-4BCA-4879-AF60-DE3E8611AB48}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D82:D87">
+  <conditionalFormatting sqref="D80:D85">
     <cfRule type="dataBar" priority="13">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15372,12 +15302,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8BD0F448-3835-4C55-AAB8-2D8F5A63B17E}</x14:id>
+          <x14:id>{82E5E15F-3CDE-4734-8AB7-4D8B4ABBE038}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D99:D100">
+  <conditionalFormatting sqref="D97:D98">
     <cfRule type="dataBar" priority="14">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15386,12 +15316,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1CCC7EA1-F02D-4AD1-A5A0-F879CC8BB773}</x14:id>
+          <x14:id>{6D47ABF5-A756-4811-B97B-F021EB2C3C6D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D137:D138">
+  <conditionalFormatting sqref="D136:D137">
     <cfRule type="dataBar" priority="15">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15400,12 +15330,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B940D933-51CA-403B-82C3-95F8B36A2250}</x14:id>
+          <x14:id>{5CB22CC2-4276-49A0-959E-DAC1A540EB14}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D108:D117">
+  <conditionalFormatting sqref="D106:D116">
     <cfRule type="dataBar" priority="16">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15414,12 +15344,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7D30D387-48FC-4DCF-8B31-607AD1C67090}</x14:id>
+          <x14:id>{90985F7A-6F3E-4DD0-9893-177A42CE6D68}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D124">
+  <conditionalFormatting sqref="D123">
     <cfRule type="dataBar" priority="17">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15428,12 +15358,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E2FA16F7-375B-4615-9CE9-963F59D9C0CF}</x14:id>
+          <x14:id>{113440BD-D5FA-4C93-87BA-E400942D6033}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D118:D123">
+  <conditionalFormatting sqref="D117:D122">
     <cfRule type="dataBar" priority="18">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15442,12 +15372,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{AE6E8BE9-5ACC-40AC-B73A-D7A98C6C47C0}</x14:id>
+          <x14:id>{DC199A34-29E7-42AF-B0CC-E672AD58702B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D130:D134">
+  <conditionalFormatting sqref="D129:D133">
     <cfRule type="dataBar" priority="19">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15456,12 +15386,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F5CEBBA7-D4A3-4A78-B3F2-8391456640C0}</x14:id>
+          <x14:id>{10E9C435-F893-4995-B0F3-3131BFB65D37}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D150:D155">
+  <conditionalFormatting sqref="D149:D154">
     <cfRule type="dataBar" priority="20">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15470,12 +15400,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E042E570-7B1E-41A2-93D6-DD2A3039AB68}</x14:id>
+          <x14:id>{B312AF5C-B53C-4E98-9124-7190993BA731}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D139:D145">
+  <conditionalFormatting sqref="D138:D144">
     <cfRule type="dataBar" priority="21">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15484,12 +15414,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{47CB6FC0-B263-47BD-A711-25BFD1A477E9}</x14:id>
+          <x14:id>{337B9E47-43DF-4DE8-95F0-2747DAAA55F4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D157">
+  <conditionalFormatting sqref="D156">
     <cfRule type="dataBar" priority="22">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15498,12 +15428,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2BF0D138-C833-48A3-A2BC-40EF12F079F2}</x14:id>
+          <x14:id>{3035CB22-CC23-4320-8DE5-7951CB4480C1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D156">
+  <conditionalFormatting sqref="D155">
     <cfRule type="dataBar" priority="23">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15512,12 +15442,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8FE0C4D0-5BCA-41E8-8886-1A6486489075}</x14:id>
+          <x14:id>{90AF463A-E934-4930-82B2-9CFC8A3B6DAA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D176">
+  <conditionalFormatting sqref="D175">
     <cfRule type="dataBar" priority="24">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15526,12 +15456,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{77D63316-20D2-4C21-8CFF-B72B6EAF1690}</x14:id>
+          <x14:id>{FB2EC979-83DF-429B-9931-4180D6BDE7A0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D171:D175">
+  <conditionalFormatting sqref="D170:D174">
     <cfRule type="dataBar" priority="25">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -15540,7 +15470,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8197C44A-E0BC-426B-85CA-D0F4EC7D8070}</x14:id>
+          <x14:id>{A3D6A3CE-81B2-4C77-B786-8284CB1066B0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15562,7 +15492,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6F4E1070-46A0-434B-9442-E0F7779B1E2C}">
+          <x14:cfRule type="dataBar" id="{3AAB484E-2246-46C7-BAB5-902CFF5230FE}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15574,10 +15504,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D44 D71:D81 D88:D91 D98 D101:D107 D125:D129 D146:D149</xm:sqref>
+          <xm:sqref>D7:D44 D70:D79 D86:D89 D96 D99:D105 D124:D128 D145:D148</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B5182A24-F1E4-441E-8F3B-BEFADF855772}">
+          <x14:cfRule type="dataBar" id="{E9FE152D-BEEA-4F54-AFA1-F9CEBD6055CE}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15589,10 +15519,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D92:D97</xm:sqref>
+          <xm:sqref>D90:D95</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CAC4D5B2-BD12-45AF-977E-5E8059CC2280}">
+          <x14:cfRule type="dataBar" id="{EDB86696-8D41-4C4E-A626-A3902F37BC71}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15604,10 +15534,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D135:D136</xm:sqref>
+          <xm:sqref>D134:D135</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{AE208D84-3557-4BCA-9C17-F4D83B61BA4E}">
+          <x14:cfRule type="dataBar" id="{D42E474A-D3F6-4532-9730-E630FCECF518}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15619,10 +15549,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D158:D170</xm:sqref>
+          <xm:sqref>D157:D169</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{44DD904D-9E38-486D-B8EC-C19B70F2EE17}">
+          <x14:cfRule type="dataBar" id="{6B6729A7-9A31-451D-A654-A04BB8D8953B}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15634,10 +15564,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D45:D52</xm:sqref>
+          <xm:sqref>D45:D51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{674E5E4D-94CF-4742-9CF1-E116E416D71F}">
+          <x14:cfRule type="dataBar" id="{D8DD32ED-2011-42C9-8970-90EB215D25DA}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15649,10 +15579,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D53:D59</xm:sqref>
+          <xm:sqref>D52:D58</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5EF02217-6B93-4AA0-98AC-98DDA9E4BC82}">
+          <x14:cfRule type="dataBar" id="{49B3E9F6-88DA-4350-BE6A-23865CAF4AF7}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15664,10 +15594,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D60:D62</xm:sqref>
+          <xm:sqref>D59:D61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7DBB1733-0074-4356-9480-1DB041706A7B}">
+          <x14:cfRule type="dataBar" id="{168569D0-4BCA-4879-AF60-DE3E8611AB48}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15679,10 +15609,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D63:D70</xm:sqref>
+          <xm:sqref>D62:D69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8BD0F448-3835-4C55-AAB8-2D8F5A63B17E}">
+          <x14:cfRule type="dataBar" id="{82E5E15F-3CDE-4734-8AB7-4D8B4ABBE038}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15694,10 +15624,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D82:D87</xm:sqref>
+          <xm:sqref>D80:D85</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1CCC7EA1-F02D-4AD1-A5A0-F879CC8BB773}">
+          <x14:cfRule type="dataBar" id="{6D47ABF5-A756-4811-B97B-F021EB2C3C6D}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15709,10 +15639,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D99:D100</xm:sqref>
+          <xm:sqref>D97:D98</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B940D933-51CA-403B-82C3-95F8B36A2250}">
+          <x14:cfRule type="dataBar" id="{5CB22CC2-4276-49A0-959E-DAC1A540EB14}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15724,10 +15654,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D137:D138</xm:sqref>
+          <xm:sqref>D136:D137</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7D30D387-48FC-4DCF-8B31-607AD1C67090}">
+          <x14:cfRule type="dataBar" id="{90985F7A-6F3E-4DD0-9893-177A42CE6D68}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15739,10 +15669,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D108:D117</xm:sqref>
+          <xm:sqref>D106:D116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E2FA16F7-375B-4615-9CE9-963F59D9C0CF}">
+          <x14:cfRule type="dataBar" id="{113440BD-D5FA-4C93-87BA-E400942D6033}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15754,10 +15684,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D124</xm:sqref>
+          <xm:sqref>D123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{AE6E8BE9-5ACC-40AC-B73A-D7A98C6C47C0}">
+          <x14:cfRule type="dataBar" id="{DC199A34-29E7-42AF-B0CC-E672AD58702B}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15769,10 +15699,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D118:D123</xm:sqref>
+          <xm:sqref>D117:D122</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F5CEBBA7-D4A3-4A78-B3F2-8391456640C0}">
+          <x14:cfRule type="dataBar" id="{10E9C435-F893-4995-B0F3-3131BFB65D37}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15784,10 +15714,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D130:D134</xm:sqref>
+          <xm:sqref>D129:D133</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E042E570-7B1E-41A2-93D6-DD2A3039AB68}">
+          <x14:cfRule type="dataBar" id="{B312AF5C-B53C-4E98-9124-7190993BA731}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15799,10 +15729,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D150:D155</xm:sqref>
+          <xm:sqref>D149:D154</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{47CB6FC0-B263-47BD-A711-25BFD1A477E9}">
+          <x14:cfRule type="dataBar" id="{337B9E47-43DF-4DE8-95F0-2747DAAA55F4}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15814,25 +15744,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D139:D145</xm:sqref>
+          <xm:sqref>D138:D144</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2BF0D138-C833-48A3-A2BC-40EF12F079F2}">
-            <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D157</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8FE0C4D0-5BCA-41E8-8886-1A6486489075}">
+          <x14:cfRule type="dataBar" id="{3035CB22-CC23-4320-8DE5-7951CB4480C1}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15847,7 +15762,7 @@
           <xm:sqref>D156</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{77D63316-20D2-4C21-8CFF-B72B6EAF1690}">
+          <x14:cfRule type="dataBar" id="{90AF463A-E934-4930-82B2-9CFC8A3B6DAA}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15859,10 +15774,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D176</xm:sqref>
+          <xm:sqref>D155</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8197C44A-E0BC-426B-85CA-D0F4EC7D8070}">
+          <x14:cfRule type="dataBar" id="{FB2EC979-83DF-429B-9931-4180D6BDE7A0}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15874,7 +15789,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D171:D175</xm:sqref>
+          <xm:sqref>D175</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A3D6A3CE-81B2-4C77-B786-8284CB1066B0}">
+            <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D170:D174</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -15902,79 +15832,79 @@
     <row r="1" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" s="107" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="106" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" s="106"/>
     </row>
     <row r="3" s="109" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="108" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" s="108"/>
     </row>
     <row r="4" s="111" customFormat="true" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="110" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="74.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="112" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="110" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" s="105" customFormat="true" ht="204.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="113" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" s="111" customFormat="true" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="110" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="112" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" s="105" customFormat="true" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="114" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" s="111" customFormat="true" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="110" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="112" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" s="105" customFormat="true" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="114" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" s="111" customFormat="true" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="110" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="112" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="112" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Development section to doc
</commit_message>
<xml_diff>
--- a/Documentation/Obtayn-gantt-chart.xlsx
+++ b/Documentation/Obtayn-gantt-chart.xlsx
@@ -509,7 +509,7 @@
     <t xml:space="preserve">Filter</t>
   </si>
   <si>
-    <t xml:space="preserve">Create filter options - #request &amp; #post.</t>
+    <t xml:space="preserve">Create filter options - #request &amp; #appreciation.</t>
   </si>
   <si>
     <t xml:space="preserve">Write a function to fetch the selected option.</t>
@@ -1799,10 +1799,10 @@
   </sheetPr>
   <dimension ref="A1:BL1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L133" activeCellId="0" sqref="L133"/>
+      <selection pane="bottomLeft" activeCell="U12" activeCellId="0" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1819,7 +1819,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="69" style="0" width="10.29"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1833,7 +1833,7 @@
       <c r="H1" s="7"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" customFormat="false" ht="6.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" customFormat="false" ht="11.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="BK4" s="17"/>
       <c r="BL4" s="17"/>
     </row>
-    <row r="5" customFormat="false" ht="6.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="5.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -15851,7 +15851,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2B60B0F5-3347-47D2-9774-3E8F1EA115C0}</x14:id>
+          <x14:id>{DB225D56-D2E5-477F-86EE-757B184E703C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15878,7 +15878,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{94EBACA1-E15E-4AE5-9731-6D1AA7E05E17}</x14:id>
+          <x14:id>{C630E0CB-B5FF-46F0-9710-F59AE0A02431}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15892,7 +15892,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{26706D66-4C42-4759-B8BB-7762946F8721}</x14:id>
+          <x14:id>{77E04084-567C-4539-9DC8-C596B4C2A0D6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15906,7 +15906,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{78EFB83B-EFDB-4EEC-8534-97954BD9C371}</x14:id>
+          <x14:id>{47F6A975-40C0-47F3-9460-7943C4304534}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15920,7 +15920,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{95C69679-84BF-4DA5-95A1-1BBF17DC1FF0}</x14:id>
+          <x14:id>{E36A9F9C-FAE9-4311-89B5-D8433F845CD9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15934,7 +15934,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F8952027-4E69-494A-B129-80DEF4B6DC80}</x14:id>
+          <x14:id>{70937610-EBCF-4C24-BE4C-AB861B356E60}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15948,7 +15948,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{563DE45C-B295-4423-B662-917097DD51E0}</x14:id>
+          <x14:id>{A5C067EA-3E47-4633-8A24-E226A02FA031}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15962,7 +15962,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5BE02D90-1479-46C2-B68A-E55ABA8CEC67}</x14:id>
+          <x14:id>{F0CD9DC1-81FD-46CA-BF52-1D43E72E4B2B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15976,7 +15976,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1BE4B2FF-D831-40F5-8828-D2C493D072C3}</x14:id>
+          <x14:id>{6043A1A7-C818-47B1-AF00-DE707D6C8B7D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15990,7 +15990,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A95AE5A7-E8A0-4A4B-A89D-6715A19C39E6}</x14:id>
+          <x14:id>{2494F4D4-CC97-49D0-B2A6-4B8087005F1D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16004,7 +16004,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{63372B55-2F8C-4020-9D97-7DA1615D4381}</x14:id>
+          <x14:id>{1D452313-FD76-47CE-B4C0-2540A1E43844}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16018,7 +16018,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7569D9C4-4BE4-47CC-9C27-753433C03CFB}</x14:id>
+          <x14:id>{879B51BF-C053-48F1-A7A0-C75D3513C527}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16032,7 +16032,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CC50EF6C-3FFB-4FBC-8DE4-EAB4232B93CA}</x14:id>
+          <x14:id>{D7E4C329-B0EB-47DE-B0C0-00FF115EDEA2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16046,7 +16046,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4040B59A-9A20-47B5-A0CF-AC2641D899BF}</x14:id>
+          <x14:id>{B0DF86B0-496F-4C9F-A320-93D490DE9F5E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16060,7 +16060,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F4C0398F-5E88-4630-AD5E-5BC1F323C37B}</x14:id>
+          <x14:id>{3931CCC7-DF44-4C1A-B55C-6015EBDDFC21}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16074,7 +16074,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8DCD7BDF-6852-43A0-B7C0-A22EFC733CA8}</x14:id>
+          <x14:id>{78A2591B-2090-408F-BEF8-563050E05168}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16088,7 +16088,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CECC7F46-9610-446E-8B5F-3229686ECCE8}</x14:id>
+          <x14:id>{D098A28B-E589-4B15-9888-6871B21F9F69}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16102,7 +16102,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9B82F1AB-9B40-4677-BF90-5C1E69A53E70}</x14:id>
+          <x14:id>{3979B483-D49E-4200-A4AB-9939C9895448}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16116,7 +16116,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3372EDDA-EB2D-4311-8EE1-85A6329CD0EF}</x14:id>
+          <x14:id>{5FB98087-2E36-4C72-9784-24A5A69CD3AC}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16130,7 +16130,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7D32944D-602C-46F5-924E-2F7554F84FE0}</x14:id>
+          <x14:id>{417273A3-B013-4993-A0D4-D4EF6B19F588}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16144,7 +16144,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{43239399-5998-4DCC-B982-F35D1884496D}</x14:id>
+          <x14:id>{BB55A090-E0A9-4DF0-BE83-30501B171FEA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16158,7 +16158,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{AD2070E0-93AF-42D9-89E8-B534F8468462}</x14:id>
+          <x14:id>{184BD19D-97D0-48D3-945E-33E2B6A4F4A3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16172,7 +16172,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FE792930-65DA-4EA0-B92F-A0202F94C5C6}</x14:id>
+          <x14:id>{93ADE0D2-69F1-4D96-8C7C-603F7E3BD936}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -16194,7 +16194,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2B60B0F5-3347-47D2-9774-3E8F1EA115C0}">
+          <x14:cfRule type="dataBar" id="{DB225D56-D2E5-477F-86EE-757B184E703C}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16209,7 +16209,7 @@
           <xm:sqref>D7:D46 D72:D81 D88:D91 D98 D101:D107 D125:D129 D146:D149</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{94EBACA1-E15E-4AE5-9731-6D1AA7E05E17}">
+          <x14:cfRule type="dataBar" id="{C630E0CB-B5FF-46F0-9710-F59AE0A02431}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16224,7 +16224,7 @@
           <xm:sqref>D92:D97</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{26706D66-4C42-4759-B8BB-7762946F8721}">
+          <x14:cfRule type="dataBar" id="{77E04084-567C-4539-9DC8-C596B4C2A0D6}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16239,7 +16239,7 @@
           <xm:sqref>D135:D136</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{78EFB83B-EFDB-4EEC-8534-97954BD9C371}">
+          <x14:cfRule type="dataBar" id="{47F6A975-40C0-47F3-9460-7943C4304534}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16254,7 +16254,7 @@
           <xm:sqref>D158:D168</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{95C69679-84BF-4DA5-95A1-1BBF17DC1FF0}">
+          <x14:cfRule type="dataBar" id="{E36A9F9C-FAE9-4311-89B5-D8433F845CD9}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16269,7 +16269,7 @@
           <xm:sqref>D47:D53</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F8952027-4E69-494A-B129-80DEF4B6DC80}">
+          <x14:cfRule type="dataBar" id="{70937610-EBCF-4C24-BE4C-AB861B356E60}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16284,7 +16284,7 @@
           <xm:sqref>D54:D60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{563DE45C-B295-4423-B662-917097DD51E0}">
+          <x14:cfRule type="dataBar" id="{A5C067EA-3E47-4633-8A24-E226A02FA031}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16299,7 +16299,7 @@
           <xm:sqref>D61:D63</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5BE02D90-1479-46C2-B68A-E55ABA8CEC67}">
+          <x14:cfRule type="dataBar" id="{F0CD9DC1-81FD-46CA-BF52-1D43E72E4B2B}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16314,7 +16314,7 @@
           <xm:sqref>D64:D71</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1BE4B2FF-D831-40F5-8828-D2C493D072C3}">
+          <x14:cfRule type="dataBar" id="{6043A1A7-C818-47B1-AF00-DE707D6C8B7D}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16329,7 +16329,7 @@
           <xm:sqref>D82:D87</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A95AE5A7-E8A0-4A4B-A89D-6715A19C39E6}">
+          <x14:cfRule type="dataBar" id="{2494F4D4-CC97-49D0-B2A6-4B8087005F1D}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16344,7 +16344,7 @@
           <xm:sqref>D99:D100</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{63372B55-2F8C-4020-9D97-7DA1615D4381}">
+          <x14:cfRule type="dataBar" id="{1D452313-FD76-47CE-B4C0-2540A1E43844}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16359,7 +16359,7 @@
           <xm:sqref>D137:D138</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7569D9C4-4BE4-47CC-9C27-753433C03CFB}">
+          <x14:cfRule type="dataBar" id="{879B51BF-C053-48F1-A7A0-C75D3513C527}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16374,7 +16374,7 @@
           <xm:sqref>D108:D117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CC50EF6C-3FFB-4FBC-8DE4-EAB4232B93CA}">
+          <x14:cfRule type="dataBar" id="{D7E4C329-B0EB-47DE-B0C0-00FF115EDEA2}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16389,7 +16389,7 @@
           <xm:sqref>D124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4040B59A-9A20-47B5-A0CF-AC2641D899BF}">
+          <x14:cfRule type="dataBar" id="{B0DF86B0-496F-4C9F-A320-93D490DE9F5E}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16404,7 +16404,7 @@
           <xm:sqref>D118:D123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F4C0398F-5E88-4630-AD5E-5BC1F323C37B}">
+          <x14:cfRule type="dataBar" id="{3931CCC7-DF44-4C1A-B55C-6015EBDDFC21}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16419,7 +16419,7 @@
           <xm:sqref>D130:D134</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8DCD7BDF-6852-43A0-B7C0-A22EFC733CA8}">
+          <x14:cfRule type="dataBar" id="{78A2591B-2090-408F-BEF8-563050E05168}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16434,7 +16434,7 @@
           <xm:sqref>D150:D155</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CECC7F46-9610-446E-8B5F-3229686ECCE8}">
+          <x14:cfRule type="dataBar" id="{D098A28B-E589-4B15-9888-6871B21F9F69}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16449,7 +16449,7 @@
           <xm:sqref>D139:D145</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9B82F1AB-9B40-4677-BF90-5C1E69A53E70}">
+          <x14:cfRule type="dataBar" id="{3979B483-D49E-4200-A4AB-9939C9895448}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16464,7 +16464,7 @@
           <xm:sqref>D157</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3372EDDA-EB2D-4311-8EE1-85A6329CD0EF}">
+          <x14:cfRule type="dataBar" id="{5FB98087-2E36-4C72-9784-24A5A69CD3AC}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16479,7 +16479,7 @@
           <xm:sqref>D156</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7D32944D-602C-46F5-924E-2F7554F84FE0}">
+          <x14:cfRule type="dataBar" id="{417273A3-B013-4993-A0D4-D4EF6B19F588}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16494,7 +16494,7 @@
           <xm:sqref>D183</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{43239399-5998-4DCC-B982-F35D1884496D}">
+          <x14:cfRule type="dataBar" id="{BB55A090-E0A9-4DF0-BE83-30501B171FEA}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16509,7 +16509,7 @@
           <xm:sqref>D174:D182</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{AD2070E0-93AF-42D9-89E8-B534F8468462}">
+          <x14:cfRule type="dataBar" id="{184BD19D-97D0-48D3-945E-33E2B6A4F4A3}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16524,7 +16524,7 @@
           <xm:sqref>D170:D173</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FE792930-65DA-4EA0-B92F-A0202F94C5C6}">
+          <x14:cfRule type="dataBar" id="{93ADE0D2-69F1-4D96-8C7C-603F7E3BD936}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -16551,7 +16551,7 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>